<commit_message>
Lasan EDP recorrection + NM recorrection
</commit_message>
<xml_diff>
--- a/output/CGPA_Results.xlsx
+++ b/output/CGPA_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\GitHub\CGPA-gen\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0346911C-B75F-416B-A114-604A3DE73214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F86E32-E511-4FCF-81E5-B74CBAB2B079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,6 +46,9 @@
     <t>JATHUNWATHTHA J.C.R.N.</t>
   </si>
   <si>
+    <t>PERERA W.A.L.S.</t>
+  </si>
+  <si>
     <t>ADIKARAM D.M.G.H.</t>
   </si>
   <si>
@@ -64,9 +67,6 @@
     <t>PERERA G.M.B.</t>
   </si>
   <si>
-    <t>PERERA W.A.L.S.</t>
-  </si>
-  <si>
     <t>DHANANJAYA K.T.G.T.N.</t>
   </si>
   <si>
@@ -142,6 +142,9 @@
     <t>DHARMAKEERTHI P.K.G.C.L.</t>
   </si>
   <si>
+    <t>RANASINGHE D.P.H.</t>
+  </si>
+  <si>
     <t>RASANJANA W.P.G.R.A.</t>
   </si>
   <si>
@@ -151,9 +154,6 @@
     <t>KARUNARATHNA G.K.T.</t>
   </si>
   <si>
-    <t>RANASINGHE D.P.H.</t>
-  </si>
-  <si>
     <t>WEDAMESTRIGE A.N.</t>
   </si>
   <si>
@@ -172,6 +172,9 @@
     <t>DESHAN W.U.</t>
   </si>
   <si>
+    <t>DILHAN W.A.</t>
+  </si>
+  <si>
     <t>GUNASEKARA L.U.A.</t>
   </si>
   <si>
@@ -181,9 +184,6 @@
     <t>KARUNANAYAKE A.H.D.</t>
   </si>
   <si>
-    <t>DILHAN W.A.</t>
-  </si>
-  <si>
     <t>PERERA H.A.J.I.</t>
   </si>
   <si>
@@ -232,6 +232,9 @@
     <t>PRIYADARSHANA S.A.D.</t>
   </si>
   <si>
+    <t>GUNATHUNGA U.A.</t>
+  </si>
+  <si>
     <t>RANATHUNGA R.J.K.O.H.</t>
   </si>
   <si>
@@ -241,15 +244,12 @@
     <t>ATHUKORALA U.R.</t>
   </si>
   <si>
-    <t>GUNATHUNGA U.A.</t>
+    <t>BALASOORIYA B.R.B.D.</t>
   </si>
   <si>
     <t>ABISHEK L.</t>
   </si>
   <si>
-    <t>BALASOORIYA B.R.B.D.</t>
-  </si>
-  <si>
     <t>DISSANAYAKE R.K.T.</t>
   </si>
   <si>
@@ -286,6 +286,9 @@
     <t>PERAMUNAGE D.S.</t>
   </si>
   <si>
+    <t>WIJESINGHE W.A.P.W.</t>
+  </si>
+  <si>
     <t>ABEYWARDHANA T.C.W.</t>
   </si>
   <si>
@@ -298,31 +301,28 @@
     <t>RANASINGHE A.G.N.S.</t>
   </si>
   <si>
-    <t>WIJESINGHE W.A.P.W.</t>
-  </si>
-  <si>
     <t>PRABHARSHA H.W.D.</t>
   </si>
   <si>
     <t>LENMINI B.L.W.</t>
   </si>
   <si>
+    <t>MEEDENIYA M.M.H.</t>
+  </si>
+  <si>
     <t>NIRMANI W.T.</t>
   </si>
   <si>
     <t>INDUWARA M.L.A.S.</t>
   </si>
   <si>
-    <t>MEEDENIYA M.M.H.</t>
-  </si>
-  <si>
     <t>PALIHENA H.H.</t>
   </si>
   <si>
+    <t>RANAWAKA R.A.G.K.</t>
+  </si>
+  <si>
     <t>HIMASARA W.V.M.J.</t>
-  </si>
-  <si>
-    <t>RANAWAKA R.A.G.K.</t>
   </si>
   <si>
     <t>WITHANAGE G.D.N.</t>
@@ -729,11 +729,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="B115" sqref="B115"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -787,7 +789,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>230018</v>
+        <v>230487</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -799,10 +801,10 @@
         <v>4</v>
       </c>
       <c r="F3">
-        <v>3.96</v>
+        <v>4</v>
       </c>
       <c r="G3">
-        <v>3.99</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -810,7 +812,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>230074</v>
+        <v>230018</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -833,7 +835,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>230082</v>
+        <v>230074</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -856,7 +858,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>230171</v>
+        <v>230082</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -868,7 +870,7 @@
         <v>4</v>
       </c>
       <c r="F6">
-        <v>3.97</v>
+        <v>3.96</v>
       </c>
       <c r="G6">
         <v>3.99</v>
@@ -879,7 +881,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>230436</v>
+        <v>230171</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
@@ -888,10 +890,10 @@
         <v>4</v>
       </c>
       <c r="E7">
-        <v>3.96</v>
+        <v>4</v>
       </c>
       <c r="F7">
-        <v>4</v>
+        <v>3.97</v>
       </c>
       <c r="G7">
         <v>3.99</v>
@@ -902,7 +904,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>230476</v>
+        <v>230436</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
@@ -911,10 +913,10 @@
         <v>4</v>
       </c>
       <c r="E8">
-        <v>4</v>
+        <v>3.96</v>
       </c>
       <c r="F8">
-        <v>3.96</v>
+        <v>4</v>
       </c>
       <c r="G8">
         <v>3.99</v>
@@ -925,7 +927,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>230487</v>
+        <v>230476</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
@@ -934,10 +936,10 @@
         <v>4</v>
       </c>
       <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9">
         <v>3.96</v>
-      </c>
-      <c r="F9">
-        <v>4</v>
       </c>
       <c r="G9">
         <v>3.99</v>
@@ -1523,19 +1525,19 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>230536</v>
+        <v>230521</v>
       </c>
       <c r="C35" t="s">
         <v>40</v>
       </c>
       <c r="D35">
-        <v>3.96</v>
+        <v>4</v>
       </c>
       <c r="E35">
-        <v>3.96</v>
+        <v>4</v>
       </c>
       <c r="F35">
-        <v>3.85</v>
+        <v>3.79</v>
       </c>
       <c r="G35">
         <v>3.92</v>
@@ -1546,22 +1548,22 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>230197</v>
+        <v>230536</v>
       </c>
       <c r="C36" t="s">
         <v>41</v>
       </c>
       <c r="D36">
-        <v>4</v>
+        <v>3.96</v>
       </c>
       <c r="E36">
-        <v>3.88</v>
+        <v>3.96</v>
       </c>
       <c r="F36">
-        <v>3.9</v>
+        <v>3.85</v>
       </c>
       <c r="G36">
-        <v>3.91</v>
+        <v>3.92</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -1569,7 +1571,7 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>230322</v>
+        <v>230197</v>
       </c>
       <c r="C37" t="s">
         <v>42</v>
@@ -1578,10 +1580,10 @@
         <v>4</v>
       </c>
       <c r="E37">
-        <v>3.92</v>
+        <v>3.88</v>
       </c>
       <c r="F37">
-        <v>3.86</v>
+        <v>3.9</v>
       </c>
       <c r="G37">
         <v>3.91</v>
@@ -1592,7 +1594,7 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>230521</v>
+        <v>230322</v>
       </c>
       <c r="C38" t="s">
         <v>43</v>
@@ -1601,10 +1603,10 @@
         <v>4</v>
       </c>
       <c r="E38">
-        <v>4</v>
+        <v>3.92</v>
       </c>
       <c r="F38">
-        <v>3.76</v>
+        <v>3.86</v>
       </c>
       <c r="G38">
         <v>3.91</v>
@@ -1753,19 +1755,19 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>230212</v>
+        <v>230145</v>
       </c>
       <c r="C45" t="s">
         <v>50</v>
       </c>
       <c r="D45">
-        <v>3.96</v>
+        <v>3.94</v>
       </c>
       <c r="E45">
-        <v>3.88</v>
+        <v>4</v>
       </c>
       <c r="F45">
-        <v>3.82</v>
+        <v>3.7</v>
       </c>
       <c r="G45">
         <v>3.88</v>
@@ -1776,19 +1778,19 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>230300</v>
+        <v>230212</v>
       </c>
       <c r="C46" t="s">
         <v>51</v>
       </c>
       <c r="D46">
-        <v>3.94</v>
+        <v>3.96</v>
       </c>
       <c r="E46">
-        <v>4</v>
+        <v>3.88</v>
       </c>
       <c r="F46">
-        <v>3.71</v>
+        <v>3.82</v>
       </c>
       <c r="G46">
         <v>3.88</v>
@@ -1799,19 +1801,19 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>230321</v>
+        <v>230300</v>
       </c>
       <c r="C47" t="s">
         <v>52</v>
       </c>
       <c r="D47">
-        <v>4</v>
+        <v>3.94</v>
       </c>
       <c r="E47">
-        <v>3.95</v>
+        <v>4</v>
       </c>
       <c r="F47">
-        <v>3.73</v>
+        <v>3.71</v>
       </c>
       <c r="G47">
         <v>3.88</v>
@@ -1822,22 +1824,22 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>230145</v>
+        <v>230321</v>
       </c>
       <c r="C48" t="s">
         <v>53</v>
       </c>
       <c r="D48">
-        <v>3.94</v>
+        <v>4</v>
       </c>
       <c r="E48">
-        <v>4</v>
+        <v>3.95</v>
       </c>
       <c r="F48">
-        <v>3.68</v>
+        <v>3.73</v>
       </c>
       <c r="G48">
-        <v>3.87</v>
+        <v>3.88</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
@@ -2213,19 +2215,19 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>230525</v>
+        <v>230218</v>
       </c>
       <c r="C65" t="s">
         <v>70</v>
       </c>
       <c r="D65">
-        <v>4</v>
+        <v>3.94</v>
       </c>
       <c r="E65">
-        <v>4</v>
+        <v>3.77</v>
       </c>
       <c r="F65">
-        <v>3.5</v>
+        <v>3.78</v>
       </c>
       <c r="G65">
         <v>3.81</v>
@@ -2236,19 +2238,19 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <v>230726</v>
+        <v>230525</v>
       </c>
       <c r="C66" t="s">
         <v>71</v>
       </c>
       <c r="D66">
-        <v>3.89</v>
+        <v>4</v>
       </c>
       <c r="E66">
-        <v>3.9</v>
+        <v>4</v>
       </c>
       <c r="F66">
-        <v>3.66</v>
+        <v>3.5</v>
       </c>
       <c r="G66">
         <v>3.81</v>
@@ -2259,22 +2261,22 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <v>230063</v>
+        <v>230726</v>
       </c>
       <c r="C67" t="s">
         <v>72</v>
       </c>
       <c r="D67">
-        <v>4</v>
+        <v>3.89</v>
       </c>
       <c r="E67">
-        <v>3.92</v>
+        <v>3.9</v>
       </c>
       <c r="F67">
-        <v>3.56</v>
+        <v>3.66</v>
       </c>
       <c r="G67">
-        <v>3.8</v>
+        <v>3.81</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
@@ -2282,19 +2284,19 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <v>230218</v>
+        <v>230063</v>
       </c>
       <c r="C68" t="s">
         <v>73</v>
       </c>
       <c r="D68">
-        <v>3.94</v>
+        <v>4</v>
       </c>
       <c r="E68">
-        <v>3.77</v>
+        <v>3.92</v>
       </c>
       <c r="F68">
-        <v>3.75</v>
+        <v>3.56</v>
       </c>
       <c r="G68">
         <v>3.8</v>
@@ -2305,22 +2307,22 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <v>230016</v>
+        <v>230070</v>
       </c>
       <c r="C69" t="s">
         <v>74</v>
       </c>
       <c r="D69">
-        <v>4</v>
+        <v>3.96</v>
       </c>
       <c r="E69">
-        <v>3.91</v>
+        <v>3.82</v>
       </c>
       <c r="F69">
-        <v>3.48</v>
+        <v>3.67</v>
       </c>
       <c r="G69">
-        <v>3.79</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
@@ -2328,19 +2330,19 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <v>230070</v>
+        <v>230016</v>
       </c>
       <c r="C70" t="s">
         <v>75</v>
       </c>
       <c r="D70">
-        <v>3.96</v>
+        <v>4</v>
       </c>
       <c r="E70">
-        <v>3.82</v>
+        <v>3.91</v>
       </c>
       <c r="F70">
-        <v>3.64</v>
+        <v>3.48</v>
       </c>
       <c r="G70">
         <v>3.79</v>
@@ -2627,22 +2629,22 @@
         <v>82</v>
       </c>
       <c r="B83">
-        <v>230012</v>
+        <v>230727</v>
       </c>
       <c r="C83" t="s">
         <v>88</v>
       </c>
       <c r="D83">
-        <v>3.91</v>
+        <v>3.79</v>
       </c>
       <c r="E83">
-        <v>3.8</v>
+        <v>3.87</v>
       </c>
       <c r="F83">
-        <v>3.56</v>
+        <v>3.54</v>
       </c>
       <c r="G83">
-        <v>3.73</v>
+        <v>3.74</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
@@ -2650,19 +2652,19 @@
         <v>83</v>
       </c>
       <c r="B84">
-        <v>230147</v>
+        <v>230012</v>
       </c>
       <c r="C84" t="s">
         <v>89</v>
       </c>
       <c r="D84">
-        <v>3.89</v>
+        <v>3.91</v>
       </c>
       <c r="E84">
-        <v>3.83</v>
+        <v>3.8</v>
       </c>
       <c r="F84">
-        <v>3.51</v>
+        <v>3.56</v>
       </c>
       <c r="G84">
         <v>3.73</v>
@@ -2673,22 +2675,22 @@
         <v>84</v>
       </c>
       <c r="B85">
-        <v>230077</v>
+        <v>230147</v>
       </c>
       <c r="C85" t="s">
         <v>90</v>
       </c>
       <c r="D85">
-        <v>3.79</v>
+        <v>3.89</v>
       </c>
       <c r="E85">
-        <v>3.75</v>
+        <v>3.83</v>
       </c>
       <c r="F85">
-        <v>3.62</v>
+        <v>3.51</v>
       </c>
       <c r="G85">
-        <v>3.72</v>
+        <v>3.73</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
@@ -2696,19 +2698,19 @@
         <v>85</v>
       </c>
       <c r="B86">
-        <v>230520</v>
+        <v>230077</v>
       </c>
       <c r="C86" t="s">
         <v>91</v>
       </c>
       <c r="D86">
-        <v>3.85</v>
+        <v>3.79</v>
       </c>
       <c r="E86">
-        <v>3.85</v>
+        <v>3.75</v>
       </c>
       <c r="F86">
-        <v>3.49</v>
+        <v>3.62</v>
       </c>
       <c r="G86">
         <v>3.72</v>
@@ -2719,19 +2721,19 @@
         <v>86</v>
       </c>
       <c r="B87">
-        <v>230727</v>
+        <v>230520</v>
       </c>
       <c r="C87" t="s">
         <v>92</v>
       </c>
       <c r="D87">
-        <v>3.79</v>
+        <v>3.85</v>
       </c>
       <c r="E87">
-        <v>3.87</v>
+        <v>3.85</v>
       </c>
       <c r="F87">
-        <v>3.5</v>
+        <v>3.49</v>
       </c>
       <c r="G87">
         <v>3.72</v>
@@ -2788,19 +2790,19 @@
         <v>89</v>
       </c>
       <c r="B90">
-        <v>230444</v>
+        <v>230407</v>
       </c>
       <c r="C90" t="s">
         <v>95</v>
       </c>
       <c r="D90">
-        <v>3.79</v>
+        <v>4</v>
       </c>
       <c r="E90">
-        <v>3.62</v>
+        <v>3.75</v>
       </c>
       <c r="F90">
-        <v>3.76</v>
+        <v>3.47</v>
       </c>
       <c r="G90">
         <v>3.7</v>
@@ -2811,22 +2813,22 @@
         <v>90</v>
       </c>
       <c r="B91">
-        <v>230261</v>
+        <v>230444</v>
       </c>
       <c r="C91" t="s">
         <v>96</v>
       </c>
       <c r="D91">
-        <v>4</v>
+        <v>3.79</v>
       </c>
       <c r="E91">
-        <v>3.77</v>
+        <v>3.62</v>
       </c>
       <c r="F91">
-        <v>3.42</v>
+        <v>3.76</v>
       </c>
       <c r="G91">
-        <v>3.69</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
@@ -2834,7 +2836,7 @@
         <v>91</v>
       </c>
       <c r="B92">
-        <v>230407</v>
+        <v>230261</v>
       </c>
       <c r="C92" t="s">
         <v>97</v>
@@ -2843,10 +2845,10 @@
         <v>4</v>
       </c>
       <c r="E92">
-        <v>3.75</v>
+        <v>3.77</v>
       </c>
       <c r="F92">
-        <v>3.44</v>
+        <v>3.42</v>
       </c>
       <c r="G92">
         <v>3.69</v>
@@ -2880,22 +2882,22 @@
         <v>93</v>
       </c>
       <c r="B94">
-        <v>230248</v>
+        <v>230527</v>
       </c>
       <c r="C94" t="s">
         <v>99</v>
       </c>
       <c r="D94">
-        <v>3.94</v>
+        <v>4</v>
       </c>
       <c r="E94">
-        <v>3.66</v>
+        <v>3.86</v>
       </c>
       <c r="F94">
-        <v>3.54</v>
+        <v>3.34</v>
       </c>
       <c r="G94">
-        <v>3.68</v>
+        <v>3.69</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
@@ -2903,19 +2905,19 @@
         <v>94</v>
       </c>
       <c r="B95">
-        <v>230527</v>
+        <v>230248</v>
       </c>
       <c r="C95" t="s">
         <v>100</v>
       </c>
       <c r="D95">
-        <v>4</v>
+        <v>3.94</v>
       </c>
       <c r="E95">
-        <v>3.86</v>
+        <v>3.66</v>
       </c>
       <c r="F95">
-        <v>3.3</v>
+        <v>3.54</v>
       </c>
       <c r="G95">
         <v>3.68</v>

</xml_diff>

<commit_message>
Applied Stat results commit
</commit_message>
<xml_diff>
--- a/output/CGPA_Results.xlsx
+++ b/output/CGPA_Results.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\GitHub\CGPA-gen\output\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F86E32-E511-4FCF-81E5-B74CBAB2B079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="CGPA" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -391,8 +385,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -429,21 +423,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -481,7 +467,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -515,7 +501,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -550,10 +535,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -726,19 +710,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="B115" sqref="B115"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" width="17.109375" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -761,7 +740,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
@@ -784,7 +763,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2</v>
       </c>
@@ -807,7 +786,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
@@ -830,7 +809,7 @@
         <v>3.99</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>4</v>
       </c>
@@ -853,7 +832,7 @@
         <v>3.99</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>5</v>
       </c>
@@ -876,7 +855,7 @@
         <v>3.99</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>6</v>
       </c>
@@ -899,7 +878,7 @@
         <v>3.99</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>7</v>
       </c>
@@ -922,7 +901,7 @@
         <v>3.99</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>8</v>
       </c>
@@ -945,7 +924,7 @@
         <v>3.99</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>9</v>
       </c>
@@ -968,7 +947,7 @@
         <v>3.98</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>10</v>
       </c>
@@ -991,7 +970,7 @@
         <v>3.98</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1014,7 +993,7 @@
         <v>3.98</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1037,7 +1016,7 @@
         <v>3.97</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1060,7 +1039,7 @@
         <v>3.97</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1083,7 +1062,7 @@
         <v>3.97</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1106,7 +1085,7 @@
         <v>3.97</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1129,7 +1108,7 @@
         <v>3.97</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1152,7 +1131,7 @@
         <v>3.97</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1175,7 +1154,7 @@
         <v>3.96</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1198,7 +1177,7 @@
         <v>3.96</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1221,7 +1200,7 @@
         <v>3.96</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1244,7 +1223,7 @@
         <v>3.96</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1267,7 +1246,7 @@
         <v>3.95</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1290,7 +1269,7 @@
         <v>3.95</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1313,7 +1292,7 @@
         <v>3.95</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1336,7 +1315,7 @@
         <v>3.95</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1359,7 +1338,7 @@
         <v>3.95</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1382,7 +1361,7 @@
         <v>3.94</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1405,7 +1384,7 @@
         <v>3.94</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1428,7 +1407,7 @@
         <v>3.94</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1451,7 +1430,7 @@
         <v>3.94</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1474,7 +1453,7 @@
         <v>3.93</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1497,7 +1476,7 @@
         <v>3.93</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1520,7 +1499,7 @@
         <v>3.92</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1543,7 +1522,7 @@
         <v>3.92</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1566,7 +1545,7 @@
         <v>3.92</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1589,7 +1568,7 @@
         <v>3.91</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1612,7 +1591,7 @@
         <v>3.91</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1635,7 +1614,7 @@
         <v>3.91</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1658,7 +1637,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1681,7 +1660,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1704,7 +1683,7 @@
         <v>3.89</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1727,7 +1706,7 @@
         <v>3.89</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1750,7 +1729,7 @@
         <v>3.88</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1773,7 +1752,7 @@
         <v>3.88</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1796,7 +1775,7 @@
         <v>3.88</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1819,7 +1798,7 @@
         <v>3.88</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1842,7 +1821,7 @@
         <v>3.88</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1865,7 +1844,7 @@
         <v>3.87</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1888,7 +1867,7 @@
         <v>3.87</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1911,7 +1890,7 @@
         <v>3.87</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1934,7 +1913,7 @@
         <v>3.86</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1957,7 +1936,7 @@
         <v>3.86</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1980,7 +1959,7 @@
         <v>3.86</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2003,7 +1982,7 @@
         <v>3.86</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2026,7 +2005,7 @@
         <v>3.85</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2049,7 +2028,7 @@
         <v>3.85</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2072,7 +2051,7 @@
         <v>3.84</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2095,7 +2074,7 @@
         <v>3.83</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2118,7 +2097,7 @@
         <v>3.83</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2141,7 +2120,7 @@
         <v>3.82</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2164,7 +2143,7 @@
         <v>3.82</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2187,7 +2166,7 @@
         <v>3.82</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2210,7 +2189,7 @@
         <v>3.82</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2233,7 +2212,7 @@
         <v>3.81</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2256,7 +2235,7 @@
         <v>3.81</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2279,7 +2258,7 @@
         <v>3.81</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2302,7 +2281,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2325,7 +2304,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2348,7 +2327,7 @@
         <v>3.79</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2371,7 +2350,7 @@
         <v>3.79</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2394,7 +2373,7 @@
         <v>3.79</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2417,7 +2396,7 @@
         <v>3.79</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2440,7 +2419,7 @@
         <v>3.79</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2463,7 +2442,7 @@
         <v>3.79</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2486,7 +2465,7 @@
         <v>3.77</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2509,7 +2488,7 @@
         <v>3.76</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2532,7 +2511,7 @@
         <v>3.76</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2555,7 +2534,7 @@
         <v>3.76</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2578,7 +2557,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2601,7 +2580,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2624,7 +2603,7 @@
         <v>3.74</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7">
       <c r="A83">
         <v>82</v>
       </c>
@@ -2647,7 +2626,7 @@
         <v>3.74</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2670,7 +2649,7 @@
         <v>3.73</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2693,7 +2672,7 @@
         <v>3.73</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7">
       <c r="A86">
         <v>85</v>
       </c>
@@ -2716,7 +2695,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2739,7 +2718,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7">
       <c r="A88">
         <v>87</v>
       </c>
@@ -2762,7 +2741,7 @@
         <v>3.71</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7">
       <c r="A89">
         <v>88</v>
       </c>
@@ -2785,7 +2764,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7">
       <c r="A90">
         <v>89</v>
       </c>
@@ -2808,7 +2787,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7">
       <c r="A91">
         <v>90</v>
       </c>
@@ -2831,7 +2810,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7">
       <c r="A92">
         <v>91</v>
       </c>
@@ -2854,7 +2833,7 @@
         <v>3.69</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7">
       <c r="A93">
         <v>92</v>
       </c>
@@ -2877,7 +2856,7 @@
         <v>3.69</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7">
       <c r="A94">
         <v>93</v>
       </c>
@@ -2900,7 +2879,7 @@
         <v>3.69</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7">
       <c r="A95">
         <v>94</v>
       </c>
@@ -2923,7 +2902,7 @@
         <v>3.68</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7">
       <c r="A96">
         <v>95</v>
       </c>
@@ -2946,7 +2925,7 @@
         <v>3.68</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7">
       <c r="A97">
         <v>96</v>
       </c>
@@ -2969,7 +2948,7 @@
         <v>3.67</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7">
       <c r="A98">
         <v>97</v>
       </c>
@@ -2992,7 +2971,7 @@
         <v>3.67</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7">
       <c r="A99">
         <v>98</v>
       </c>
@@ -3015,7 +2994,7 @@
         <v>3.66</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7">
       <c r="A100">
         <v>99</v>
       </c>
@@ -3038,7 +3017,7 @@
         <v>3.65</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7">
       <c r="A101">
         <v>100</v>
       </c>
@@ -3061,7 +3040,7 @@
         <v>3.65</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7">
       <c r="A102">
         <v>101</v>
       </c>
@@ -3084,7 +3063,7 @@
         <v>3.65</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7">
       <c r="A103">
         <v>102</v>
       </c>
@@ -3107,7 +3086,7 @@
         <v>3.63</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7">
       <c r="A104">
         <v>103</v>
       </c>
@@ -3130,7 +3109,7 @@
         <v>3.63</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7">
       <c r="A105">
         <v>104</v>
       </c>
@@ -3153,7 +3132,7 @@
         <v>3.61</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7">
       <c r="A106">
         <v>105</v>
       </c>
@@ -3176,7 +3155,7 @@
         <v>3.59</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7">
       <c r="A107">
         <v>106</v>
       </c>
@@ -3199,7 +3178,7 @@
         <v>3.59</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7">
       <c r="A108">
         <v>107</v>
       </c>
@@ -3222,7 +3201,7 @@
         <v>3.59</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7">
       <c r="A109">
         <v>108</v>
       </c>
@@ -3245,7 +3224,7 @@
         <v>3.58</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7">
       <c r="A110">
         <v>109</v>
       </c>
@@ -3268,7 +3247,7 @@
         <v>3.58</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7">
       <c r="A111">
         <v>110</v>
       </c>
@@ -3291,7 +3270,7 @@
         <v>3.57</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7">
       <c r="A112">
         <v>111</v>
       </c>
@@ -3314,7 +3293,7 @@
         <v>3.51</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7">
       <c r="A113">
         <v>112</v>
       </c>
@@ -3337,7 +3316,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7">
       <c r="A114">
         <v>113</v>
       </c>
@@ -3360,7 +3339,7 @@
         <v>3.49</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7">
       <c r="A115">
         <v>114</v>
       </c>
@@ -3383,7 +3362,7 @@
         <v>3.48</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7">
       <c r="A116">
         <v>115</v>
       </c>

</xml_diff>

<commit_message>
Sasandu- EDP, Hasith, Isira - Telecom correction
</commit_message>
<xml_diff>
--- a/output/CGPA_Results.xlsx
+++ b/output/CGPA_Results.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\GitHub\CGPA-gen\output\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D22DB343-3448-4B07-84B5-73FE686409B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CGPA" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -385,8 +391,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -423,13 +429,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -467,7 +481,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -501,6 +515,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -535,9 +550,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -710,14 +726,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -740,7 +759,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -763,7 +782,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -786,7 +805,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -809,7 +828,7 @@
         <v>3.99</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -832,7 +851,7 @@
         <v>3.99</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -855,7 +874,7 @@
         <v>3.99</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -878,7 +897,7 @@
         <v>3.99</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -901,7 +920,7 @@
         <v>3.99</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -924,7 +943,7 @@
         <v>3.99</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -947,7 +966,7 @@
         <v>3.98</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -970,7 +989,7 @@
         <v>3.98</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -993,7 +1012,7 @@
         <v>3.98</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1016,7 +1035,7 @@
         <v>3.97</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1039,7 +1058,7 @@
         <v>3.97</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1062,7 +1081,7 @@
         <v>3.97</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1085,7 +1104,7 @@
         <v>3.97</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1108,7 +1127,7 @@
         <v>3.97</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1131,7 +1150,7 @@
         <v>3.97</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1154,7 +1173,7 @@
         <v>3.96</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1177,7 +1196,7 @@
         <v>3.96</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1200,7 +1219,7 @@
         <v>3.96</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1223,7 +1242,7 @@
         <v>3.96</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1246,7 +1265,7 @@
         <v>3.95</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1269,7 +1288,7 @@
         <v>3.95</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1292,7 +1311,7 @@
         <v>3.95</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1315,7 +1334,7 @@
         <v>3.95</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1338,7 +1357,7 @@
         <v>3.95</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1361,7 +1380,7 @@
         <v>3.94</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1384,7 +1403,7 @@
         <v>3.94</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1407,7 +1426,7 @@
         <v>3.94</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1430,7 +1449,7 @@
         <v>3.94</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1453,7 +1472,7 @@
         <v>3.93</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1476,7 +1495,7 @@
         <v>3.93</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1499,7 +1518,7 @@
         <v>3.92</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1522,7 +1541,7 @@
         <v>3.92</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1545,7 +1564,7 @@
         <v>3.92</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1568,7 +1587,7 @@
         <v>3.91</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1591,7 +1610,7 @@
         <v>3.91</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1614,7 +1633,7 @@
         <v>3.91</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1637,7 +1656,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1660,7 +1679,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1683,7 +1702,7 @@
         <v>3.89</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1706,7 +1725,7 @@
         <v>3.89</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1729,7 +1748,7 @@
         <v>3.88</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1752,7 +1771,7 @@
         <v>3.88</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1775,7 +1794,7 @@
         <v>3.88</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1798,7 +1817,7 @@
         <v>3.88</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1821,7 +1840,7 @@
         <v>3.88</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1844,7 +1863,7 @@
         <v>3.87</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1867,7 +1886,7 @@
         <v>3.87</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1890,7 +1909,7 @@
         <v>3.87</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1913,7 +1932,7 @@
         <v>3.86</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1936,7 +1955,7 @@
         <v>3.86</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1959,7 +1978,7 @@
         <v>3.86</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1982,7 +2001,7 @@
         <v>3.86</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2005,7 +2024,7 @@
         <v>3.85</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2028,7 +2047,7 @@
         <v>3.85</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2051,7 +2070,7 @@
         <v>3.84</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2074,7 +2093,7 @@
         <v>3.83</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2097,7 +2116,7 @@
         <v>3.83</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2120,7 +2139,7 @@
         <v>3.82</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2143,7 +2162,7 @@
         <v>3.82</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2166,7 +2185,7 @@
         <v>3.82</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2189,7 +2208,7 @@
         <v>3.82</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2212,7 +2231,7 @@
         <v>3.81</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2235,7 +2254,7 @@
         <v>3.81</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2258,7 +2277,7 @@
         <v>3.81</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2281,7 +2300,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2304,7 +2323,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2327,7 +2346,7 @@
         <v>3.79</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2350,7 +2369,7 @@
         <v>3.79</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2373,7 +2392,7 @@
         <v>3.79</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2396,7 +2415,7 @@
         <v>3.79</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2419,7 +2438,7 @@
         <v>3.79</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2442,7 +2461,7 @@
         <v>3.79</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2465,7 +2484,7 @@
         <v>3.77</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2488,7 +2507,7 @@
         <v>3.76</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2511,7 +2530,7 @@
         <v>3.76</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2534,7 +2553,7 @@
         <v>3.76</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2557,7 +2576,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2580,7 +2599,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2603,7 +2622,7 @@
         <v>3.74</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
@@ -2626,7 +2645,7 @@
         <v>3.74</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2649,7 +2668,7 @@
         <v>3.73</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2672,7 +2691,7 @@
         <v>3.73</v>
       </c>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>85</v>
       </c>
@@ -2695,7 +2714,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2718,7 +2737,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>87</v>
       </c>
@@ -2741,7 +2760,7 @@
         <v>3.71</v>
       </c>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>88</v>
       </c>
@@ -2764,7 +2783,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>89</v>
       </c>
@@ -2787,7 +2806,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>90</v>
       </c>
@@ -2810,7 +2829,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>91</v>
       </c>
@@ -2833,7 +2852,7 @@
         <v>3.69</v>
       </c>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>92</v>
       </c>
@@ -2856,7 +2875,7 @@
         <v>3.69</v>
       </c>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>93</v>
       </c>
@@ -2879,7 +2898,7 @@
         <v>3.69</v>
       </c>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>94</v>
       </c>
@@ -2902,7 +2921,7 @@
         <v>3.68</v>
       </c>
     </row>
-    <row r="96" spans="1:7">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>95</v>
       </c>
@@ -2925,7 +2944,7 @@
         <v>3.68</v>
       </c>
     </row>
-    <row r="97" spans="1:7">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>96</v>
       </c>
@@ -2948,7 +2967,7 @@
         <v>3.67</v>
       </c>
     </row>
-    <row r="98" spans="1:7">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>97</v>
       </c>
@@ -2971,7 +2990,7 @@
         <v>3.67</v>
       </c>
     </row>
-    <row r="99" spans="1:7">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>98</v>
       </c>
@@ -2994,7 +3013,7 @@
         <v>3.66</v>
       </c>
     </row>
-    <row r="100" spans="1:7">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>99</v>
       </c>
@@ -3017,7 +3036,7 @@
         <v>3.65</v>
       </c>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>100</v>
       </c>
@@ -3040,7 +3059,7 @@
         <v>3.65</v>
       </c>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>101</v>
       </c>
@@ -3063,7 +3082,7 @@
         <v>3.65</v>
       </c>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>102</v>
       </c>
@@ -3086,7 +3105,7 @@
         <v>3.63</v>
       </c>
     </row>
-    <row r="104" spans="1:7">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>103</v>
       </c>
@@ -3109,7 +3128,7 @@
         <v>3.63</v>
       </c>
     </row>
-    <row r="105" spans="1:7">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>104</v>
       </c>
@@ -3132,7 +3151,7 @@
         <v>3.61</v>
       </c>
     </row>
-    <row r="106" spans="1:7">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>105</v>
       </c>
@@ -3155,7 +3174,7 @@
         <v>3.59</v>
       </c>
     </row>
-    <row r="107" spans="1:7">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>106</v>
       </c>
@@ -3178,7 +3197,7 @@
         <v>3.59</v>
       </c>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>107</v>
       </c>
@@ -3201,7 +3220,7 @@
         <v>3.59</v>
       </c>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>108</v>
       </c>
@@ -3224,7 +3243,7 @@
         <v>3.58</v>
       </c>
     </row>
-    <row r="110" spans="1:7">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>109</v>
       </c>
@@ -3247,7 +3266,7 @@
         <v>3.58</v>
       </c>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>110</v>
       </c>
@@ -3270,7 +3289,7 @@
         <v>3.57</v>
       </c>
     </row>
-    <row r="112" spans="1:7">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>111</v>
       </c>
@@ -3293,7 +3312,7 @@
         <v>3.51</v>
       </c>
     </row>
-    <row r="113" spans="1:7">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>112</v>
       </c>
@@ -3316,7 +3335,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="114" spans="1:7">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>113</v>
       </c>
@@ -3339,7 +3358,7 @@
         <v>3.49</v>
       </c>
     </row>
-    <row r="115" spans="1:7">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>114</v>
       </c>
@@ -3362,7 +3381,7 @@
         <v>3.48</v>
       </c>
     </row>
-    <row r="116" spans="1:7">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>115</v>
       </c>

</xml_diff>

<commit_message>
Results sheet update commit
</commit_message>
<xml_diff>
--- a/output/CGPA_Results.xlsx
+++ b/output/CGPA_Results.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\GitHub\CGPA-gen\output\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D22DB343-3448-4B07-84B5-73FE686409B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="CGPA" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -391,8 +385,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -429,21 +423,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -481,7 +467,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -515,7 +501,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -550,10 +535,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -726,17 +710,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" width="21.6640625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -759,7 +740,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
@@ -782,7 +763,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2</v>
       </c>
@@ -805,7 +786,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
@@ -828,7 +809,7 @@
         <v>3.99</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>4</v>
       </c>
@@ -851,7 +832,7 @@
         <v>3.99</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>5</v>
       </c>
@@ -874,7 +855,7 @@
         <v>3.99</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>6</v>
       </c>
@@ -897,7 +878,7 @@
         <v>3.99</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>7</v>
       </c>
@@ -920,7 +901,7 @@
         <v>3.99</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>8</v>
       </c>
@@ -943,7 +924,7 @@
         <v>3.99</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>9</v>
       </c>
@@ -966,7 +947,7 @@
         <v>3.98</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>10</v>
       </c>
@@ -989,7 +970,7 @@
         <v>3.98</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1012,7 +993,7 @@
         <v>3.98</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1035,7 +1016,7 @@
         <v>3.97</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1058,7 +1039,7 @@
         <v>3.97</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1081,7 +1062,7 @@
         <v>3.97</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1104,7 +1085,7 @@
         <v>3.97</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1127,7 +1108,7 @@
         <v>3.97</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1150,7 +1131,7 @@
         <v>3.97</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1173,7 +1154,7 @@
         <v>3.96</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1196,7 +1177,7 @@
         <v>3.96</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1219,7 +1200,7 @@
         <v>3.96</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1242,7 +1223,7 @@
         <v>3.96</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1265,7 +1246,7 @@
         <v>3.95</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1288,7 +1269,7 @@
         <v>3.95</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1311,7 +1292,7 @@
         <v>3.95</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1334,7 +1315,7 @@
         <v>3.95</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1357,7 +1338,7 @@
         <v>3.95</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1380,7 +1361,7 @@
         <v>3.94</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1403,7 +1384,7 @@
         <v>3.94</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1426,7 +1407,7 @@
         <v>3.94</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1449,7 +1430,7 @@
         <v>3.94</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1472,7 +1453,7 @@
         <v>3.93</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1495,7 +1476,7 @@
         <v>3.93</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1518,7 +1499,7 @@
         <v>3.92</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1541,7 +1522,7 @@
         <v>3.92</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1564,7 +1545,7 @@
         <v>3.92</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1587,7 +1568,7 @@
         <v>3.91</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1610,7 +1591,7 @@
         <v>3.91</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1633,7 +1614,7 @@
         <v>3.91</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1656,7 +1637,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1679,7 +1660,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1702,7 +1683,7 @@
         <v>3.89</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1725,7 +1706,7 @@
         <v>3.89</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1748,7 +1729,7 @@
         <v>3.88</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1771,7 +1752,7 @@
         <v>3.88</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1794,7 +1775,7 @@
         <v>3.88</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1817,7 +1798,7 @@
         <v>3.88</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1840,7 +1821,7 @@
         <v>3.88</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1863,7 +1844,7 @@
         <v>3.87</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1886,7 +1867,7 @@
         <v>3.87</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1909,7 +1890,7 @@
         <v>3.87</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1932,7 +1913,7 @@
         <v>3.86</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1955,7 +1936,7 @@
         <v>3.86</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1978,7 +1959,7 @@
         <v>3.86</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2001,7 +1982,7 @@
         <v>3.86</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2024,7 +2005,7 @@
         <v>3.85</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2047,7 +2028,7 @@
         <v>3.85</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2070,7 +2051,7 @@
         <v>3.84</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2093,7 +2074,7 @@
         <v>3.83</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2116,7 +2097,7 @@
         <v>3.83</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2139,7 +2120,7 @@
         <v>3.82</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2162,7 +2143,7 @@
         <v>3.82</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2185,7 +2166,7 @@
         <v>3.82</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2208,7 +2189,7 @@
         <v>3.82</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2231,7 +2212,7 @@
         <v>3.81</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2254,7 +2235,7 @@
         <v>3.81</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2277,7 +2258,7 @@
         <v>3.81</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2300,7 +2281,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2323,7 +2304,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2346,7 +2327,7 @@
         <v>3.79</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2369,7 +2350,7 @@
         <v>3.79</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2392,7 +2373,7 @@
         <v>3.79</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2415,7 +2396,7 @@
         <v>3.79</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2438,7 +2419,7 @@
         <v>3.79</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2461,7 +2442,7 @@
         <v>3.79</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2484,7 +2465,7 @@
         <v>3.77</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2507,7 +2488,7 @@
         <v>3.76</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2530,7 +2511,7 @@
         <v>3.76</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2553,7 +2534,7 @@
         <v>3.76</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2576,7 +2557,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2599,7 +2580,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2622,7 +2603,7 @@
         <v>3.74</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7">
       <c r="A83">
         <v>82</v>
       </c>
@@ -2645,7 +2626,7 @@
         <v>3.74</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2668,7 +2649,7 @@
         <v>3.73</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2691,7 +2672,7 @@
         <v>3.73</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7">
       <c r="A86">
         <v>85</v>
       </c>
@@ -2714,7 +2695,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2737,7 +2718,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7">
       <c r="A88">
         <v>87</v>
       </c>
@@ -2760,7 +2741,7 @@
         <v>3.71</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7">
       <c r="A89">
         <v>88</v>
       </c>
@@ -2783,7 +2764,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7">
       <c r="A90">
         <v>89</v>
       </c>
@@ -2806,7 +2787,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7">
       <c r="A91">
         <v>90</v>
       </c>
@@ -2829,7 +2810,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7">
       <c r="A92">
         <v>91</v>
       </c>
@@ -2852,7 +2833,7 @@
         <v>3.69</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7">
       <c r="A93">
         <v>92</v>
       </c>
@@ -2875,7 +2856,7 @@
         <v>3.69</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7">
       <c r="A94">
         <v>93</v>
       </c>
@@ -2898,7 +2879,7 @@
         <v>3.69</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7">
       <c r="A95">
         <v>94</v>
       </c>
@@ -2921,7 +2902,7 @@
         <v>3.68</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7">
       <c r="A96">
         <v>95</v>
       </c>
@@ -2944,7 +2925,7 @@
         <v>3.68</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7">
       <c r="A97">
         <v>96</v>
       </c>
@@ -2967,7 +2948,7 @@
         <v>3.67</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7">
       <c r="A98">
         <v>97</v>
       </c>
@@ -2990,7 +2971,7 @@
         <v>3.67</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7">
       <c r="A99">
         <v>98</v>
       </c>
@@ -3013,7 +2994,7 @@
         <v>3.66</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7">
       <c r="A100">
         <v>99</v>
       </c>
@@ -3036,7 +3017,7 @@
         <v>3.65</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7">
       <c r="A101">
         <v>100</v>
       </c>
@@ -3059,7 +3040,7 @@
         <v>3.65</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7">
       <c r="A102">
         <v>101</v>
       </c>
@@ -3082,7 +3063,7 @@
         <v>3.65</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7">
       <c r="A103">
         <v>102</v>
       </c>
@@ -3105,7 +3086,7 @@
         <v>3.63</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7">
       <c r="A104">
         <v>103</v>
       </c>
@@ -3128,7 +3109,7 @@
         <v>3.63</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7">
       <c r="A105">
         <v>104</v>
       </c>
@@ -3151,7 +3132,7 @@
         <v>3.61</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7">
       <c r="A106">
         <v>105</v>
       </c>
@@ -3174,7 +3155,7 @@
         <v>3.59</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7">
       <c r="A107">
         <v>106</v>
       </c>
@@ -3197,7 +3178,7 @@
         <v>3.59</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7">
       <c r="A108">
         <v>107</v>
       </c>
@@ -3220,7 +3201,7 @@
         <v>3.59</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7">
       <c r="A109">
         <v>108</v>
       </c>
@@ -3243,7 +3224,7 @@
         <v>3.58</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7">
       <c r="A110">
         <v>109</v>
       </c>
@@ -3266,7 +3247,7 @@
         <v>3.58</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7">
       <c r="A111">
         <v>110</v>
       </c>
@@ -3289,7 +3270,7 @@
         <v>3.57</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7">
       <c r="A112">
         <v>111</v>
       </c>
@@ -3312,7 +3293,7 @@
         <v>3.51</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7">
       <c r="A113">
         <v>112</v>
       </c>
@@ -3335,7 +3316,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7">
       <c r="A114">
         <v>113</v>
       </c>
@@ -3358,7 +3339,7 @@
         <v>3.49</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7">
       <c r="A115">
         <v>114</v>
       </c>
@@ -3381,7 +3362,7 @@
         <v>3.48</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7">
       <c r="A116">
         <v>115</v>
       </c>

</xml_diff>

<commit_message>
Applied stat added to sem3.json
</commit_message>
<xml_diff>
--- a/output/CGPA_Results.xlsx
+++ b/output/CGPA_Results.xlsx
@@ -43,6 +43,9 @@
     <t>PERERA W.A.L.S.</t>
   </si>
   <si>
+    <t>ELAPATHA C.D.</t>
+  </si>
+  <si>
     <t>ADIKARAM D.M.G.H.</t>
   </si>
   <si>
@@ -52,9 +55,6 @@
     <t>BANDARA W.D.A.C.</t>
   </si>
   <si>
-    <t>ELAPATHA C.D.</t>
-  </si>
-  <si>
     <t>NETTIKUMARA N.A.H.G.</t>
   </si>
   <si>
@@ -70,63 +70,63 @@
     <t>WEERAKOON A.H.T.M.</t>
   </si>
   <si>
+    <t>ILANKOON I.M.M.K.B.</t>
+  </si>
+  <si>
+    <t>KARIYAWASAM J.H.D.</t>
+  </si>
+  <si>
     <t>COLOMBAGE D.M.</t>
   </si>
   <si>
-    <t>ILANKOON I.M.M.K.B.</t>
-  </si>
-  <si>
-    <t>KARIYAWASAM J.H.D.</t>
-  </si>
-  <si>
     <t>KUMARA K.B.R.</t>
   </si>
   <si>
+    <t>RATHNAYAKE M.A.G.K.N.</t>
+  </si>
+  <si>
     <t>PERERA K.W.A.O.V.</t>
   </si>
   <si>
-    <t>RATHNAYAKE M.A.G.K.N.</t>
+    <t>WANIGASUNDARA W.M.H.</t>
+  </si>
+  <si>
+    <t>KUMARASINGHE M.N.</t>
+  </si>
+  <si>
+    <t>PEIRIS E.A.S.S.</t>
   </si>
   <si>
     <t>DE MEL D.J.</t>
   </si>
   <si>
-    <t>KUMARASINGHE M.N.</t>
-  </si>
-  <si>
-    <t>PEIRIS E.A.S.S.</t>
-  </si>
-  <si>
-    <t>WANIGASUNDARA W.M.H.</t>
-  </si>
-  <si>
     <t>DISSANAYAKA D.M.D.P.</t>
   </si>
   <si>
+    <t>RAHUL B.</t>
+  </si>
+  <si>
+    <t>MALDENIYA P.A.D.G.R.</t>
+  </si>
+  <si>
+    <t>FERNANDO W.H.D.</t>
+  </si>
+  <si>
     <t>DISSANAYAKE G.R.G.K.</t>
   </si>
   <si>
-    <t>FERNANDO W.H.D.</t>
-  </si>
-  <si>
-    <t>MALDENIYA P.A.D.G.R.</t>
-  </si>
-  <si>
-    <t>RAHUL B.</t>
+    <t>IMADUWAGE O.N.H.</t>
+  </si>
+  <si>
+    <t>PATHIRANA P.T.S.</t>
+  </si>
+  <si>
+    <t>SAMARASINGHE S.M.R.R.</t>
   </si>
   <si>
     <t>ARACHCHI A.D.I.D.</t>
   </si>
   <si>
-    <t>IMADUWAGE O.N.H.</t>
-  </si>
-  <si>
-    <t>PATHIRANA P.T.S.</t>
-  </si>
-  <si>
-    <t>SAMARASINGHE S.M.R.R.</t>
-  </si>
-  <si>
     <t>KEERAWELLA K.P.C.P.</t>
   </si>
   <si>
@@ -151,54 +151,54 @@
     <t>WEDAMESTRIGE A.N.</t>
   </si>
   <si>
+    <t>WIJESEKARA W.A.G.S.</t>
+  </si>
+  <si>
     <t>CHANDRAKUMARA H.A.D.C.</t>
   </si>
   <si>
-    <t>WIJESEKARA W.A.G.S.</t>
+    <t>MUNASINGHE A.I.</t>
   </si>
   <si>
     <t>AMARATHUNGE A.M.N.L.</t>
   </si>
   <si>
-    <t>MUNASINGHE A.I.</t>
-  </si>
-  <si>
     <t>DESHAN W.U.</t>
   </si>
   <si>
+    <t>KARUNANAYAKE A.H.D.</t>
+  </si>
+  <si>
+    <t>JAYAWEERA N.S.</t>
+  </si>
+  <si>
     <t>DILHAN W.A.</t>
   </si>
   <si>
     <t>GUNASEKARA L.U.A.</t>
   </si>
   <si>
-    <t>JAYAWEERA N.S.</t>
-  </si>
-  <si>
-    <t>KARUNANAYAKE A.H.D.</t>
+    <t>UPEKSHANI T.S.</t>
   </si>
   <si>
     <t>PERERA H.A.J.I.</t>
   </si>
   <si>
-    <t>UPEKSHANI T.S.</t>
-  </si>
-  <si>
     <t>WEERASINGHE J.A.H.R.</t>
   </si>
   <si>
+    <t>SHEHAN M.N.N.</t>
+  </si>
+  <si>
+    <t>AROSHANA H.A.P.</t>
+  </si>
+  <si>
+    <t>AYANAJA N.B.G.M.</t>
+  </si>
+  <si>
     <t>ANTHONY C.S.B.</t>
   </si>
   <si>
-    <t>AROSHANA H.A.P.</t>
-  </si>
-  <si>
-    <t>AYANAJA N.B.G.M.</t>
-  </si>
-  <si>
-    <t>SHEHAN M.N.N.</t>
-  </si>
-  <si>
     <t>GUNASEKARA K.S.</t>
   </si>
   <si>
@@ -214,27 +214,27 @@
     <t>TENNAKOON U.G.R.B.</t>
   </si>
   <si>
+    <t>PEIRIS T.S.R.</t>
+  </si>
+  <si>
     <t>FERNANDO H.M.D.</t>
   </si>
   <si>
     <t>KUMARA P.K.M.P.</t>
   </si>
   <si>
-    <t>PEIRIS T.S.R.</t>
-  </si>
-  <si>
     <t>PRIYADARSHANA S.A.D.</t>
   </si>
   <si>
     <t>GUNATHUNGA U.A.</t>
   </si>
   <si>
+    <t>WIJESINGHE U.G.S.K.D.</t>
+  </si>
+  <si>
     <t>RANATHUNGA R.J.K.O.H.</t>
   </si>
   <si>
-    <t>WIJESINGHE U.G.S.K.D.</t>
-  </si>
-  <si>
     <t>ATHUKORALA U.R.</t>
   </si>
   <si>
@@ -244,67 +244,70 @@
     <t>ABISHEK L.</t>
   </si>
   <si>
+    <t>JAYASINGHE J.A.P.R.</t>
+  </si>
+  <si>
+    <t>SARUKA U.</t>
+  </si>
+  <si>
+    <t>RAHMAN M.F.A.</t>
+  </si>
+  <si>
     <t>DISSANAYAKE R.K.T.</t>
   </si>
   <si>
     <t>GAMAGE SK</t>
   </si>
   <si>
-    <t>JAYASINGHE J.A.P.R.</t>
-  </si>
-  <si>
-    <t>RAHMAN M.F.A.</t>
-  </si>
-  <si>
-    <t>SARUKA U.</t>
-  </si>
-  <si>
     <t>RANAWAKA R.A.C.D.</t>
   </si>
   <si>
+    <t>UMAIR A.</t>
+  </si>
+  <si>
     <t>AHAMED A.M.S.</t>
   </si>
   <si>
     <t>ARACHCHIGE M. A. D. T. S.</t>
   </si>
   <si>
-    <t>UMAIR A.</t>
+    <t>KAUSHALYA R.G.S.P.</t>
   </si>
   <si>
     <t>ADHIKARI A.H.C.S.</t>
   </si>
   <si>
-    <t>KAUSHALYA R.G.S.P.</t>
+    <t>WIJESINGHE W.A.P.W.</t>
   </si>
   <si>
     <t>PERAMUNAGE D.S.</t>
   </si>
   <si>
-    <t>WIJESINGHE W.A.P.W.</t>
-  </si>
-  <si>
     <t>ABEYWARDHANA T.C.W.</t>
   </si>
   <si>
     <t>DILHARA D.S.</t>
   </si>
   <si>
+    <t>RANASINGHE A.G.N.S.</t>
+  </si>
+  <si>
     <t>BANDARA K.M.N.D.</t>
   </si>
   <si>
-    <t>RANASINGHE A.G.N.S.</t>
-  </si>
-  <si>
     <t>PRABHARSHA H.W.D.</t>
   </si>
   <si>
+    <t>NIRMANI W.T.</t>
+  </si>
+  <si>
     <t>LENMINI B.L.W.</t>
   </si>
   <si>
     <t>MEEDENIYA M.M.H.</t>
   </si>
   <si>
-    <t>NIRMANI W.T.</t>
+    <t>RANAWAKA R.A.G.K.</t>
   </si>
   <si>
     <t>INDUWARA M.L.A.S.</t>
@@ -313,55 +316,52 @@
     <t>PALIHENA H.H.</t>
   </si>
   <si>
-    <t>RANAWAKA R.A.G.K.</t>
+    <t>WITHANAGE G.D.N.</t>
   </si>
   <si>
     <t>HIMASARA W.V.M.J.</t>
   </si>
   <si>
-    <t>WITHANAGE G.D.N.</t>
+    <t>SANTHOSH S.</t>
   </si>
   <si>
     <t>HANSINDU M.M.A.D.</t>
   </si>
   <si>
-    <t>SANTHOSH S.</t>
-  </si>
-  <si>
     <t>UBEYSEKARA V.T.T.</t>
   </si>
   <si>
     <t>ABEYWARNA D.H.</t>
   </si>
   <si>
+    <t>GUNASEKARA H.M.</t>
+  </si>
+  <si>
     <t>ERANGA W.A.O.</t>
   </si>
   <si>
-    <t>GUNASEKARA H.M.</t>
+    <t>SAMARANAYAKA H.D.J.D.</t>
   </si>
   <si>
     <t>HENDENIYA H.M.J.C.</t>
   </si>
   <si>
-    <t>SAMARANAYAKA H.D.J.D.</t>
-  </si>
-  <si>
     <t>PIYUMAL N.P.P.</t>
   </si>
   <si>
+    <t>MANATUNGA K.D.</t>
+  </si>
+  <si>
     <t>IMBULPITIYA B.N.</t>
   </si>
   <si>
-    <t>MANATUNGA K.D.</t>
-  </si>
-  <si>
     <t>WIJETHILAKA J.S.</t>
   </si>
   <si>
+    <t>THARUSHIKA G.K.E.</t>
+  </si>
+  <si>
     <t>AMARASINGHE A.A.D.K.</t>
-  </si>
-  <si>
-    <t>THARUSHIKA G.K.E.</t>
   </si>
   <si>
     <t>FERNANDO LTJ</t>
@@ -791,7 +791,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>230018</v>
+        <v>230171</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -803,10 +803,10 @@
         <v>4</v>
       </c>
       <c r="F4">
-        <v>3.96</v>
+        <v>3.9739</v>
       </c>
       <c r="G4">
-        <v>3.99</v>
+        <v>3.9903</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -814,7 +814,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>230074</v>
+        <v>230018</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -826,10 +826,10 @@
         <v>4</v>
       </c>
       <c r="F5">
-        <v>3.96</v>
+        <v>3.9609</v>
       </c>
       <c r="G5">
-        <v>3.99</v>
+        <v>3.9855</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -837,7 +837,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>230082</v>
+        <v>230074</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -849,10 +849,10 @@
         <v>4</v>
       </c>
       <c r="F6">
-        <v>3.96</v>
+        <v>3.9609</v>
       </c>
       <c r="G6">
-        <v>3.99</v>
+        <v>3.9855</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -860,7 +860,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>230171</v>
+        <v>230082</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
@@ -872,10 +872,10 @@
         <v>4</v>
       </c>
       <c r="F7">
-        <v>3.97</v>
+        <v>3.9609</v>
       </c>
       <c r="G7">
-        <v>3.99</v>
+        <v>3.9855</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -892,13 +892,13 @@
         <v>4</v>
       </c>
       <c r="E8">
-        <v>3.96</v>
+        <v>3.964</v>
       </c>
       <c r="F8">
         <v>4</v>
       </c>
       <c r="G8">
-        <v>3.99</v>
+        <v>3.9855</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -918,10 +918,10 @@
         <v>4</v>
       </c>
       <c r="F9">
-        <v>3.96</v>
+        <v>3.9609</v>
       </c>
       <c r="G9">
-        <v>3.99</v>
+        <v>3.9855</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -941,10 +941,10 @@
         <v>4</v>
       </c>
       <c r="F10">
-        <v>3.96</v>
+        <v>3.9571</v>
       </c>
       <c r="G10">
-        <v>3.98</v>
+        <v>3.985</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -964,10 +964,10 @@
         <v>4</v>
       </c>
       <c r="F11">
-        <v>3.96</v>
+        <v>3.9609</v>
       </c>
       <c r="G11">
-        <v>3.98</v>
+        <v>3.9847</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -990,7 +990,7 @@
         <v>3.95</v>
       </c>
       <c r="G12">
-        <v>3.98</v>
+        <v>3.9833</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -998,22 +998,22 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>230108</v>
+        <v>230256</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
       </c>
       <c r="D13">
-        <v>3.94</v>
+        <v>4</v>
       </c>
       <c r="E13">
         <v>4</v>
       </c>
       <c r="F13">
-        <v>3.95</v>
+        <v>3.925</v>
       </c>
       <c r="G13">
-        <v>3.97</v>
+        <v>3.9714</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1021,7 +1021,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>230256</v>
+        <v>230318</v>
       </c>
       <c r="C14" t="s">
         <v>19</v>
@@ -1033,10 +1033,10 @@
         <v>4</v>
       </c>
       <c r="F14">
-        <v>3.93</v>
+        <v>3.925</v>
       </c>
       <c r="G14">
-        <v>3.97</v>
+        <v>3.9714</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1044,22 +1044,22 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>230318</v>
+        <v>230108</v>
       </c>
       <c r="C15" t="s">
         <v>20</v>
       </c>
       <c r="D15">
-        <v>4</v>
+        <v>3.9357</v>
       </c>
       <c r="E15">
         <v>4</v>
       </c>
       <c r="F15">
-        <v>3.92</v>
+        <v>3.955</v>
       </c>
       <c r="G15">
-        <v>3.97</v>
+        <v>3.971</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1073,16 +1073,16 @@
         <v>21</v>
       </c>
       <c r="D16">
-        <v>3.94</v>
+        <v>3.9357</v>
       </c>
       <c r="E16">
         <v>4</v>
       </c>
       <c r="F16">
-        <v>3.96</v>
+        <v>3.9609</v>
       </c>
       <c r="G16">
-        <v>3.97</v>
+        <v>3.971</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1090,22 +1090,22 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>230481</v>
+        <v>230544</v>
       </c>
       <c r="C17" t="s">
         <v>22</v>
       </c>
       <c r="D17">
-        <v>3.85</v>
+        <v>4</v>
       </c>
       <c r="E17">
         <v>4</v>
       </c>
       <c r="F17">
-        <v>4</v>
+        <v>3.9217</v>
       </c>
       <c r="G17">
-        <v>3.97</v>
+        <v>3.9695</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1113,22 +1113,22 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>230544</v>
+        <v>230481</v>
       </c>
       <c r="C18" t="s">
         <v>23</v>
       </c>
       <c r="D18">
-        <v>4</v>
+        <v>3.85</v>
       </c>
       <c r="E18">
         <v>4</v>
       </c>
       <c r="F18">
-        <v>3.92</v>
+        <v>4</v>
       </c>
       <c r="G18">
-        <v>3.97</v>
+        <v>3.9661</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1136,22 +1136,22 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>230121</v>
+        <v>230680</v>
       </c>
       <c r="C19" t="s">
         <v>24</v>
       </c>
       <c r="D19">
-        <v>3.96</v>
+        <v>4</v>
       </c>
       <c r="E19">
         <v>4</v>
       </c>
       <c r="F19">
-        <v>3.92</v>
+        <v>3.9</v>
       </c>
       <c r="G19">
-        <v>3.96</v>
+        <v>3.9632</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1174,7 +1174,7 @@
         <v>3.9</v>
       </c>
       <c r="G20">
-        <v>3.96</v>
+        <v>3.9629</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1191,13 +1191,13 @@
         <v>4</v>
       </c>
       <c r="E21">
-        <v>3.96</v>
+        <v>3.964</v>
       </c>
       <c r="F21">
-        <v>3.94</v>
+        <v>3.9375</v>
       </c>
       <c r="G21">
-        <v>3.96</v>
+        <v>3.9619</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1205,22 +1205,22 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>230680</v>
+        <v>230121</v>
       </c>
       <c r="C22" t="s">
         <v>27</v>
       </c>
       <c r="D22">
-        <v>4</v>
+        <v>3.9571</v>
       </c>
       <c r="E22">
         <v>4</v>
       </c>
       <c r="F22">
-        <v>3.9</v>
+        <v>3.9217</v>
       </c>
       <c r="G22">
-        <v>3.96</v>
+        <v>3.9613</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1237,13 +1237,13 @@
         <v>4</v>
       </c>
       <c r="E23">
-        <v>3.93</v>
+        <v>3.928</v>
       </c>
       <c r="F23">
-        <v>3.96</v>
+        <v>3.9571</v>
       </c>
       <c r="G23">
-        <v>3.95</v>
+        <v>3.955</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1251,7 +1251,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>230159</v>
+        <v>230508</v>
       </c>
       <c r="C24" t="s">
         <v>29</v>
@@ -1260,13 +1260,13 @@
         <v>4</v>
       </c>
       <c r="E24">
-        <v>3.96</v>
+        <v>4</v>
       </c>
       <c r="F24">
-        <v>3.9</v>
+        <v>3.8826</v>
       </c>
       <c r="G24">
-        <v>3.95</v>
+        <v>3.9542</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1274,7 +1274,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>230186</v>
+        <v>230390</v>
       </c>
       <c r="C25" t="s">
         <v>30</v>
@@ -1286,10 +1286,10 @@
         <v>4</v>
       </c>
       <c r="F25">
-        <v>3.87</v>
+        <v>3.8739</v>
       </c>
       <c r="G25">
-        <v>3.95</v>
+        <v>3.9532</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1297,7 +1297,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>230390</v>
+        <v>230186</v>
       </c>
       <c r="C26" t="s">
         <v>31</v>
@@ -1309,10 +1309,10 @@
         <v>4</v>
       </c>
       <c r="F26">
-        <v>3.87</v>
+        <v>3.8696</v>
       </c>
       <c r="G26">
-        <v>3.95</v>
+        <v>3.9516</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1320,7 +1320,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>230508</v>
+        <v>230159</v>
       </c>
       <c r="C27" t="s">
         <v>32</v>
@@ -1329,13 +1329,13 @@
         <v>4</v>
       </c>
       <c r="E27">
-        <v>4</v>
+        <v>3.9571</v>
       </c>
       <c r="F27">
-        <v>3.87</v>
+        <v>3.895</v>
       </c>
       <c r="G27">
-        <v>3.95</v>
+        <v>3.9468</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1343,22 +1343,22 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>230051</v>
+        <v>230258</v>
       </c>
       <c r="C28" t="s">
         <v>33</v>
       </c>
       <c r="D28">
-        <v>4</v>
+        <v>3.8929</v>
       </c>
       <c r="E28">
-        <v>4</v>
+        <v>3.964</v>
       </c>
       <c r="F28">
-        <v>3.83</v>
+        <v>3.9571</v>
       </c>
       <c r="G28">
-        <v>3.94</v>
+        <v>3.945</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1366,22 +1366,22 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>230258</v>
+        <v>230468</v>
       </c>
       <c r="C29" t="s">
         <v>34</v>
       </c>
       <c r="D29">
-        <v>3.89</v>
+        <v>3.9143</v>
       </c>
       <c r="E29">
-        <v>3.96</v>
+        <v>4</v>
       </c>
       <c r="F29">
-        <v>3.96</v>
+        <v>3.8957</v>
       </c>
       <c r="G29">
-        <v>3.94</v>
+        <v>3.9419</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1389,22 +1389,22 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>230468</v>
+        <v>230566</v>
       </c>
       <c r="C30" t="s">
         <v>35</v>
       </c>
       <c r="D30">
-        <v>3.91</v>
+        <v>3.9571</v>
       </c>
       <c r="E30">
         <v>4</v>
       </c>
       <c r="F30">
-        <v>3.9</v>
+        <v>3.8846</v>
       </c>
       <c r="G30">
-        <v>3.94</v>
+        <v>3.9419</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1412,22 +1412,22 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>230566</v>
+        <v>230051</v>
       </c>
       <c r="C31" t="s">
         <v>36</v>
       </c>
       <c r="D31">
-        <v>3.96</v>
+        <v>4</v>
       </c>
       <c r="E31">
         <v>4</v>
       </c>
       <c r="F31">
-        <v>3.88</v>
+        <v>3.8304</v>
       </c>
       <c r="G31">
-        <v>3.94</v>
+        <v>3.9371</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1450,7 +1450,7 @@
         <v>3.79</v>
       </c>
       <c r="G32">
-        <v>3.93</v>
+        <v>3.9323</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1470,10 +1470,10 @@
         <v>4</v>
       </c>
       <c r="F33">
-        <v>3.83</v>
+        <v>3.8269</v>
       </c>
       <c r="G33">
-        <v>3.93</v>
+        <v>3.9308</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1487,16 +1487,16 @@
         <v>39</v>
       </c>
       <c r="D34">
-        <v>3.94</v>
+        <v>3.9357</v>
       </c>
       <c r="E34">
-        <v>3.96</v>
+        <v>3.964</v>
       </c>
       <c r="F34">
-        <v>3.87</v>
+        <v>3.8739</v>
       </c>
       <c r="G34">
-        <v>3.92</v>
+        <v>3.9242</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1516,10 +1516,10 @@
         <v>4</v>
       </c>
       <c r="F35">
-        <v>3.79</v>
+        <v>3.7913</v>
       </c>
       <c r="G35">
-        <v>3.92</v>
+        <v>3.9186</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1533,16 +1533,16 @@
         <v>41</v>
       </c>
       <c r="D36">
-        <v>3.96</v>
+        <v>3.9571</v>
       </c>
       <c r="E36">
-        <v>3.96</v>
+        <v>3.9591</v>
       </c>
       <c r="F36">
-        <v>3.85</v>
+        <v>3.8478</v>
       </c>
       <c r="G36">
-        <v>3.92</v>
+        <v>3.9153</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1565,7 +1565,7 @@
         <v>3.9</v>
       </c>
       <c r="G37">
-        <v>3.91</v>
+        <v>3.9145</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1582,13 +1582,13 @@
         <v>4</v>
       </c>
       <c r="E38">
-        <v>3.92</v>
+        <v>3.916</v>
       </c>
       <c r="F38">
-        <v>3.86</v>
+        <v>3.8625</v>
       </c>
       <c r="G38">
-        <v>3.91</v>
+        <v>3.9143</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1605,13 +1605,13 @@
         <v>4</v>
       </c>
       <c r="E39">
-        <v>3.93</v>
+        <v>3.9318</v>
       </c>
       <c r="F39">
-        <v>3.83</v>
+        <v>3.8304</v>
       </c>
       <c r="G39">
-        <v>3.91</v>
+        <v>3.9085</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1619,7 +1619,7 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>230100</v>
+        <v>230724</v>
       </c>
       <c r="C40" t="s">
         <v>45</v>
@@ -1628,13 +1628,13 @@
         <v>4</v>
       </c>
       <c r="E40">
-        <v>4</v>
+        <v>3.9045</v>
       </c>
       <c r="F40">
-        <v>3.72</v>
+        <v>3.8478</v>
       </c>
       <c r="G40">
-        <v>3.9</v>
+        <v>3.9051</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1642,7 +1642,7 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>230724</v>
+        <v>230100</v>
       </c>
       <c r="C41" t="s">
         <v>46</v>
@@ -1651,13 +1651,13 @@
         <v>4</v>
       </c>
       <c r="E41">
-        <v>3.9</v>
+        <v>4</v>
       </c>
       <c r="F41">
-        <v>3.83</v>
+        <v>3.7217</v>
       </c>
       <c r="G41">
-        <v>3.9</v>
+        <v>3.8968</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -1665,7 +1665,7 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>230038</v>
+        <v>230417</v>
       </c>
       <c r="C42" t="s">
         <v>47</v>
@@ -1674,13 +1674,13 @@
         <v>4</v>
       </c>
       <c r="E42">
-        <v>4</v>
+        <v>3.916</v>
       </c>
       <c r="F42">
-        <v>3.69</v>
+        <v>3.8043</v>
       </c>
       <c r="G42">
-        <v>3.89</v>
+        <v>3.8935</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1688,7 +1688,7 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>230417</v>
+        <v>230038</v>
       </c>
       <c r="C43" t="s">
         <v>48</v>
@@ -1697,13 +1697,13 @@
         <v>4</v>
       </c>
       <c r="E43">
-        <v>3.92</v>
+        <v>4</v>
       </c>
       <c r="F43">
-        <v>3.8</v>
+        <v>3.6913</v>
       </c>
       <c r="G43">
-        <v>3.89</v>
+        <v>3.8855</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -1720,13 +1720,13 @@
         <v>4</v>
       </c>
       <c r="E44">
-        <v>3.96</v>
+        <v>3.964</v>
       </c>
       <c r="F44">
-        <v>3.71</v>
+        <v>3.7143</v>
       </c>
       <c r="G44">
-        <v>3.88</v>
+        <v>3.885</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1734,22 +1734,22 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>230145</v>
+        <v>230321</v>
       </c>
       <c r="C45" t="s">
         <v>50</v>
       </c>
       <c r="D45">
-        <v>3.94</v>
+        <v>4</v>
       </c>
       <c r="E45">
-        <v>4</v>
+        <v>3.952</v>
       </c>
       <c r="F45">
-        <v>3.7</v>
+        <v>3.7304</v>
       </c>
       <c r="G45">
-        <v>3.88</v>
+        <v>3.8806</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -1757,22 +1757,22 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>230212</v>
+        <v>230300</v>
       </c>
       <c r="C46" t="s">
         <v>51</v>
       </c>
       <c r="D46">
-        <v>3.96</v>
+        <v>3.9357</v>
       </c>
       <c r="E46">
-        <v>3.88</v>
+        <v>4</v>
       </c>
       <c r="F46">
-        <v>3.82</v>
+        <v>3.713</v>
       </c>
       <c r="G46">
-        <v>3.88</v>
+        <v>3.879</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -1780,22 +1780,22 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>230300</v>
+        <v>230145</v>
       </c>
       <c r="C47" t="s">
         <v>52</v>
       </c>
       <c r="D47">
-        <v>3.94</v>
+        <v>3.9357</v>
       </c>
       <c r="E47">
         <v>4</v>
       </c>
       <c r="F47">
-        <v>3.71</v>
+        <v>3.7043</v>
       </c>
       <c r="G47">
-        <v>3.88</v>
+        <v>3.8758</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -1803,22 +1803,22 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>230321</v>
+        <v>230212</v>
       </c>
       <c r="C48" t="s">
         <v>53</v>
       </c>
       <c r="D48">
-        <v>4</v>
+        <v>3.9571</v>
       </c>
       <c r="E48">
-        <v>3.95</v>
+        <v>3.88</v>
       </c>
       <c r="F48">
-        <v>3.73</v>
+        <v>3.8217</v>
       </c>
       <c r="G48">
-        <v>3.88</v>
+        <v>3.8758</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -1826,22 +1826,22 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>230477</v>
+        <v>230659</v>
       </c>
       <c r="C49" t="s">
         <v>54</v>
       </c>
       <c r="D49">
-        <v>3.94</v>
+        <v>3.8571</v>
       </c>
       <c r="E49">
-        <v>3.83</v>
+        <v>3.9591</v>
       </c>
       <c r="F49">
-        <v>3.87</v>
+        <v>3.8043</v>
       </c>
       <c r="G49">
-        <v>3.87</v>
+        <v>3.8746</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -1849,22 +1849,22 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>230659</v>
+        <v>230477</v>
       </c>
       <c r="C50" t="s">
         <v>55</v>
       </c>
       <c r="D50">
-        <v>3.86</v>
+        <v>3.9357</v>
       </c>
       <c r="E50">
-        <v>3.96</v>
+        <v>3.832</v>
       </c>
       <c r="F50">
-        <v>3.8</v>
+        <v>3.8739</v>
       </c>
       <c r="G50">
-        <v>3.87</v>
+        <v>3.871</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -1878,16 +1878,16 @@
         <v>56</v>
       </c>
       <c r="D51">
-        <v>3.96</v>
+        <v>3.9571</v>
       </c>
       <c r="E51">
         <v>4</v>
       </c>
       <c r="F51">
-        <v>3.67</v>
+        <v>3.6714</v>
       </c>
       <c r="G51">
-        <v>3.87</v>
+        <v>3.8684</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -1895,7 +1895,7 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>230045</v>
+        <v>230613</v>
       </c>
       <c r="C52" t="s">
         <v>57</v>
@@ -1904,13 +1904,13 @@
         <v>4</v>
       </c>
       <c r="E52">
-        <v>3.92</v>
+        <v>3.9455</v>
       </c>
       <c r="F52">
         <v>3.7</v>
       </c>
       <c r="G52">
-        <v>3.86</v>
+        <v>3.8627</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -1927,13 +1927,13 @@
         <v>4</v>
       </c>
       <c r="E53">
-        <v>3.92</v>
+        <v>3.916</v>
       </c>
       <c r="F53">
-        <v>3.71</v>
+        <v>3.713</v>
       </c>
       <c r="G53">
-        <v>3.86</v>
+        <v>3.8597</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -1947,16 +1947,16 @@
         <v>59</v>
       </c>
       <c r="D54">
-        <v>3.89</v>
+        <v>3.8929</v>
       </c>
       <c r="E54">
-        <v>3.84</v>
+        <v>3.844</v>
       </c>
       <c r="F54">
         <v>3.85</v>
       </c>
       <c r="G54">
-        <v>3.86</v>
+        <v>3.8576</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -1964,7 +1964,7 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>230613</v>
+        <v>230045</v>
       </c>
       <c r="C55" t="s">
         <v>60</v>
@@ -1973,13 +1973,13 @@
         <v>4</v>
       </c>
       <c r="E55">
-        <v>3.95</v>
+        <v>3.916</v>
       </c>
       <c r="F55">
-        <v>3.67</v>
+        <v>3.7043</v>
       </c>
       <c r="G55">
-        <v>3.86</v>
+        <v>3.8565</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -1996,13 +1996,13 @@
         <v>4</v>
       </c>
       <c r="E56">
-        <v>3.89</v>
+        <v>3.892</v>
       </c>
       <c r="F56">
-        <v>3.72</v>
+        <v>3.7217</v>
       </c>
       <c r="G56">
-        <v>3.85</v>
+        <v>3.8532</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -2016,16 +2016,16 @@
         <v>62</v>
       </c>
       <c r="D57">
-        <v>3.94</v>
+        <v>3.9357</v>
       </c>
       <c r="E57">
         <v>4</v>
       </c>
       <c r="F57">
-        <v>3.65</v>
+        <v>3.6522</v>
       </c>
       <c r="G57">
-        <v>3.85</v>
+        <v>3.8492</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -2039,16 +2039,16 @@
         <v>63</v>
       </c>
       <c r="D58">
-        <v>3.94</v>
+        <v>3.9357</v>
       </c>
       <c r="E58">
-        <v>3.92</v>
+        <v>3.916</v>
       </c>
       <c r="F58">
-        <v>3.69</v>
+        <v>3.6905</v>
       </c>
       <c r="G58">
-        <v>3.84</v>
+        <v>3.8417</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -2062,16 +2062,16 @@
         <v>64</v>
       </c>
       <c r="D59">
-        <v>3.96</v>
+        <v>3.9571</v>
       </c>
       <c r="E59">
-        <v>3.9</v>
+        <v>3.9045</v>
       </c>
       <c r="F59">
-        <v>3.68</v>
+        <v>3.6783</v>
       </c>
       <c r="G59">
-        <v>3.83</v>
+        <v>3.8288</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -2085,16 +2085,16 @@
         <v>65</v>
       </c>
       <c r="D60">
-        <v>3.96</v>
+        <v>3.9571</v>
       </c>
       <c r="E60">
-        <v>3.9</v>
+        <v>3.9045</v>
       </c>
       <c r="F60">
-        <v>3.67</v>
+        <v>3.6739</v>
       </c>
       <c r="G60">
-        <v>3.83</v>
+        <v>3.8271</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -2102,22 +2102,22 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>230180</v>
+        <v>230470</v>
       </c>
       <c r="C61" t="s">
         <v>66</v>
       </c>
       <c r="D61">
-        <v>3.94</v>
+        <v>4</v>
       </c>
       <c r="E61">
-        <v>3.83</v>
+        <v>4</v>
       </c>
       <c r="F61">
-        <v>3.74</v>
+        <v>3.5261</v>
       </c>
       <c r="G61">
-        <v>3.82</v>
+        <v>3.8242</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -2125,22 +2125,22 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>230353</v>
+        <v>230180</v>
       </c>
       <c r="C62" t="s">
         <v>67</v>
       </c>
       <c r="D62">
-        <v>3.9</v>
+        <v>3.9357</v>
       </c>
       <c r="E62">
-        <v>3.96</v>
+        <v>3.832</v>
       </c>
       <c r="F62">
-        <v>3.61</v>
+        <v>3.7391</v>
       </c>
       <c r="G62">
-        <v>3.82</v>
+        <v>3.821</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -2148,22 +2148,22 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>230470</v>
+        <v>230353</v>
       </c>
       <c r="C63" t="s">
         <v>68</v>
       </c>
       <c r="D63">
-        <v>4</v>
+        <v>3.9</v>
       </c>
       <c r="E63">
-        <v>4</v>
+        <v>3.964</v>
       </c>
       <c r="F63">
-        <v>3.53</v>
+        <v>3.613</v>
       </c>
       <c r="G63">
-        <v>3.82</v>
+        <v>3.8194</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -2180,13 +2180,13 @@
         <v>4</v>
       </c>
       <c r="E64">
-        <v>3.95</v>
+        <v>3.9455</v>
       </c>
       <c r="F64">
-        <v>3.59</v>
+        <v>3.587</v>
       </c>
       <c r="G64">
-        <v>3.82</v>
+        <v>3.8186</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -2200,16 +2200,16 @@
         <v>70</v>
       </c>
       <c r="D65">
-        <v>3.94</v>
+        <v>3.9357</v>
       </c>
       <c r="E65">
-        <v>3.77</v>
+        <v>3.775</v>
       </c>
       <c r="F65">
         <v>3.78</v>
       </c>
       <c r="G65">
-        <v>3.81</v>
+        <v>3.8129</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -2217,22 +2217,22 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <v>230525</v>
+        <v>230726</v>
       </c>
       <c r="C66" t="s">
         <v>71</v>
       </c>
       <c r="D66">
-        <v>4</v>
+        <v>3.8929</v>
       </c>
       <c r="E66">
-        <v>4</v>
+        <v>3.9045</v>
       </c>
       <c r="F66">
-        <v>3.5</v>
+        <v>3.6609</v>
       </c>
       <c r="G66">
-        <v>3.81</v>
+        <v>3.8068</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -2240,22 +2240,22 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <v>230726</v>
+        <v>230525</v>
       </c>
       <c r="C67" t="s">
         <v>72</v>
       </c>
       <c r="D67">
-        <v>3.89</v>
+        <v>4</v>
       </c>
       <c r="E67">
-        <v>3.9</v>
+        <v>4</v>
       </c>
       <c r="F67">
-        <v>3.66</v>
+        <v>3.5</v>
       </c>
       <c r="G67">
-        <v>3.81</v>
+        <v>3.8051</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -2272,13 +2272,13 @@
         <v>4</v>
       </c>
       <c r="E68">
-        <v>3.92</v>
+        <v>3.916</v>
       </c>
       <c r="F68">
-        <v>3.56</v>
+        <v>3.5609</v>
       </c>
       <c r="G68">
-        <v>3.8</v>
+        <v>3.8032</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -2292,16 +2292,16 @@
         <v>74</v>
       </c>
       <c r="D69">
-        <v>3.96</v>
+        <v>3.9571</v>
       </c>
       <c r="E69">
-        <v>3.82</v>
+        <v>3.824</v>
       </c>
       <c r="F69">
-        <v>3.67</v>
+        <v>3.6652</v>
       </c>
       <c r="G69">
-        <v>3.8</v>
+        <v>3.7952</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -2318,13 +2318,13 @@
         <v>4</v>
       </c>
       <c r="E70">
-        <v>3.91</v>
+        <v>3.9143</v>
       </c>
       <c r="F70">
         <v>3.48</v>
       </c>
       <c r="G70">
-        <v>3.79</v>
+        <v>3.7935</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -2332,22 +2332,22 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>230164</v>
+        <v>230280</v>
       </c>
       <c r="C71" t="s">
         <v>76</v>
       </c>
       <c r="D71">
-        <v>3.96</v>
+        <v>3.85</v>
       </c>
       <c r="E71">
-        <v>3.88</v>
+        <v>3.916</v>
       </c>
       <c r="F71">
-        <v>3.59</v>
+        <v>3.6</v>
       </c>
       <c r="G71">
-        <v>3.79</v>
+        <v>3.7932</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -2355,22 +2355,22 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <v>230195</v>
+        <v>230585</v>
       </c>
       <c r="C72" t="s">
         <v>77</v>
       </c>
       <c r="D72">
-        <v>3.96</v>
+        <v>3.9357</v>
       </c>
       <c r="E72">
-        <v>3.8</v>
+        <v>3.9591</v>
       </c>
       <c r="F72">
-        <v>3.68</v>
+        <v>3.5435</v>
       </c>
       <c r="G72">
-        <v>3.79</v>
+        <v>3.7915</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -2378,22 +2378,22 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <v>230280</v>
+        <v>230507</v>
       </c>
       <c r="C73" t="s">
         <v>78</v>
       </c>
       <c r="D73">
-        <v>3.85</v>
+        <v>3.8571</v>
       </c>
       <c r="E73">
-        <v>3.92</v>
+        <v>3.868</v>
       </c>
       <c r="F73">
-        <v>3.6</v>
+        <v>3.645</v>
       </c>
       <c r="G73">
-        <v>3.79</v>
+        <v>3.7898</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -2401,22 +2401,22 @@
         <v>73</v>
       </c>
       <c r="B74">
-        <v>230507</v>
+        <v>230164</v>
       </c>
       <c r="C74" t="s">
         <v>79</v>
       </c>
       <c r="D74">
-        <v>3.86</v>
+        <v>3.9571</v>
       </c>
       <c r="E74">
-        <v>3.87</v>
+        <v>3.88</v>
       </c>
       <c r="F74">
-        <v>3.65</v>
+        <v>3.587</v>
       </c>
       <c r="G74">
-        <v>3.79</v>
+        <v>3.7887</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -2424,22 +2424,22 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <v>230585</v>
+        <v>230195</v>
       </c>
       <c r="C75" t="s">
         <v>80</v>
       </c>
       <c r="D75">
-        <v>3.94</v>
+        <v>3.9571</v>
       </c>
       <c r="E75">
-        <v>3.96</v>
+        <v>3.796</v>
       </c>
       <c r="F75">
-        <v>3.54</v>
+        <v>3.6783</v>
       </c>
       <c r="G75">
-        <v>3.79</v>
+        <v>3.7887</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -2453,16 +2453,16 @@
         <v>81</v>
       </c>
       <c r="D76">
-        <v>3.94</v>
+        <v>3.9357</v>
       </c>
       <c r="E76">
-        <v>3.95</v>
+        <v>3.9455</v>
       </c>
       <c r="F76">
-        <v>3.5</v>
+        <v>3.4957</v>
       </c>
       <c r="G76">
-        <v>3.77</v>
+        <v>3.7678</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -2470,22 +2470,22 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <v>230020</v>
+        <v>230654</v>
       </c>
       <c r="C77" t="s">
         <v>82</v>
       </c>
       <c r="D77">
-        <v>4</v>
+        <v>3.9357</v>
       </c>
       <c r="E77">
-        <v>3.87</v>
+        <v>3.8318</v>
       </c>
       <c r="F77">
-        <v>3.46</v>
+        <v>3.5913</v>
       </c>
       <c r="G77">
-        <v>3.76</v>
+        <v>3.7627</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -2493,22 +2493,22 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <v>230052</v>
+        <v>230020</v>
       </c>
       <c r="C78" t="s">
         <v>83</v>
       </c>
       <c r="D78">
-        <v>3.75</v>
+        <v>4</v>
       </c>
       <c r="E78">
-        <v>3.85</v>
+        <v>3.868</v>
       </c>
       <c r="F78">
-        <v>3.63</v>
+        <v>3.455</v>
       </c>
       <c r="G78">
-        <v>3.76</v>
+        <v>3.7593</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -2516,22 +2516,22 @@
         <v>78</v>
       </c>
       <c r="B79">
-        <v>230654</v>
+        <v>230052</v>
       </c>
       <c r="C79" t="s">
         <v>84</v>
       </c>
       <c r="D79">
-        <v>3.94</v>
+        <v>3.75</v>
       </c>
       <c r="E79">
-        <v>3.83</v>
+        <v>3.85</v>
       </c>
       <c r="F79">
-        <v>3.59</v>
+        <v>3.63</v>
       </c>
       <c r="G79">
-        <v>3.76</v>
+        <v>3.7565</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -2539,22 +2539,22 @@
         <v>79</v>
       </c>
       <c r="B80">
-        <v>230017</v>
+        <v>230327</v>
       </c>
       <c r="C80" t="s">
         <v>85</v>
       </c>
       <c r="D80">
-        <v>3.9</v>
+        <v>3.85</v>
       </c>
       <c r="E80">
-        <v>3.95</v>
+        <v>3.684</v>
       </c>
       <c r="F80">
-        <v>3.44</v>
+        <v>3.7652</v>
       </c>
       <c r="G80">
-        <v>3.75</v>
+        <v>3.7516</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -2562,22 +2562,22 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <v>230327</v>
+        <v>230017</v>
       </c>
       <c r="C81" t="s">
         <v>86</v>
       </c>
       <c r="D81">
-        <v>3.85</v>
+        <v>3.9</v>
       </c>
       <c r="E81">
-        <v>3.68</v>
+        <v>3.952</v>
       </c>
       <c r="F81">
-        <v>3.77</v>
+        <v>3.4417</v>
       </c>
       <c r="G81">
-        <v>3.75</v>
+        <v>3.746</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -2585,22 +2585,22 @@
         <v>81</v>
       </c>
       <c r="B82">
-        <v>230473</v>
+        <v>230727</v>
       </c>
       <c r="C82" t="s">
         <v>87</v>
       </c>
       <c r="D82">
-        <v>3.89</v>
+        <v>3.7857</v>
       </c>
       <c r="E82">
-        <v>3.92</v>
+        <v>3.868</v>
       </c>
       <c r="F82">
-        <v>3.44</v>
+        <v>3.54</v>
       </c>
       <c r="G82">
-        <v>3.74</v>
+        <v>3.7373</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -2608,22 +2608,22 @@
         <v>82</v>
       </c>
       <c r="B83">
-        <v>230727</v>
+        <v>230473</v>
       </c>
       <c r="C83" t="s">
         <v>88</v>
       </c>
       <c r="D83">
-        <v>3.79</v>
+        <v>3.8929</v>
       </c>
       <c r="E83">
-        <v>3.87</v>
+        <v>3.916</v>
       </c>
       <c r="F83">
-        <v>3.54</v>
+        <v>3.4435</v>
       </c>
       <c r="G83">
-        <v>3.74</v>
+        <v>3.7355</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -2637,16 +2637,16 @@
         <v>89</v>
       </c>
       <c r="D84">
-        <v>3.91</v>
+        <v>3.9143</v>
       </c>
       <c r="E84">
-        <v>3.8</v>
+        <v>3.796</v>
       </c>
       <c r="F84">
-        <v>3.56</v>
+        <v>3.5583</v>
       </c>
       <c r="G84">
-        <v>3.73</v>
+        <v>3.7317</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -2660,16 +2660,16 @@
         <v>90</v>
       </c>
       <c r="D85">
-        <v>3.89</v>
+        <v>3.8929</v>
       </c>
       <c r="E85">
-        <v>3.83</v>
+        <v>3.832</v>
       </c>
       <c r="F85">
-        <v>3.51</v>
+        <v>3.5087</v>
       </c>
       <c r="G85">
-        <v>3.73</v>
+        <v>3.7258</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -2677,22 +2677,22 @@
         <v>85</v>
       </c>
       <c r="B86">
-        <v>230077</v>
+        <v>230520</v>
       </c>
       <c r="C86" t="s">
         <v>91</v>
       </c>
       <c r="D86">
-        <v>3.79</v>
+        <v>3.85</v>
       </c>
       <c r="E86">
-        <v>3.75</v>
+        <v>3.85</v>
       </c>
       <c r="F86">
-        <v>3.62</v>
+        <v>3.495</v>
       </c>
       <c r="G86">
-        <v>3.72</v>
+        <v>3.7232</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -2700,22 +2700,22 @@
         <v>86</v>
       </c>
       <c r="B87">
-        <v>230520</v>
+        <v>230077</v>
       </c>
       <c r="C87" t="s">
         <v>92</v>
       </c>
       <c r="D87">
-        <v>3.85</v>
+        <v>3.7857</v>
       </c>
       <c r="E87">
-        <v>3.85</v>
+        <v>3.7536</v>
       </c>
       <c r="F87">
-        <v>3.49</v>
+        <v>3.619</v>
       </c>
       <c r="G87">
-        <v>3.72</v>
+        <v>3.7159</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -2732,13 +2732,13 @@
         <v>3.85</v>
       </c>
       <c r="E88">
-        <v>3.92</v>
+        <v>3.9182</v>
       </c>
       <c r="F88">
-        <v>3.42</v>
+        <v>3.4174</v>
       </c>
       <c r="G88">
-        <v>3.71</v>
+        <v>3.7068</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -2746,22 +2746,22 @@
         <v>88</v>
       </c>
       <c r="B89">
-        <v>230375</v>
+        <v>230444</v>
       </c>
       <c r="C89" t="s">
         <v>94</v>
       </c>
       <c r="D89">
-        <v>3.85</v>
+        <v>3.7857</v>
       </c>
       <c r="E89">
-        <v>3.71</v>
+        <v>3.625</v>
       </c>
       <c r="F89">
-        <v>3.6</v>
+        <v>3.7571</v>
       </c>
       <c r="G89">
-        <v>3.7</v>
+        <v>3.7048</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -2769,22 +2769,22 @@
         <v>89</v>
       </c>
       <c r="B90">
-        <v>230407</v>
+        <v>230375</v>
       </c>
       <c r="C90" t="s">
         <v>95</v>
       </c>
       <c r="D90">
-        <v>4</v>
+        <v>3.85</v>
       </c>
       <c r="E90">
-        <v>3.75</v>
+        <v>3.712</v>
       </c>
       <c r="F90">
-        <v>3.47</v>
+        <v>3.6</v>
       </c>
       <c r="G90">
-        <v>3.7</v>
+        <v>3.7016</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -2792,22 +2792,22 @@
         <v>90</v>
       </c>
       <c r="B91">
-        <v>230444</v>
+        <v>230407</v>
       </c>
       <c r="C91" t="s">
         <v>96</v>
       </c>
       <c r="D91">
-        <v>3.79</v>
+        <v>4</v>
       </c>
       <c r="E91">
-        <v>3.62</v>
+        <v>3.748</v>
       </c>
       <c r="F91">
-        <v>3.76</v>
+        <v>3.4696</v>
       </c>
       <c r="G91">
-        <v>3.7</v>
+        <v>3.7016</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -2815,7 +2815,7 @@
         <v>91</v>
       </c>
       <c r="B92">
-        <v>230261</v>
+        <v>230527</v>
       </c>
       <c r="C92" t="s">
         <v>97</v>
@@ -2824,13 +2824,13 @@
         <v>4</v>
       </c>
       <c r="E92">
-        <v>3.77</v>
+        <v>3.8636</v>
       </c>
       <c r="F92">
-        <v>3.42</v>
+        <v>3.3391</v>
       </c>
       <c r="G92">
-        <v>3.69</v>
+        <v>3.6915</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -2838,22 +2838,22 @@
         <v>92</v>
       </c>
       <c r="B93">
-        <v>230458</v>
+        <v>230261</v>
       </c>
       <c r="C93" t="s">
         <v>98</v>
       </c>
       <c r="D93">
-        <v>3.96</v>
+        <v>4</v>
       </c>
       <c r="E93">
-        <v>3.74</v>
+        <v>3.768</v>
       </c>
       <c r="F93">
-        <v>3.47</v>
+        <v>3.425</v>
       </c>
       <c r="G93">
-        <v>3.69</v>
+        <v>3.6889</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -2861,22 +2861,22 @@
         <v>93</v>
       </c>
       <c r="B94">
-        <v>230527</v>
+        <v>230458</v>
       </c>
       <c r="C94" t="s">
         <v>99</v>
       </c>
       <c r="D94">
-        <v>4</v>
+        <v>3.9571</v>
       </c>
       <c r="E94">
-        <v>3.86</v>
+        <v>3.736</v>
       </c>
       <c r="F94">
-        <v>3.34</v>
+        <v>3.4652</v>
       </c>
       <c r="G94">
-        <v>3.69</v>
+        <v>3.6855</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -2884,22 +2884,22 @@
         <v>94</v>
       </c>
       <c r="B95">
-        <v>230248</v>
+        <v>230735</v>
       </c>
       <c r="C95" t="s">
         <v>100</v>
       </c>
       <c r="D95">
-        <v>3.94</v>
+        <v>3.9357</v>
       </c>
       <c r="E95">
-        <v>3.66</v>
+        <v>3.8182</v>
       </c>
       <c r="F95">
-        <v>3.54</v>
+        <v>3.4</v>
       </c>
       <c r="G95">
-        <v>3.68</v>
+        <v>3.6831</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -2907,22 +2907,22 @@
         <v>95</v>
       </c>
       <c r="B96">
-        <v>230735</v>
+        <v>230248</v>
       </c>
       <c r="C96" t="s">
         <v>101</v>
       </c>
       <c r="D96">
-        <v>3.94</v>
+        <v>3.9357</v>
       </c>
       <c r="E96">
-        <v>3.82</v>
+        <v>3.664</v>
       </c>
       <c r="F96">
-        <v>3.4</v>
+        <v>3.5435</v>
       </c>
       <c r="G96">
-        <v>3.68</v>
+        <v>3.6806</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -2930,22 +2930,22 @@
         <v>96</v>
       </c>
       <c r="B97">
-        <v>230229</v>
+        <v>230581</v>
       </c>
       <c r="C97" t="s">
         <v>102</v>
       </c>
       <c r="D97">
-        <v>3.85</v>
+        <v>3.7929</v>
       </c>
       <c r="E97">
-        <v>3.78</v>
+        <v>3.684</v>
       </c>
       <c r="F97">
-        <v>3.4</v>
+        <v>3.5471</v>
       </c>
       <c r="G97">
-        <v>3.67</v>
+        <v>3.6696</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -2953,22 +2953,22 @@
         <v>97</v>
       </c>
       <c r="B98">
-        <v>230581</v>
+        <v>230229</v>
       </c>
       <c r="C98" t="s">
         <v>103</v>
       </c>
       <c r="D98">
-        <v>3.79</v>
+        <v>3.85</v>
       </c>
       <c r="E98">
-        <v>3.68</v>
+        <v>3.784</v>
       </c>
       <c r="F98">
-        <v>3.55</v>
+        <v>3.4</v>
       </c>
       <c r="G98">
-        <v>3.67</v>
+        <v>3.665</v>
       </c>
     </row>
     <row r="99" spans="1:7">
@@ -2985,13 +2985,13 @@
         <v>4</v>
       </c>
       <c r="E99">
-        <v>3.74</v>
+        <v>3.7364</v>
       </c>
       <c r="F99">
-        <v>3.37</v>
+        <v>3.3739</v>
       </c>
       <c r="G99">
-        <v>3.66</v>
+        <v>3.6576</v>
       </c>
     </row>
     <row r="100" spans="1:7">
@@ -3011,10 +3011,10 @@
         <v>3.6</v>
       </c>
       <c r="F100">
-        <v>3.59</v>
+        <v>3.5913</v>
       </c>
       <c r="G100">
-        <v>3.65</v>
+        <v>3.6532</v>
       </c>
     </row>
     <row r="101" spans="1:7">
@@ -3022,22 +3022,22 @@
         <v>100</v>
       </c>
       <c r="B101">
-        <v>230175</v>
+        <v>230208</v>
       </c>
       <c r="C101" t="s">
         <v>106</v>
       </c>
       <c r="D101">
-        <v>3.96</v>
+        <v>4</v>
       </c>
       <c r="E101">
-        <v>3.7</v>
+        <v>3.636</v>
       </c>
       <c r="F101">
-        <v>3.4</v>
+        <v>3.4609</v>
       </c>
       <c r="G101">
-        <v>3.65</v>
+        <v>3.6532</v>
       </c>
     </row>
     <row r="102" spans="1:7">
@@ -3045,22 +3045,22 @@
         <v>101</v>
       </c>
       <c r="B102">
-        <v>230208</v>
+        <v>230175</v>
       </c>
       <c r="C102" t="s">
         <v>107</v>
       </c>
       <c r="D102">
-        <v>4</v>
+        <v>3.9571</v>
       </c>
       <c r="E102">
-        <v>3.64</v>
+        <v>3.696</v>
       </c>
       <c r="F102">
-        <v>3.46</v>
+        <v>3.4043</v>
       </c>
       <c r="G102">
-        <v>3.65</v>
+        <v>3.6468</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -3068,22 +3068,22 @@
         <v>102</v>
       </c>
       <c r="B103">
-        <v>230238</v>
+        <v>230563</v>
       </c>
       <c r="C103" t="s">
         <v>108</v>
       </c>
       <c r="D103">
-        <v>3.76</v>
+        <v>3.8929</v>
       </c>
       <c r="E103">
-        <v>3.48</v>
+        <v>3.8091</v>
       </c>
       <c r="F103">
-        <v>3.75</v>
+        <v>3.3043</v>
       </c>
       <c r="G103">
-        <v>3.63</v>
+        <v>3.6322</v>
       </c>
     </row>
     <row r="104" spans="1:7">
@@ -3091,22 +3091,22 @@
         <v>103</v>
       </c>
       <c r="B104">
-        <v>230563</v>
+        <v>230238</v>
       </c>
       <c r="C104" t="s">
         <v>109</v>
       </c>
       <c r="D104">
-        <v>3.89</v>
+        <v>3.7643</v>
       </c>
       <c r="E104">
-        <v>3.81</v>
+        <v>3.4786</v>
       </c>
       <c r="F104">
-        <v>3.3</v>
+        <v>3.75</v>
       </c>
       <c r="G104">
-        <v>3.63</v>
+        <v>3.6267</v>
       </c>
     </row>
     <row r="105" spans="1:7">
@@ -3120,16 +3120,16 @@
         <v>110</v>
       </c>
       <c r="D105">
-        <v>3.94</v>
+        <v>3.9357</v>
       </c>
       <c r="E105">
-        <v>3.69</v>
+        <v>3.6947</v>
       </c>
       <c r="F105">
-        <v>3.33</v>
+        <v>3.3348</v>
       </c>
       <c r="G105">
-        <v>3.61</v>
+        <v>3.6071</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -3137,7 +3137,7 @@
         <v>105</v>
       </c>
       <c r="B106">
-        <v>230259</v>
+        <v>230395</v>
       </c>
       <c r="C106" t="s">
         <v>111</v>
@@ -3146,13 +3146,13 @@
         <v>3.85</v>
       </c>
       <c r="E106">
-        <v>3.57</v>
+        <v>3.684</v>
       </c>
       <c r="F106">
-        <v>3.45</v>
+        <v>3.3348</v>
       </c>
       <c r="G106">
-        <v>3.59</v>
+        <v>3.5919</v>
       </c>
     </row>
     <row r="107" spans="1:7">
@@ -3160,7 +3160,7 @@
         <v>106</v>
       </c>
       <c r="B107">
-        <v>230395</v>
+        <v>230259</v>
       </c>
       <c r="C107" t="s">
         <v>112</v>
@@ -3169,13 +3169,13 @@
         <v>3.85</v>
       </c>
       <c r="E107">
-        <v>3.68</v>
+        <v>3.5679</v>
       </c>
       <c r="F107">
-        <v>3.33</v>
+        <v>3.4476</v>
       </c>
       <c r="G107">
-        <v>3.59</v>
+        <v>3.5905</v>
       </c>
     </row>
     <row r="108" spans="1:7">
@@ -3195,10 +3195,10 @@
         <v>3.65</v>
       </c>
       <c r="F108">
-        <v>3.17</v>
+        <v>3.1706</v>
       </c>
       <c r="G108">
-        <v>3.59</v>
+        <v>3.5887</v>
       </c>
     </row>
     <row r="109" spans="1:7">
@@ -3206,22 +3206,22 @@
         <v>108</v>
       </c>
       <c r="B109">
-        <v>230033</v>
+        <v>230636</v>
       </c>
       <c r="C109" t="s">
         <v>114</v>
       </c>
       <c r="D109">
-        <v>3.85</v>
+        <v>3.8929</v>
       </c>
       <c r="E109">
-        <v>3.64</v>
+        <v>3.7364</v>
       </c>
       <c r="F109">
-        <v>3.35</v>
+        <v>3.2391</v>
       </c>
       <c r="G109">
-        <v>3.58</v>
+        <v>3.5797</v>
       </c>
     </row>
     <row r="110" spans="1:7">
@@ -3229,22 +3229,22 @@
         <v>109</v>
       </c>
       <c r="B110">
-        <v>230636</v>
+        <v>230033</v>
       </c>
       <c r="C110" t="s">
         <v>115</v>
       </c>
       <c r="D110">
-        <v>3.89</v>
+        <v>3.85</v>
       </c>
       <c r="E110">
-        <v>3.74</v>
+        <v>3.636</v>
       </c>
       <c r="F110">
-        <v>3.24</v>
+        <v>3.3478</v>
       </c>
       <c r="G110">
-        <v>3.58</v>
+        <v>3.5774</v>
       </c>
     </row>
     <row r="111" spans="1:7">
@@ -3261,13 +3261,13 @@
         <v>4</v>
       </c>
       <c r="E111">
-        <v>3.54</v>
+        <v>3.536</v>
       </c>
       <c r="F111">
-        <v>3.25</v>
+        <v>3.2529</v>
       </c>
       <c r="G111">
-        <v>3.57</v>
+        <v>3.5661</v>
       </c>
     </row>
     <row r="112" spans="1:7">
@@ -3281,16 +3281,16 @@
         <v>117</v>
       </c>
       <c r="D112">
-        <v>3.87</v>
+        <v>3.8714</v>
       </c>
       <c r="E112">
-        <v>3.57</v>
+        <v>3.5727</v>
       </c>
       <c r="F112">
-        <v>3.22</v>
+        <v>3.2217</v>
       </c>
       <c r="G112">
-        <v>3.51</v>
+        <v>3.5068</v>
       </c>
     </row>
     <row r="113" spans="1:7">
@@ -3307,13 +3307,13 @@
         <v>3.85</v>
       </c>
       <c r="E113">
-        <v>3.49</v>
+        <v>3.488</v>
       </c>
       <c r="F113">
         <v>3.25</v>
       </c>
       <c r="G113">
-        <v>3.5</v>
+        <v>3.5018</v>
       </c>
     </row>
     <row r="114" spans="1:7">
@@ -3330,13 +3330,13 @@
         <v>3.85</v>
       </c>
       <c r="E114">
-        <v>3.53</v>
+        <v>3.528</v>
       </c>
       <c r="F114">
-        <v>3.22</v>
+        <v>3.2217</v>
       </c>
       <c r="G114">
-        <v>3.49</v>
+        <v>3.4871</v>
       </c>
     </row>
     <row r="115" spans="1:7">
@@ -3356,10 +3356,10 @@
         <v>3.62</v>
       </c>
       <c r="F115">
-        <v>3.1</v>
+        <v>3.0957</v>
       </c>
       <c r="G115">
-        <v>3.48</v>
+        <v>3.4774</v>
       </c>
     </row>
     <row r="116" spans="1:7">
@@ -3373,16 +3373,16 @@
         <v>121</v>
       </c>
       <c r="D116">
-        <v>3.81</v>
+        <v>3.8071</v>
       </c>
       <c r="E116">
-        <v>3.32</v>
+        <v>3.3179</v>
       </c>
       <c r="F116">
-        <v>2.83</v>
+        <v>2.835</v>
       </c>
       <c r="G116">
-        <v>3.27</v>
+        <v>3.2726</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Literay criticism - EL2410 addition to sem 3
</commit_message>
<xml_diff>
--- a/output/CGPA_Results.xlsx
+++ b/output/CGPA_Results.xlsx
@@ -208,6 +208,9 @@
     <t>PITIWADUGE D.N.</t>
   </si>
   <si>
+    <t>GUNATHUNGA U.A.</t>
+  </si>
+  <si>
     <t>PRISHMIKA H.W.N.</t>
   </si>
   <si>
@@ -226,9 +229,6 @@
     <t>PRIYADARSHANA S.A.D.</t>
   </si>
   <si>
-    <t>GUNATHUNGA U.A.</t>
-  </si>
-  <si>
     <t>WIJESINGHE U.G.S.K.D.</t>
   </si>
   <si>
@@ -325,13 +325,13 @@
     <t>SANTHOSH S.</t>
   </si>
   <si>
+    <t>ABEYWARNA D.H.</t>
+  </si>
+  <si>
     <t>HANSINDU M.M.A.D.</t>
   </si>
   <si>
     <t>UBEYSEKARA V.T.T.</t>
-  </si>
-  <si>
-    <t>ABEYWARNA D.H.</t>
   </si>
   <si>
     <t>GUNASEKARA H.M.</t>
@@ -2056,22 +2056,22 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>230500</v>
+        <v>230218</v>
       </c>
       <c r="C59" t="s">
         <v>64</v>
       </c>
       <c r="D59">
-        <v>3.9571</v>
+        <v>3.9357</v>
       </c>
       <c r="E59">
-        <v>3.9045</v>
+        <v>3.8179</v>
       </c>
       <c r="F59">
-        <v>3.6783</v>
+        <v>3.78</v>
       </c>
       <c r="G59">
-        <v>3.8288</v>
+        <v>3.8323</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -2079,7 +2079,7 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>230629</v>
+        <v>230500</v>
       </c>
       <c r="C60" t="s">
         <v>65</v>
@@ -2091,10 +2091,10 @@
         <v>3.9045</v>
       </c>
       <c r="F60">
-        <v>3.6739</v>
+        <v>3.6783</v>
       </c>
       <c r="G60">
-        <v>3.8271</v>
+        <v>3.8288</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -2102,22 +2102,22 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>230470</v>
+        <v>230629</v>
       </c>
       <c r="C61" t="s">
         <v>66</v>
       </c>
       <c r="D61">
-        <v>4</v>
+        <v>3.9571</v>
       </c>
       <c r="E61">
-        <v>4</v>
+        <v>3.9045</v>
       </c>
       <c r="F61">
-        <v>3.5261</v>
+        <v>3.6739</v>
       </c>
       <c r="G61">
-        <v>3.8242</v>
+        <v>3.8271</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -2125,22 +2125,22 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>230180</v>
+        <v>230470</v>
       </c>
       <c r="C62" t="s">
         <v>67</v>
       </c>
       <c r="D62">
-        <v>3.9357</v>
+        <v>4</v>
       </c>
       <c r="E62">
-        <v>3.832</v>
+        <v>4</v>
       </c>
       <c r="F62">
-        <v>3.7391</v>
+        <v>3.5261</v>
       </c>
       <c r="G62">
-        <v>3.821</v>
+        <v>3.8242</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -2148,22 +2148,22 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>230353</v>
+        <v>230180</v>
       </c>
       <c r="C63" t="s">
         <v>68</v>
       </c>
       <c r="D63">
-        <v>3.9</v>
+        <v>3.9357</v>
       </c>
       <c r="E63">
-        <v>3.964</v>
+        <v>3.832</v>
       </c>
       <c r="F63">
-        <v>3.613</v>
+        <v>3.7391</v>
       </c>
       <c r="G63">
-        <v>3.8194</v>
+        <v>3.821</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -2171,22 +2171,22 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <v>230502</v>
+        <v>230353</v>
       </c>
       <c r="C64" t="s">
         <v>69</v>
       </c>
       <c r="D64">
-        <v>4</v>
+        <v>3.9</v>
       </c>
       <c r="E64">
-        <v>3.9455</v>
+        <v>3.964</v>
       </c>
       <c r="F64">
-        <v>3.587</v>
+        <v>3.613</v>
       </c>
       <c r="G64">
-        <v>3.8186</v>
+        <v>3.8194</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -2194,22 +2194,22 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>230218</v>
+        <v>230502</v>
       </c>
       <c r="C65" t="s">
         <v>70</v>
       </c>
       <c r="D65">
-        <v>3.9357</v>
+        <v>4</v>
       </c>
       <c r="E65">
-        <v>3.775</v>
+        <v>3.9455</v>
       </c>
       <c r="F65">
-        <v>3.78</v>
+        <v>3.587</v>
       </c>
       <c r="G65">
-        <v>3.8129</v>
+        <v>3.8186</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -2953,7 +2953,7 @@
         <v>97</v>
       </c>
       <c r="B98">
-        <v>230229</v>
+        <v>230013</v>
       </c>
       <c r="C98" t="s">
         <v>103</v>
@@ -2962,13 +2962,13 @@
         <v>3.85</v>
       </c>
       <c r="E98">
-        <v>3.784</v>
+        <v>3.6</v>
       </c>
       <c r="F98">
-        <v>3.4</v>
+        <v>3.6385</v>
       </c>
       <c r="G98">
-        <v>3.665</v>
+        <v>3.6692</v>
       </c>
     </row>
     <row r="99" spans="1:7">
@@ -2976,22 +2976,22 @@
         <v>98</v>
       </c>
       <c r="B99">
-        <v>230650</v>
+        <v>230229</v>
       </c>
       <c r="C99" t="s">
         <v>104</v>
       </c>
       <c r="D99">
-        <v>4</v>
+        <v>3.85</v>
       </c>
       <c r="E99">
-        <v>3.7364</v>
+        <v>3.784</v>
       </c>
       <c r="F99">
-        <v>3.3739</v>
+        <v>3.4</v>
       </c>
       <c r="G99">
-        <v>3.6576</v>
+        <v>3.665</v>
       </c>
     </row>
     <row r="100" spans="1:7">
@@ -2999,22 +2999,22 @@
         <v>99</v>
       </c>
       <c r="B100">
-        <v>230013</v>
+        <v>230650</v>
       </c>
       <c r="C100" t="s">
         <v>105</v>
       </c>
       <c r="D100">
-        <v>3.85</v>
+        <v>4</v>
       </c>
       <c r="E100">
-        <v>3.6</v>
+        <v>3.7364</v>
       </c>
       <c r="F100">
-        <v>3.5913</v>
+        <v>3.3739</v>
       </c>
       <c r="G100">
-        <v>3.6532</v>
+        <v>3.6576</v>
       </c>
     </row>
     <row r="101" spans="1:7">

</xml_diff>

<commit_message>
correction.json file grade format corrected
</commit_message>
<xml_diff>
--- a/output/CGPA_Results.xlsx
+++ b/output/CGPA_Results.xlsx
@@ -103,6 +103,9 @@
     <t>DISSANAYAKA D.M.D.P.</t>
   </si>
   <si>
+    <t>IMADUWAGE O.N.H.</t>
+  </si>
+  <si>
     <t>RAHUL B.</t>
   </si>
   <si>
@@ -115,9 +118,6 @@
     <t>DISSANAYAKE G.R.G.K.</t>
   </si>
   <si>
-    <t>IMADUWAGE O.N.H.</t>
-  </si>
-  <si>
     <t>PATHIRANA P.T.S.</t>
   </si>
   <si>
@@ -127,6 +127,9 @@
     <t>ARACHCHI A.D.I.D.</t>
   </si>
   <si>
+    <t>GARUSINGHE S.B.</t>
+  </si>
+  <si>
     <t>KEERAWELLA K.P.C.P.</t>
   </si>
   <si>
@@ -142,9 +145,6 @@
     <t>RASANJANA W.P.G.R.A.</t>
   </si>
   <si>
-    <t>GARUSINGHE S.B.</t>
-  </si>
-  <si>
     <t>KARUNARATHNA G.K.T.</t>
   </si>
   <si>
@@ -313,6 +313,9 @@
     <t>INDUWARA M.L.A.S.</t>
   </si>
   <si>
+    <t>ABEYWARNA D.H.</t>
+  </si>
+  <si>
     <t>PALIHENA H.H.</t>
   </si>
   <si>
@@ -323,9 +326,6 @@
   </si>
   <si>
     <t>SANTHOSH S.</t>
-  </si>
-  <si>
-    <t>ABEYWARNA D.H.</t>
   </si>
   <si>
     <t>HANSINDU M.M.A.D.</t>
@@ -1251,22 +1251,22 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>230508</v>
+        <v>230258</v>
       </c>
       <c r="C24" t="s">
         <v>29</v>
       </c>
       <c r="D24">
-        <v>4</v>
+        <v>3.9357</v>
       </c>
       <c r="E24">
-        <v>4</v>
+        <v>3.964</v>
       </c>
       <c r="F24">
-        <v>3.8826</v>
+        <v>3.9571</v>
       </c>
       <c r="G24">
-        <v>3.9542</v>
+        <v>3.955</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1274,7 +1274,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>230390</v>
+        <v>230508</v>
       </c>
       <c r="C25" t="s">
         <v>30</v>
@@ -1286,10 +1286,10 @@
         <v>4</v>
       </c>
       <c r="F25">
-        <v>3.8739</v>
+        <v>3.8826</v>
       </c>
       <c r="G25">
-        <v>3.9532</v>
+        <v>3.9542</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1297,7 +1297,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>230186</v>
+        <v>230390</v>
       </c>
       <c r="C26" t="s">
         <v>31</v>
@@ -1309,10 +1309,10 @@
         <v>4</v>
       </c>
       <c r="F26">
-        <v>3.8696</v>
+        <v>3.8739</v>
       </c>
       <c r="G26">
-        <v>3.9516</v>
+        <v>3.9532</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1320,7 +1320,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>230159</v>
+        <v>230186</v>
       </c>
       <c r="C27" t="s">
         <v>32</v>
@@ -1329,13 +1329,13 @@
         <v>4</v>
       </c>
       <c r="E27">
-        <v>3.9571</v>
+        <v>4</v>
       </c>
       <c r="F27">
-        <v>3.895</v>
+        <v>3.8696</v>
       </c>
       <c r="G27">
-        <v>3.9468</v>
+        <v>3.9516</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1343,22 +1343,22 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>230258</v>
+        <v>230159</v>
       </c>
       <c r="C28" t="s">
         <v>33</v>
       </c>
       <c r="D28">
-        <v>3.8929</v>
+        <v>4</v>
       </c>
       <c r="E28">
-        <v>3.964</v>
+        <v>3.9571</v>
       </c>
       <c r="F28">
-        <v>3.9571</v>
+        <v>3.895</v>
       </c>
       <c r="G28">
-        <v>3.945</v>
+        <v>3.9468</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1435,7 +1435,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>230332</v>
+        <v>230197</v>
       </c>
       <c r="C32" t="s">
         <v>37</v>
@@ -1444,13 +1444,13 @@
         <v>4</v>
       </c>
       <c r="E32">
-        <v>4</v>
+        <v>3.928</v>
       </c>
       <c r="F32">
-        <v>3.79</v>
+        <v>3.9</v>
       </c>
       <c r="G32">
-        <v>3.9323</v>
+        <v>3.9339</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1458,7 +1458,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>230486</v>
+        <v>230332</v>
       </c>
       <c r="C33" t="s">
         <v>38</v>
@@ -1470,10 +1470,10 @@
         <v>4</v>
       </c>
       <c r="F33">
-        <v>3.8269</v>
+        <v>3.79</v>
       </c>
       <c r="G33">
-        <v>3.9308</v>
+        <v>3.9323</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1481,22 +1481,22 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>230140</v>
+        <v>230486</v>
       </c>
       <c r="C34" t="s">
         <v>39</v>
       </c>
       <c r="D34">
-        <v>3.9357</v>
+        <v>4</v>
       </c>
       <c r="E34">
-        <v>3.964</v>
+        <v>4</v>
       </c>
       <c r="F34">
-        <v>3.8739</v>
+        <v>3.8269</v>
       </c>
       <c r="G34">
-        <v>3.9242</v>
+        <v>3.9308</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1504,22 +1504,22 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>230521</v>
+        <v>230140</v>
       </c>
       <c r="C35" t="s">
         <v>40</v>
       </c>
       <c r="D35">
-        <v>4</v>
+        <v>3.9357</v>
       </c>
       <c r="E35">
-        <v>4</v>
+        <v>3.964</v>
       </c>
       <c r="F35">
-        <v>3.7913</v>
+        <v>3.8739</v>
       </c>
       <c r="G35">
-        <v>3.9186</v>
+        <v>3.9242</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1527,22 +1527,22 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>230536</v>
+        <v>230521</v>
       </c>
       <c r="C36" t="s">
         <v>41</v>
       </c>
       <c r="D36">
-        <v>3.9571</v>
+        <v>4</v>
       </c>
       <c r="E36">
-        <v>3.9591</v>
+        <v>4</v>
       </c>
       <c r="F36">
-        <v>3.8478</v>
+        <v>3.7913</v>
       </c>
       <c r="G36">
-        <v>3.9153</v>
+        <v>3.9186</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1550,22 +1550,22 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>230197</v>
+        <v>230536</v>
       </c>
       <c r="C37" t="s">
         <v>42</v>
       </c>
       <c r="D37">
-        <v>4</v>
+        <v>3.9571</v>
       </c>
       <c r="E37">
-        <v>3.88</v>
+        <v>3.9591</v>
       </c>
       <c r="F37">
-        <v>3.9</v>
+        <v>3.8478</v>
       </c>
       <c r="G37">
-        <v>3.9145</v>
+        <v>3.9153</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -2861,22 +2861,22 @@
         <v>93</v>
       </c>
       <c r="B94">
-        <v>230458</v>
+        <v>230013</v>
       </c>
       <c r="C94" t="s">
         <v>99</v>
       </c>
       <c r="D94">
-        <v>3.9571</v>
+        <v>3.85</v>
       </c>
       <c r="E94">
-        <v>3.736</v>
+        <v>3.648</v>
       </c>
       <c r="F94">
-        <v>3.4652</v>
+        <v>3.6385</v>
       </c>
       <c r="G94">
-        <v>3.6855</v>
+        <v>3.6877</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -2884,22 +2884,22 @@
         <v>94</v>
       </c>
       <c r="B95">
-        <v>230735</v>
+        <v>230458</v>
       </c>
       <c r="C95" t="s">
         <v>100</v>
       </c>
       <c r="D95">
-        <v>3.9357</v>
+        <v>3.9571</v>
       </c>
       <c r="E95">
-        <v>3.8182</v>
+        <v>3.736</v>
       </c>
       <c r="F95">
-        <v>3.4</v>
+        <v>3.4652</v>
       </c>
       <c r="G95">
-        <v>3.6831</v>
+        <v>3.6855</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -2907,7 +2907,7 @@
         <v>95</v>
       </c>
       <c r="B96">
-        <v>230248</v>
+        <v>230735</v>
       </c>
       <c r="C96" t="s">
         <v>101</v>
@@ -2916,13 +2916,13 @@
         <v>3.9357</v>
       </c>
       <c r="E96">
-        <v>3.664</v>
+        <v>3.8182</v>
       </c>
       <c r="F96">
-        <v>3.5435</v>
+        <v>3.4</v>
       </c>
       <c r="G96">
-        <v>3.6806</v>
+        <v>3.6831</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -2930,22 +2930,22 @@
         <v>96</v>
       </c>
       <c r="B97">
-        <v>230581</v>
+        <v>230248</v>
       </c>
       <c r="C97" t="s">
         <v>102</v>
       </c>
       <c r="D97">
-        <v>3.7929</v>
+        <v>3.9357</v>
       </c>
       <c r="E97">
-        <v>3.684</v>
+        <v>3.664</v>
       </c>
       <c r="F97">
-        <v>3.5471</v>
+        <v>3.5435</v>
       </c>
       <c r="G97">
-        <v>3.6696</v>
+        <v>3.6806</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -2953,22 +2953,22 @@
         <v>97</v>
       </c>
       <c r="B98">
-        <v>230013</v>
+        <v>230581</v>
       </c>
       <c r="C98" t="s">
         <v>103</v>
       </c>
       <c r="D98">
-        <v>3.85</v>
+        <v>3.7929</v>
       </c>
       <c r="E98">
-        <v>3.6</v>
+        <v>3.684</v>
       </c>
       <c r="F98">
-        <v>3.6385</v>
+        <v>3.5471</v>
       </c>
       <c r="G98">
-        <v>3.6692</v>
+        <v>3.6696</v>
       </c>
     </row>
     <row r="99" spans="1:7">

</xml_diff>

<commit_message>
telecom recorrected results commit
</commit_message>
<xml_diff>
--- a/output/CGPA_Results.xlsx
+++ b/output/CGPA_Results.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\GitHub\CGPA-gen\output\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF6240E-0C7E-4E1C-A706-90D2F7AEA2A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CGPA" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -118,6 +124,9 @@
     <t>DISSANAYAKE G.R.G.K.</t>
   </si>
   <si>
+    <t>PERERA U.I.H.</t>
+  </si>
+  <si>
     <t>PATHIRANA P.T.S.</t>
   </si>
   <si>
@@ -133,9 +142,6 @@
     <t>KEERAWELLA K.P.C.P.</t>
   </si>
   <si>
-    <t>PERERA U.I.H.</t>
-  </si>
-  <si>
     <t>DHARMAKEERTHI P.K.G.C.L.</t>
   </si>
   <si>
@@ -208,6 +214,9 @@
     <t>PITIWADUGE D.N.</t>
   </si>
   <si>
+    <t>FERNANDO H.M.D.</t>
+  </si>
+  <si>
     <t>GUNATHUNGA U.A.</t>
   </si>
   <si>
@@ -220,9 +229,6 @@
     <t>PEIRIS T.S.R.</t>
   </si>
   <si>
-    <t>FERNANDO H.M.D.</t>
-  </si>
-  <si>
     <t>KUMARA P.K.M.P.</t>
   </si>
   <si>
@@ -238,6 +244,9 @@
     <t>ATHUKORALA U.R.</t>
   </si>
   <si>
+    <t>DISSANAYAKE R.K.T.</t>
+  </si>
+  <si>
     <t>BALASOORIYA B.R.B.D.</t>
   </si>
   <si>
@@ -253,9 +262,6 @@
     <t>RAHMAN M.F.A.</t>
   </si>
   <si>
-    <t>DISSANAYAKE R.K.T.</t>
-  </si>
-  <si>
     <t>GAMAGE SK</t>
   </si>
   <si>
@@ -349,6 +355,9 @@
     <t>PIYUMAL N.P.P.</t>
   </si>
   <si>
+    <t>THARUSHIKA G.K.E.</t>
+  </si>
+  <si>
     <t>MANATUNGA K.D.</t>
   </si>
   <si>
@@ -356,9 +365,6 @@
   </si>
   <si>
     <t>WIJETHILAKA J.S.</t>
-  </si>
-  <si>
-    <t>THARUSHIKA G.K.E.</t>
   </si>
   <si>
     <t>AMARASINGHE A.A.D.K.</t>
@@ -385,8 +391,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -423,13 +429,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -467,7 +481,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -501,6 +515,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -535,9 +550,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -710,14 +726,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -740,7 +759,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -763,7 +782,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -786,7 +805,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -809,7 +828,7 @@
         <v>3.9903</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -826,13 +845,13 @@
         <v>4</v>
       </c>
       <c r="F5">
-        <v>3.9609</v>
+        <v>3.9609000000000001</v>
       </c>
       <c r="G5">
         <v>3.9855</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -849,13 +868,13 @@
         <v>4</v>
       </c>
       <c r="F6">
-        <v>3.9609</v>
+        <v>3.9609000000000001</v>
       </c>
       <c r="G6">
         <v>3.9855</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -872,13 +891,13 @@
         <v>4</v>
       </c>
       <c r="F7">
-        <v>3.9609</v>
+        <v>3.9609000000000001</v>
       </c>
       <c r="G7">
         <v>3.9855</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -901,7 +920,7 @@
         <v>3.9855</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -918,13 +937,13 @@
         <v>4</v>
       </c>
       <c r="F9">
-        <v>3.9609</v>
+        <v>3.9609000000000001</v>
       </c>
       <c r="G9">
         <v>3.9855</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -941,13 +960,13 @@
         <v>4</v>
       </c>
       <c r="F10">
-        <v>3.9571</v>
+        <v>3.9571000000000001</v>
       </c>
       <c r="G10">
-        <v>3.985</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>3.9849999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -964,13 +983,13 @@
         <v>4</v>
       </c>
       <c r="F11">
-        <v>3.9609</v>
+        <v>3.9609000000000001</v>
       </c>
       <c r="G11">
-        <v>3.9847</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>3.9847000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -990,10 +1009,10 @@
         <v>3.95</v>
       </c>
       <c r="G12">
-        <v>3.9833</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>3.9832999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1010,13 +1029,13 @@
         <v>4</v>
       </c>
       <c r="F13">
-        <v>3.925</v>
+        <v>3.9249999999999998</v>
       </c>
       <c r="G13">
         <v>3.9714</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1033,13 +1052,13 @@
         <v>4</v>
       </c>
       <c r="F14">
-        <v>3.925</v>
+        <v>3.9249999999999998</v>
       </c>
       <c r="G14">
         <v>3.9714</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1050,19 +1069,19 @@
         <v>20</v>
       </c>
       <c r="D15">
-        <v>3.9357</v>
+        <v>3.9357000000000002</v>
       </c>
       <c r="E15">
         <v>4</v>
       </c>
       <c r="F15">
-        <v>3.955</v>
+        <v>3.9550000000000001</v>
       </c>
       <c r="G15">
-        <v>3.971</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>3.9710000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1073,19 +1092,19 @@
         <v>21</v>
       </c>
       <c r="D16">
-        <v>3.9357</v>
+        <v>3.9357000000000002</v>
       </c>
       <c r="E16">
         <v>4</v>
       </c>
       <c r="F16">
-        <v>3.9609</v>
+        <v>3.9609000000000001</v>
       </c>
       <c r="G16">
-        <v>3.971</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>3.9710000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1108,7 +1127,7 @@
         <v>3.9695</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1131,7 +1150,7 @@
         <v>3.9661</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1151,10 +1170,10 @@
         <v>3.9</v>
       </c>
       <c r="G19">
-        <v>3.9632</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>3.9632000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1174,10 +1193,10 @@
         <v>3.9</v>
       </c>
       <c r="G20">
-        <v>3.9629</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>3.9628999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1200,7 +1219,7 @@
         <v>3.9619</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1211,7 +1230,7 @@
         <v>27</v>
       </c>
       <c r="D22">
-        <v>3.9571</v>
+        <v>3.9571000000000001</v>
       </c>
       <c r="E22">
         <v>4</v>
@@ -1223,7 +1242,7 @@
         <v>3.9613</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1237,16 +1256,16 @@
         <v>4</v>
       </c>
       <c r="E23">
-        <v>3.928</v>
+        <v>3.9279999999999999</v>
       </c>
       <c r="F23">
-        <v>3.9571</v>
+        <v>3.9571000000000001</v>
       </c>
       <c r="G23">
-        <v>3.955</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>3.9550000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1257,19 +1276,19 @@
         <v>29</v>
       </c>
       <c r="D24">
-        <v>3.9357</v>
+        <v>3.9357000000000002</v>
       </c>
       <c r="E24">
         <v>3.964</v>
       </c>
       <c r="F24">
-        <v>3.9571</v>
+        <v>3.9571000000000001</v>
       </c>
       <c r="G24">
-        <v>3.955</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+        <v>3.9550000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1286,13 +1305,13 @@
         <v>4</v>
       </c>
       <c r="F25">
-        <v>3.8826</v>
+        <v>3.8826000000000001</v>
       </c>
       <c r="G25">
-        <v>3.9542</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>3.9542000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1309,13 +1328,13 @@
         <v>4</v>
       </c>
       <c r="F26">
-        <v>3.8739</v>
+        <v>3.8738999999999999</v>
       </c>
       <c r="G26">
-        <v>3.9532</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+        <v>3.9531999999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1332,13 +1351,13 @@
         <v>4</v>
       </c>
       <c r="F27">
-        <v>3.8696</v>
+        <v>3.8696000000000002</v>
       </c>
       <c r="G27">
         <v>3.9516</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1352,90 +1371,90 @@
         <v>4</v>
       </c>
       <c r="E28">
-        <v>3.9571</v>
+        <v>3.9571000000000001</v>
       </c>
       <c r="F28">
         <v>3.895</v>
       </c>
       <c r="G28">
-        <v>3.9468</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+        <v>3.9468000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29">
-        <v>230468</v>
+        <v>230486</v>
       </c>
       <c r="C29" t="s">
         <v>34</v>
       </c>
       <c r="D29">
-        <v>3.9143</v>
+        <v>4</v>
       </c>
       <c r="E29">
         <v>4</v>
       </c>
       <c r="F29">
-        <v>3.8957</v>
+        <v>3.8614999999999999</v>
       </c>
       <c r="G29">
-        <v>3.9419</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+        <v>3.9445999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30">
-        <v>230566</v>
+        <v>230468</v>
       </c>
       <c r="C30" t="s">
         <v>35</v>
       </c>
       <c r="D30">
-        <v>3.9571</v>
+        <v>3.9142999999999999</v>
       </c>
       <c r="E30">
         <v>4</v>
       </c>
       <c r="F30">
-        <v>3.8846</v>
+        <v>3.8957000000000002</v>
       </c>
       <c r="G30">
         <v>3.9419</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31">
-        <v>230051</v>
+        <v>230566</v>
       </c>
       <c r="C31" t="s">
         <v>36</v>
       </c>
       <c r="D31">
-        <v>4</v>
+        <v>3.9571000000000001</v>
       </c>
       <c r="E31">
         <v>4</v>
       </c>
       <c r="F31">
-        <v>3.8304</v>
+        <v>3.8845999999999998</v>
       </c>
       <c r="G31">
-        <v>3.9371</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+        <v>3.9419</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32">
-        <v>230197</v>
+        <v>230051</v>
       </c>
       <c r="C32" t="s">
         <v>37</v>
@@ -1444,21 +1463,21 @@
         <v>4</v>
       </c>
       <c r="E32">
-        <v>3.928</v>
+        <v>4</v>
       </c>
       <c r="F32">
-        <v>3.9</v>
+        <v>3.8304</v>
       </c>
       <c r="G32">
-        <v>3.9339</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+        <v>3.9371</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33">
-        <v>230332</v>
+        <v>230197</v>
       </c>
       <c r="C33" t="s">
         <v>38</v>
@@ -1467,21 +1486,21 @@
         <v>4</v>
       </c>
       <c r="E33">
-        <v>4</v>
+        <v>3.9279999999999999</v>
       </c>
       <c r="F33">
-        <v>3.79</v>
+        <v>3.9</v>
       </c>
       <c r="G33">
-        <v>3.9323</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
+        <v>3.9339</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34">
-        <v>230486</v>
+        <v>230332</v>
       </c>
       <c r="C34" t="s">
         <v>39</v>
@@ -1493,13 +1512,13 @@
         <v>4</v>
       </c>
       <c r="F34">
-        <v>3.8269</v>
+        <v>3.79</v>
       </c>
       <c r="G34">
-        <v>3.9308</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
+        <v>3.9323000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1510,19 +1529,19 @@
         <v>40</v>
       </c>
       <c r="D35">
-        <v>3.9357</v>
+        <v>3.9357000000000002</v>
       </c>
       <c r="E35">
         <v>3.964</v>
       </c>
       <c r="F35">
-        <v>3.8739</v>
+        <v>3.8738999999999999</v>
       </c>
       <c r="G35">
-        <v>3.9242</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
+        <v>3.9241999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1539,13 +1558,13 @@
         <v>4</v>
       </c>
       <c r="F36">
-        <v>3.7913</v>
+        <v>3.7913000000000001</v>
       </c>
       <c r="G36">
-        <v>3.9186</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
+        <v>3.9186000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1556,19 +1575,19 @@
         <v>42</v>
       </c>
       <c r="D37">
-        <v>3.9571</v>
+        <v>3.9571000000000001</v>
       </c>
       <c r="E37">
-        <v>3.9591</v>
+        <v>3.9590999999999998</v>
       </c>
       <c r="F37">
-        <v>3.8478</v>
+        <v>3.8477999999999999</v>
       </c>
       <c r="G37">
-        <v>3.9153</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
+        <v>3.9152999999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1582,16 +1601,16 @@
         <v>4</v>
       </c>
       <c r="E38">
-        <v>3.916</v>
+        <v>3.9159999999999999</v>
       </c>
       <c r="F38">
-        <v>3.8625</v>
+        <v>3.8624999999999998</v>
       </c>
       <c r="G38">
-        <v>3.9143</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
+        <v>3.9142999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1611,10 +1630,10 @@
         <v>3.8304</v>
       </c>
       <c r="G39">
-        <v>3.9085</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
+        <v>3.9085000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1628,16 +1647,16 @@
         <v>4</v>
       </c>
       <c r="E40">
-        <v>3.9045</v>
+        <v>3.9045000000000001</v>
       </c>
       <c r="F40">
-        <v>3.8478</v>
+        <v>3.8477999999999999</v>
       </c>
       <c r="G40">
         <v>3.9051</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1654,13 +1673,13 @@
         <v>4</v>
       </c>
       <c r="F41">
-        <v>3.7217</v>
+        <v>3.7216999999999998</v>
       </c>
       <c r="G41">
-        <v>3.8968</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
+        <v>3.8967999999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1674,7 +1693,7 @@
         <v>4</v>
       </c>
       <c r="E42">
-        <v>3.916</v>
+        <v>3.9159999999999999</v>
       </c>
       <c r="F42">
         <v>3.8043</v>
@@ -1683,7 +1702,7 @@
         <v>3.8935</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1706,7 +1725,7 @@
         <v>3.8855</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1723,13 +1742,13 @@
         <v>3.964</v>
       </c>
       <c r="F44">
-        <v>3.7143</v>
+        <v>3.7143000000000002</v>
       </c>
       <c r="G44">
-        <v>3.885</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
+        <v>3.8849999999999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1746,13 +1765,13 @@
         <v>3.952</v>
       </c>
       <c r="F45">
-        <v>3.7304</v>
+        <v>3.7303999999999999</v>
       </c>
       <c r="G45">
-        <v>3.8806</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
+        <v>3.8805999999999998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1763,19 +1782,19 @@
         <v>51</v>
       </c>
       <c r="D46">
-        <v>3.9357</v>
+        <v>3.9357000000000002</v>
       </c>
       <c r="E46">
         <v>4</v>
       </c>
       <c r="F46">
-        <v>3.713</v>
+        <v>3.7130000000000001</v>
       </c>
       <c r="G46">
         <v>3.879</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1786,19 +1805,19 @@
         <v>52</v>
       </c>
       <c r="D47">
-        <v>3.9357</v>
+        <v>3.9357000000000002</v>
       </c>
       <c r="E47">
         <v>4</v>
       </c>
       <c r="F47">
-        <v>3.7043</v>
+        <v>3.7042999999999999</v>
       </c>
       <c r="G47">
-        <v>3.8758</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
+        <v>3.8757999999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1809,19 +1828,19 @@
         <v>53</v>
       </c>
       <c r="D48">
-        <v>3.9571</v>
+        <v>3.9571000000000001</v>
       </c>
       <c r="E48">
         <v>3.88</v>
       </c>
       <c r="F48">
-        <v>3.8217</v>
+        <v>3.8216999999999999</v>
       </c>
       <c r="G48">
-        <v>3.8758</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7">
+        <v>3.8757999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1835,7 +1854,7 @@
         <v>3.8571</v>
       </c>
       <c r="E49">
-        <v>3.9591</v>
+        <v>3.9590999999999998</v>
       </c>
       <c r="F49">
         <v>3.8043</v>
@@ -1844,7 +1863,7 @@
         <v>3.8746</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1855,19 +1874,19 @@
         <v>55</v>
       </c>
       <c r="D50">
-        <v>3.9357</v>
+        <v>3.9357000000000002</v>
       </c>
       <c r="E50">
-        <v>3.832</v>
+        <v>3.8319999999999999</v>
       </c>
       <c r="F50">
-        <v>3.8739</v>
+        <v>3.8738999999999999</v>
       </c>
       <c r="G50">
         <v>3.871</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1878,19 +1897,19 @@
         <v>56</v>
       </c>
       <c r="D51">
-        <v>3.9571</v>
+        <v>3.9571000000000001</v>
       </c>
       <c r="E51">
         <v>4</v>
       </c>
       <c r="F51">
-        <v>3.6714</v>
+        <v>3.6714000000000002</v>
       </c>
       <c r="G51">
-        <v>3.8684</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7">
+        <v>3.8683999999999998</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1910,10 +1929,10 @@
         <v>3.7</v>
       </c>
       <c r="G52">
-        <v>3.8627</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7">
+        <v>3.8626999999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1927,16 +1946,16 @@
         <v>4</v>
       </c>
       <c r="E53">
-        <v>3.916</v>
+        <v>3.9159999999999999</v>
       </c>
       <c r="F53">
-        <v>3.713</v>
+        <v>3.7130000000000001</v>
       </c>
       <c r="G53">
-        <v>3.8597</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7">
+        <v>3.8597000000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1950,16 +1969,16 @@
         <v>3.8929</v>
       </c>
       <c r="E54">
-        <v>3.844</v>
+        <v>3.8439999999999999</v>
       </c>
       <c r="F54">
         <v>3.85</v>
       </c>
       <c r="G54">
-        <v>3.8576</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7">
+        <v>3.8576000000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1973,16 +1992,16 @@
         <v>4</v>
       </c>
       <c r="E55">
-        <v>3.916</v>
+        <v>3.9159999999999999</v>
       </c>
       <c r="F55">
-        <v>3.7043</v>
+        <v>3.7042999999999999</v>
       </c>
       <c r="G55">
         <v>3.8565</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1996,16 +2015,16 @@
         <v>4</v>
       </c>
       <c r="E56">
-        <v>3.892</v>
+        <v>3.8919999999999999</v>
       </c>
       <c r="F56">
-        <v>3.7217</v>
+        <v>3.7216999999999998</v>
       </c>
       <c r="G56">
-        <v>3.8532</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7">
+        <v>3.8532000000000002</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2016,19 +2035,19 @@
         <v>62</v>
       </c>
       <c r="D57">
-        <v>3.9357</v>
+        <v>3.9357000000000002</v>
       </c>
       <c r="E57">
         <v>4</v>
       </c>
       <c r="F57">
-        <v>3.6522</v>
+        <v>3.6522000000000001</v>
       </c>
       <c r="G57">
-        <v>3.8492</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7">
+        <v>3.8492000000000002</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2039,134 +2058,134 @@
         <v>63</v>
       </c>
       <c r="D58">
-        <v>3.9357</v>
+        <v>3.9357000000000002</v>
       </c>
       <c r="E58">
-        <v>3.916</v>
+        <v>3.9159999999999999</v>
       </c>
       <c r="F58">
-        <v>3.6905</v>
+        <v>3.6905000000000001</v>
       </c>
       <c r="G58">
-        <v>3.8417</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7">
+        <v>3.8416999999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59">
-        <v>230218</v>
+        <v>230180</v>
       </c>
       <c r="C59" t="s">
         <v>64</v>
       </c>
       <c r="D59">
-        <v>3.9357</v>
+        <v>3.9357000000000002</v>
       </c>
       <c r="E59">
-        <v>3.8179</v>
+        <v>3.8319999999999999</v>
       </c>
       <c r="F59">
-        <v>3.78</v>
+        <v>3.7783000000000002</v>
       </c>
       <c r="G59">
-        <v>3.8323</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7">
+        <v>3.8355000000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60">
-        <v>230500</v>
+        <v>230218</v>
       </c>
       <c r="C60" t="s">
         <v>65</v>
       </c>
       <c r="D60">
-        <v>3.9571</v>
+        <v>3.9357000000000002</v>
       </c>
       <c r="E60">
-        <v>3.9045</v>
+        <v>3.8178999999999998</v>
       </c>
       <c r="F60">
-        <v>3.6783</v>
+        <v>3.78</v>
       </c>
       <c r="G60">
-        <v>3.8288</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7">
+        <v>3.8323</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61">
-        <v>230629</v>
+        <v>230500</v>
       </c>
       <c r="C61" t="s">
         <v>66</v>
       </c>
       <c r="D61">
-        <v>3.9571</v>
+        <v>3.9571000000000001</v>
       </c>
       <c r="E61">
-        <v>3.9045</v>
+        <v>3.9045000000000001</v>
       </c>
       <c r="F61">
-        <v>3.6739</v>
+        <v>3.6783000000000001</v>
       </c>
       <c r="G61">
-        <v>3.8271</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7">
+        <v>3.8288000000000002</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62">
-        <v>230470</v>
+        <v>230629</v>
       </c>
       <c r="C62" t="s">
         <v>67</v>
       </c>
       <c r="D62">
-        <v>4</v>
+        <v>3.9571000000000001</v>
       </c>
       <c r="E62">
-        <v>4</v>
+        <v>3.9045000000000001</v>
       </c>
       <c r="F62">
-        <v>3.5261</v>
+        <v>3.6739000000000002</v>
       </c>
       <c r="G62">
-        <v>3.8242</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7">
+        <v>3.8271000000000002</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63">
-        <v>230180</v>
+        <v>230470</v>
       </c>
       <c r="C63" t="s">
         <v>68</v>
       </c>
       <c r="D63">
-        <v>3.9357</v>
+        <v>4</v>
       </c>
       <c r="E63">
-        <v>3.832</v>
+        <v>4</v>
       </c>
       <c r="F63">
-        <v>3.7391</v>
+        <v>3.5261</v>
       </c>
       <c r="G63">
-        <v>3.821</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7">
+        <v>3.8241999999999998</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2186,10 +2205,10 @@
         <v>3.613</v>
       </c>
       <c r="G64">
-        <v>3.8194</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7">
+        <v>3.8193999999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2206,13 +2225,13 @@
         <v>3.9455</v>
       </c>
       <c r="F65">
-        <v>3.587</v>
+        <v>3.5870000000000002</v>
       </c>
       <c r="G65">
         <v>3.8186</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2226,16 +2245,16 @@
         <v>3.8929</v>
       </c>
       <c r="E66">
-        <v>3.9045</v>
+        <v>3.9045000000000001</v>
       </c>
       <c r="F66">
-        <v>3.6609</v>
+        <v>3.6608999999999998</v>
       </c>
       <c r="G66">
         <v>3.8068</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2255,10 +2274,10 @@
         <v>3.5</v>
       </c>
       <c r="G67">
-        <v>3.8051</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7">
+        <v>3.8050999999999999</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2272,154 +2291,154 @@
         <v>4</v>
       </c>
       <c r="E68">
-        <v>3.916</v>
+        <v>3.9159999999999999</v>
       </c>
       <c r="F68">
-        <v>3.5609</v>
+        <v>3.5609000000000002</v>
       </c>
       <c r="G68">
-        <v>3.8032</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7">
+        <v>3.8031999999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69">
-        <v>230070</v>
+        <v>230164</v>
       </c>
       <c r="C69" t="s">
         <v>74</v>
       </c>
       <c r="D69">
-        <v>3.9571</v>
+        <v>3.9571000000000001</v>
       </c>
       <c r="E69">
-        <v>3.824</v>
+        <v>3.88</v>
       </c>
       <c r="F69">
-        <v>3.6652</v>
+        <v>3.6261000000000001</v>
       </c>
       <c r="G69">
-        <v>3.7952</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7">
+        <v>3.8031999999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70">
-        <v>230016</v>
+        <v>230070</v>
       </c>
       <c r="C70" t="s">
         <v>75</v>
       </c>
       <c r="D70">
-        <v>4</v>
+        <v>3.9571000000000001</v>
       </c>
       <c r="E70">
-        <v>3.9143</v>
+        <v>3.8239999999999998</v>
       </c>
       <c r="F70">
-        <v>3.48</v>
+        <v>3.6652</v>
       </c>
       <c r="G70">
-        <v>3.7935</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7">
+        <v>3.7951999999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71">
-        <v>230280</v>
+        <v>230016</v>
       </c>
       <c r="C71" t="s">
         <v>76</v>
       </c>
       <c r="D71">
-        <v>3.85</v>
+        <v>4</v>
       </c>
       <c r="E71">
-        <v>3.916</v>
+        <v>3.9142999999999999</v>
       </c>
       <c r="F71">
-        <v>3.6</v>
+        <v>3.48</v>
       </c>
       <c r="G71">
-        <v>3.7932</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7">
+        <v>3.7934999999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="B72">
-        <v>230585</v>
+        <v>230280</v>
       </c>
       <c r="C72" t="s">
         <v>77</v>
       </c>
       <c r="D72">
-        <v>3.9357</v>
+        <v>3.85</v>
       </c>
       <c r="E72">
-        <v>3.9591</v>
+        <v>3.9159999999999999</v>
       </c>
       <c r="F72">
-        <v>3.5435</v>
+        <v>3.6</v>
       </c>
       <c r="G72">
-        <v>3.7915</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7">
+        <v>3.7932000000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73">
-        <v>230507</v>
+        <v>230585</v>
       </c>
       <c r="C73" t="s">
         <v>78</v>
       </c>
       <c r="D73">
-        <v>3.8571</v>
+        <v>3.9357000000000002</v>
       </c>
       <c r="E73">
-        <v>3.868</v>
+        <v>3.9590999999999998</v>
       </c>
       <c r="F73">
-        <v>3.645</v>
+        <v>3.5434999999999999</v>
       </c>
       <c r="G73">
-        <v>3.7898</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7">
+        <v>3.7915000000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
       <c r="B74">
-        <v>230164</v>
+        <v>230507</v>
       </c>
       <c r="C74" t="s">
         <v>79</v>
       </c>
       <c r="D74">
-        <v>3.9571</v>
+        <v>3.8571</v>
       </c>
       <c r="E74">
-        <v>3.88</v>
+        <v>3.8679999999999999</v>
       </c>
       <c r="F74">
-        <v>3.587</v>
+        <v>3.645</v>
       </c>
       <c r="G74">
-        <v>3.7887</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7">
+        <v>3.7898000000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2430,19 +2449,19 @@
         <v>80</v>
       </c>
       <c r="D75">
-        <v>3.9571</v>
+        <v>3.9571000000000001</v>
       </c>
       <c r="E75">
-        <v>3.796</v>
+        <v>3.7959999999999998</v>
       </c>
       <c r="F75">
-        <v>3.6783</v>
+        <v>3.6783000000000001</v>
       </c>
       <c r="G75">
         <v>3.7887</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2453,19 +2472,19 @@
         <v>81</v>
       </c>
       <c r="D76">
-        <v>3.9357</v>
+        <v>3.9357000000000002</v>
       </c>
       <c r="E76">
         <v>3.9455</v>
       </c>
       <c r="F76">
-        <v>3.4957</v>
+        <v>3.4956999999999998</v>
       </c>
       <c r="G76">
-        <v>3.7678</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7">
+        <v>3.7677999999999998</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2476,19 +2495,19 @@
         <v>82</v>
       </c>
       <c r="D77">
-        <v>3.9357</v>
+        <v>3.9357000000000002</v>
       </c>
       <c r="E77">
-        <v>3.8318</v>
+        <v>3.8317999999999999</v>
       </c>
       <c r="F77">
-        <v>3.5913</v>
+        <v>3.5912999999999999</v>
       </c>
       <c r="G77">
-        <v>3.7627</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7">
+        <v>3.7627000000000002</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2502,16 +2521,16 @@
         <v>4</v>
       </c>
       <c r="E78">
-        <v>3.868</v>
+        <v>3.8679999999999999</v>
       </c>
       <c r="F78">
-        <v>3.455</v>
+        <v>3.4550000000000001</v>
       </c>
       <c r="G78">
-        <v>3.7593</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7">
+        <v>3.7593000000000001</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2534,7 +2553,7 @@
         <v>3.7565</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2548,16 +2567,16 @@
         <v>3.85</v>
       </c>
       <c r="E80">
-        <v>3.684</v>
+        <v>3.6840000000000002</v>
       </c>
       <c r="F80">
-        <v>3.7652</v>
+        <v>3.7652000000000001</v>
       </c>
       <c r="G80">
-        <v>3.7516</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7">
+        <v>3.7515999999999998</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2580,7 +2599,7 @@
         <v>3.746</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2591,19 +2610,19 @@
         <v>87</v>
       </c>
       <c r="D82">
-        <v>3.7857</v>
+        <v>3.7856999999999998</v>
       </c>
       <c r="E82">
-        <v>3.868</v>
+        <v>3.8679999999999999</v>
       </c>
       <c r="F82">
         <v>3.54</v>
       </c>
       <c r="G82">
-        <v>3.7373</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7">
+        <v>3.7372999999999998</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
@@ -2617,16 +2636,16 @@
         <v>3.8929</v>
       </c>
       <c r="E83">
-        <v>3.916</v>
+        <v>3.9159999999999999</v>
       </c>
       <c r="F83">
-        <v>3.4435</v>
+        <v>3.4434999999999998</v>
       </c>
       <c r="G83">
         <v>3.7355</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2637,10 +2656,10 @@
         <v>89</v>
       </c>
       <c r="D84">
-        <v>3.9143</v>
+        <v>3.9142999999999999</v>
       </c>
       <c r="E84">
-        <v>3.796</v>
+        <v>3.7959999999999998</v>
       </c>
       <c r="F84">
         <v>3.5583</v>
@@ -2649,7 +2668,7 @@
         <v>3.7317</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2663,16 +2682,16 @@
         <v>3.8929</v>
       </c>
       <c r="E85">
-        <v>3.832</v>
+        <v>3.8319999999999999</v>
       </c>
       <c r="F85">
-        <v>3.5087</v>
+        <v>3.5087000000000002</v>
       </c>
       <c r="G85">
         <v>3.7258</v>
       </c>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>85</v>
       </c>
@@ -2689,13 +2708,13 @@
         <v>3.85</v>
       </c>
       <c r="F86">
-        <v>3.495</v>
+        <v>3.4950000000000001</v>
       </c>
       <c r="G86">
-        <v>3.7232</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7">
+        <v>3.7231999999999998</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2706,19 +2725,19 @@
         <v>92</v>
       </c>
       <c r="D87">
-        <v>3.7857</v>
+        <v>3.7856999999999998</v>
       </c>
       <c r="E87">
         <v>3.7536</v>
       </c>
       <c r="F87">
-        <v>3.619</v>
+        <v>3.6190000000000002</v>
       </c>
       <c r="G87">
         <v>3.7159</v>
       </c>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>87</v>
       </c>
@@ -2732,16 +2751,16 @@
         <v>3.85</v>
       </c>
       <c r="E88">
-        <v>3.9182</v>
+        <v>3.9182000000000001</v>
       </c>
       <c r="F88">
-        <v>3.4174</v>
+        <v>3.4174000000000002</v>
       </c>
       <c r="G88">
-        <v>3.7068</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7">
+        <v>3.7067999999999999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>88</v>
       </c>
@@ -2752,19 +2771,19 @@
         <v>94</v>
       </c>
       <c r="D89">
-        <v>3.7857</v>
+        <v>3.7856999999999998</v>
       </c>
       <c r="E89">
         <v>3.625</v>
       </c>
       <c r="F89">
-        <v>3.7571</v>
+        <v>3.7570999999999999</v>
       </c>
       <c r="G89">
-        <v>3.7048</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7">
+        <v>3.7048000000000001</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>89</v>
       </c>
@@ -2778,7 +2797,7 @@
         <v>3.85</v>
       </c>
       <c r="E90">
-        <v>3.712</v>
+        <v>3.7120000000000002</v>
       </c>
       <c r="F90">
         <v>3.6</v>
@@ -2787,7 +2806,7 @@
         <v>3.7016</v>
       </c>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>90</v>
       </c>
@@ -2801,16 +2820,16 @@
         <v>4</v>
       </c>
       <c r="E91">
-        <v>3.748</v>
+        <v>3.7480000000000002</v>
       </c>
       <c r="F91">
-        <v>3.4696</v>
+        <v>3.4695999999999998</v>
       </c>
       <c r="G91">
         <v>3.7016</v>
       </c>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>91</v>
       </c>
@@ -2824,16 +2843,16 @@
         <v>4</v>
       </c>
       <c r="E92">
-        <v>3.8636</v>
+        <v>3.8635999999999999</v>
       </c>
       <c r="F92">
-        <v>3.3391</v>
+        <v>3.3391000000000002</v>
       </c>
       <c r="G92">
         <v>3.6915</v>
       </c>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>92</v>
       </c>
@@ -2847,16 +2866,16 @@
         <v>4</v>
       </c>
       <c r="E93">
-        <v>3.768</v>
+        <v>3.7679999999999998</v>
       </c>
       <c r="F93">
-        <v>3.425</v>
+        <v>3.4249999999999998</v>
       </c>
       <c r="G93">
-        <v>3.6889</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7">
+        <v>3.6888999999999998</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>93</v>
       </c>
@@ -2870,16 +2889,16 @@
         <v>3.85</v>
       </c>
       <c r="E94">
-        <v>3.648</v>
+        <v>3.6480000000000001</v>
       </c>
       <c r="F94">
-        <v>3.6385</v>
+        <v>3.6385000000000001</v>
       </c>
       <c r="G94">
         <v>3.6877</v>
       </c>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>94</v>
       </c>
@@ -2890,19 +2909,19 @@
         <v>100</v>
       </c>
       <c r="D95">
-        <v>3.9571</v>
+        <v>3.9571000000000001</v>
       </c>
       <c r="E95">
-        <v>3.736</v>
+        <v>3.7360000000000002</v>
       </c>
       <c r="F95">
-        <v>3.4652</v>
+        <v>3.4651999999999998</v>
       </c>
       <c r="G95">
-        <v>3.6855</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7">
+        <v>3.6855000000000002</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>95</v>
       </c>
@@ -2913,7 +2932,7 @@
         <v>101</v>
       </c>
       <c r="D96">
-        <v>3.9357</v>
+        <v>3.9357000000000002</v>
       </c>
       <c r="E96">
         <v>3.8182</v>
@@ -2925,7 +2944,7 @@
         <v>3.6831</v>
       </c>
     </row>
-    <row r="97" spans="1:7">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>96</v>
       </c>
@@ -2936,19 +2955,19 @@
         <v>102</v>
       </c>
       <c r="D97">
-        <v>3.9357</v>
+        <v>3.9357000000000002</v>
       </c>
       <c r="E97">
-        <v>3.664</v>
+        <v>3.6640000000000001</v>
       </c>
       <c r="F97">
-        <v>3.5435</v>
+        <v>3.5434999999999999</v>
       </c>
       <c r="G97">
-        <v>3.6806</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7">
+        <v>3.6806000000000001</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>97</v>
       </c>
@@ -2959,19 +2978,19 @@
         <v>103</v>
       </c>
       <c r="D98">
-        <v>3.7929</v>
+        <v>3.7928999999999999</v>
       </c>
       <c r="E98">
-        <v>3.684</v>
+        <v>3.6840000000000002</v>
       </c>
       <c r="F98">
-        <v>3.5471</v>
+        <v>3.5470999999999999</v>
       </c>
       <c r="G98">
         <v>3.6696</v>
       </c>
     </row>
-    <row r="99" spans="1:7">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>98</v>
       </c>
@@ -2985,7 +3004,7 @@
         <v>3.85</v>
       </c>
       <c r="E99">
-        <v>3.784</v>
+        <v>3.7839999999999998</v>
       </c>
       <c r="F99">
         <v>3.4</v>
@@ -2994,7 +3013,7 @@
         <v>3.665</v>
       </c>
     </row>
-    <row r="100" spans="1:7">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>99</v>
       </c>
@@ -3008,16 +3027,16 @@
         <v>4</v>
       </c>
       <c r="E100">
-        <v>3.7364</v>
+        <v>3.7364000000000002</v>
       </c>
       <c r="F100">
-        <v>3.3739</v>
+        <v>3.3738999999999999</v>
       </c>
       <c r="G100">
         <v>3.6576</v>
       </c>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>100</v>
       </c>
@@ -3031,16 +3050,16 @@
         <v>4</v>
       </c>
       <c r="E101">
-        <v>3.636</v>
+        <v>3.6360000000000001</v>
       </c>
       <c r="F101">
-        <v>3.4609</v>
+        <v>3.4609000000000001</v>
       </c>
       <c r="G101">
         <v>3.6532</v>
       </c>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>101</v>
       </c>
@@ -3051,19 +3070,19 @@
         <v>107</v>
       </c>
       <c r="D102">
-        <v>3.9571</v>
+        <v>3.9571000000000001</v>
       </c>
       <c r="E102">
-        <v>3.696</v>
+        <v>3.6960000000000002</v>
       </c>
       <c r="F102">
-        <v>3.4043</v>
+        <v>3.4043000000000001</v>
       </c>
       <c r="G102">
-        <v>3.6468</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7">
+        <v>3.6467999999999998</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>102</v>
       </c>
@@ -3077,16 +3096,16 @@
         <v>3.8929</v>
       </c>
       <c r="E103">
-        <v>3.8091</v>
+        <v>3.8090999999999999</v>
       </c>
       <c r="F103">
         <v>3.3043</v>
       </c>
       <c r="G103">
-        <v>3.6322</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7">
+        <v>3.6322000000000001</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>103</v>
       </c>
@@ -3100,7 +3119,7 @@
         <v>3.7643</v>
       </c>
       <c r="E104">
-        <v>3.4786</v>
+        <v>3.4786000000000001</v>
       </c>
       <c r="F104">
         <v>3.75</v>
@@ -3109,7 +3128,7 @@
         <v>3.6267</v>
       </c>
     </row>
-    <row r="105" spans="1:7">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>104</v>
       </c>
@@ -3120,10 +3139,10 @@
         <v>110</v>
       </c>
       <c r="D105">
-        <v>3.9357</v>
+        <v>3.9357000000000002</v>
       </c>
       <c r="E105">
-        <v>3.6947</v>
+        <v>3.6947000000000001</v>
       </c>
       <c r="F105">
         <v>3.3348</v>
@@ -3132,35 +3151,35 @@
         <v>3.6071</v>
       </c>
     </row>
-    <row r="106" spans="1:7">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>105</v>
       </c>
       <c r="B106">
-        <v>230395</v>
+        <v>230636</v>
       </c>
       <c r="C106" t="s">
         <v>111</v>
       </c>
       <c r="D106">
-        <v>3.85</v>
+        <v>3.8929</v>
       </c>
       <c r="E106">
-        <v>3.684</v>
+        <v>3.7364000000000002</v>
       </c>
       <c r="F106">
-        <v>3.3348</v>
+        <v>3.2783000000000002</v>
       </c>
       <c r="G106">
-        <v>3.5919</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7">
+        <v>3.5949</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>106</v>
       </c>
       <c r="B107">
-        <v>230259</v>
+        <v>230395</v>
       </c>
       <c r="C107" t="s">
         <v>112</v>
@@ -3169,62 +3188,62 @@
         <v>3.85</v>
       </c>
       <c r="E107">
-        <v>3.5679</v>
+        <v>3.6840000000000002</v>
       </c>
       <c r="F107">
-        <v>3.4476</v>
+        <v>3.3348</v>
       </c>
       <c r="G107">
-        <v>3.5905</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7">
+        <v>3.5918999999999999</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>107</v>
       </c>
       <c r="B108">
-        <v>230730</v>
+        <v>230259</v>
       </c>
       <c r="C108" t="s">
         <v>113</v>
       </c>
       <c r="D108">
-        <v>4</v>
+        <v>3.85</v>
       </c>
       <c r="E108">
-        <v>3.65</v>
+        <v>3.5678999999999998</v>
       </c>
       <c r="F108">
-        <v>3.1706</v>
+        <v>3.4476</v>
       </c>
       <c r="G108">
-        <v>3.5887</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7">
+        <v>3.5905</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>108</v>
       </c>
       <c r="B109">
-        <v>230636</v>
+        <v>230730</v>
       </c>
       <c r="C109" t="s">
         <v>114</v>
       </c>
       <c r="D109">
-        <v>3.8929</v>
+        <v>4</v>
       </c>
       <c r="E109">
-        <v>3.7364</v>
+        <v>3.65</v>
       </c>
       <c r="F109">
-        <v>3.2391</v>
+        <v>3.1705999999999999</v>
       </c>
       <c r="G109">
-        <v>3.5797</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7">
+        <v>3.5886999999999998</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>109</v>
       </c>
@@ -3238,16 +3257,16 @@
         <v>3.85</v>
       </c>
       <c r="E110">
-        <v>3.636</v>
+        <v>3.6360000000000001</v>
       </c>
       <c r="F110">
-        <v>3.3478</v>
+        <v>3.3477999999999999</v>
       </c>
       <c r="G110">
-        <v>3.5774</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7">
+        <v>3.5773999999999999</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>110</v>
       </c>
@@ -3264,13 +3283,13 @@
         <v>3.536</v>
       </c>
       <c r="F111">
-        <v>3.2529</v>
+        <v>3.2528999999999999</v>
       </c>
       <c r="G111">
         <v>3.5661</v>
       </c>
     </row>
-    <row r="112" spans="1:7">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>111</v>
       </c>
@@ -3284,16 +3303,16 @@
         <v>3.8714</v>
       </c>
       <c r="E112">
-        <v>3.5727</v>
+        <v>3.5727000000000002</v>
       </c>
       <c r="F112">
-        <v>3.2217</v>
+        <v>3.2216999999999998</v>
       </c>
       <c r="G112">
-        <v>3.5068</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7">
+        <v>3.5068000000000001</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>112</v>
       </c>
@@ -3313,10 +3332,10 @@
         <v>3.25</v>
       </c>
       <c r="G113">
-        <v>3.5018</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7">
+        <v>3.5017999999999998</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>113</v>
       </c>
@@ -3333,13 +3352,13 @@
         <v>3.528</v>
       </c>
       <c r="F114">
-        <v>3.2217</v>
+        <v>3.2216999999999998</v>
       </c>
       <c r="G114">
-        <v>3.4871</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7">
+        <v>3.4870999999999999</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>114</v>
       </c>
@@ -3356,13 +3375,13 @@
         <v>3.62</v>
       </c>
       <c r="F115">
-        <v>3.0957</v>
+        <v>3.0956999999999999</v>
       </c>
       <c r="G115">
-        <v>3.4774</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7">
+        <v>3.4773999999999998</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>115</v>
       </c>
@@ -3373,16 +3392,16 @@
         <v>121</v>
       </c>
       <c r="D116">
-        <v>3.8071</v>
+        <v>3.8071000000000002</v>
       </c>
       <c r="E116">
-        <v>3.3179</v>
+        <v>3.3178999999999998</v>
       </c>
       <c r="F116">
         <v>2.835</v>
       </c>
       <c r="G116">
-        <v>3.2726</v>
+        <v>3.2726000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pdf parsing error fix verified
</commit_message>
<xml_diff>
--- a/output/CGPA_Results.xlsx
+++ b/output/CGPA_Results.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\GitHub\CGPA-gen\output\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF6240E-0C7E-4E1C-A706-90D2F7AEA2A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="CGPA" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -67,12 +61,12 @@
     <t>PERERA G.M.B.</t>
   </si>
   <si>
+    <t>RATNAYAKE R.M.S.H.</t>
+  </si>
+  <si>
     <t>DHANANJAYA K.T.G.T.N.</t>
   </si>
   <si>
-    <t>RATNAYAKE R.M.S.H.</t>
-  </si>
-  <si>
     <t>WEERAKOON A.H.T.M.</t>
   </si>
   <si>
@@ -106,15 +100,15 @@
     <t>DE MEL D.J.</t>
   </si>
   <si>
+    <t>RAHUL B.</t>
+  </si>
+  <si>
     <t>DISSANAYAKA D.M.D.P.</t>
   </si>
   <si>
     <t>IMADUWAGE O.N.H.</t>
   </si>
   <si>
-    <t>RAHUL B.</t>
-  </si>
-  <si>
     <t>MALDENIYA P.A.D.G.R.</t>
   </si>
   <si>
@@ -127,12 +121,12 @@
     <t>PERERA U.I.H.</t>
   </si>
   <si>
+    <t>SAMARASINGHE S.M.R.R.</t>
+  </si>
+  <si>
     <t>PATHIRANA P.T.S.</t>
   </si>
   <si>
-    <t>SAMARASINGHE S.M.R.R.</t>
-  </si>
-  <si>
     <t>ARACHCHI A.D.I.D.</t>
   </si>
   <si>
@@ -157,12 +151,12 @@
     <t>WEDAMESTRIGE A.N.</t>
   </si>
   <si>
+    <t>CHANDRAKUMARA H.A.D.C.</t>
+  </si>
+  <si>
     <t>WIJESEKARA W.A.G.S.</t>
   </si>
   <si>
-    <t>CHANDRAKUMARA H.A.D.C.</t>
-  </si>
-  <si>
     <t>MUNASINGHE A.I.</t>
   </si>
   <si>
@@ -184,46 +178,49 @@
     <t>GUNASEKARA L.U.A.</t>
   </si>
   <si>
+    <t>PERERA H.A.J.I.</t>
+  </si>
+  <si>
+    <t>SHEHAN M.N.N.</t>
+  </si>
+  <si>
+    <t>WEERASINGHE J.A.H.R.</t>
+  </si>
+  <si>
+    <t>AROSHANA H.A.P.</t>
+  </si>
+  <si>
+    <t>AYANAJA N.B.G.M.</t>
+  </si>
+  <si>
+    <t>ANTHONY C.S.B.</t>
+  </si>
+  <si>
+    <t>RATHEESHAN A.R.</t>
+  </si>
+  <si>
+    <t>GUNASEKARA K.S.</t>
+  </si>
+  <si>
     <t>UPEKSHANI T.S.</t>
   </si>
   <si>
-    <t>PERERA H.A.J.I.</t>
-  </si>
-  <si>
-    <t>WEERASINGHE J.A.H.R.</t>
-  </si>
-  <si>
-    <t>SHEHAN M.N.N.</t>
-  </si>
-  <si>
-    <t>AROSHANA H.A.P.</t>
-  </si>
-  <si>
-    <t>AYANAJA N.B.G.M.</t>
-  </si>
-  <si>
-    <t>ANTHONY C.S.B.</t>
-  </si>
-  <si>
-    <t>GUNASEKARA K.S.</t>
-  </si>
-  <si>
-    <t>RATHEESHAN A.R.</t>
-  </si>
-  <si>
     <t>PITIWADUGE D.N.</t>
   </si>
   <si>
+    <t>PRISHMIKA H.W.N.</t>
+  </si>
+  <si>
     <t>FERNANDO H.M.D.</t>
   </si>
   <si>
+    <t>TENNAKOON U.G.R.B.</t>
+  </si>
+  <si>
     <t>GUNATHUNGA U.A.</t>
   </si>
   <si>
-    <t>PRISHMIKA H.W.N.</t>
-  </si>
-  <si>
-    <t>TENNAKOON U.G.R.B.</t>
+    <t>PRIYADARSHANA S.A.D.</t>
   </si>
   <si>
     <t>PEIRIS T.S.R.</t>
@@ -232,19 +229,22 @@
     <t>KUMARA P.K.M.P.</t>
   </si>
   <si>
-    <t>PRIYADARSHANA S.A.D.</t>
+    <t>RANATHUNGA R.J.K.O.H.</t>
+  </si>
+  <si>
+    <t>ATHUKORALA U.R.</t>
+  </si>
+  <si>
+    <t>DISSANAYAKE R.K.T.</t>
+  </si>
+  <si>
+    <t>SARUKA U.</t>
   </si>
   <si>
     <t>WIJESINGHE U.G.S.K.D.</t>
   </si>
   <si>
-    <t>RANATHUNGA R.J.K.O.H.</t>
-  </si>
-  <si>
-    <t>ATHUKORALA U.R.</t>
-  </si>
-  <si>
-    <t>DISSANAYAKE R.K.T.</t>
+    <t>RAHMAN M.F.A.</t>
   </si>
   <si>
     <t>BALASOORIYA B.R.B.D.</t>
@@ -256,12 +256,6 @@
     <t>JAYASINGHE J.A.P.R.</t>
   </si>
   <si>
-    <t>SARUKA U.</t>
-  </si>
-  <si>
-    <t>RAHMAN M.F.A.</t>
-  </si>
-  <si>
     <t>GAMAGE SK</t>
   </si>
   <si>
@@ -283,45 +277,45 @@
     <t>ADHIKARI A.H.C.S.</t>
   </si>
   <si>
+    <t>PERAMUNAGE D.S.</t>
+  </si>
+  <si>
     <t>WIJESINGHE W.A.P.W.</t>
   </si>
   <si>
-    <t>PERAMUNAGE D.S.</t>
-  </si>
-  <si>
     <t>ABEYWARDHANA T.C.W.</t>
   </si>
   <si>
     <t>DILHARA D.S.</t>
   </si>
   <si>
+    <t>BANDARA K.M.N.D.</t>
+  </si>
+  <si>
+    <t>NIRMANI W.T.</t>
+  </si>
+  <si>
+    <t>LENMINI B.L.W.</t>
+  </si>
+  <si>
+    <t>MEEDENIYA M.M.H.</t>
+  </si>
+  <si>
+    <t>RANAWAKA R.A.G.K.</t>
+  </si>
+  <si>
+    <t>INDUWARA M.L.A.S.</t>
+  </si>
+  <si>
+    <t>ABEYWARNA D.H.</t>
+  </si>
+  <si>
+    <t>PRABHARSHA H.W.D.</t>
+  </si>
+  <si>
     <t>RANASINGHE A.G.N.S.</t>
   </si>
   <si>
-    <t>BANDARA K.M.N.D.</t>
-  </si>
-  <si>
-    <t>PRABHARSHA H.W.D.</t>
-  </si>
-  <si>
-    <t>NIRMANI W.T.</t>
-  </si>
-  <si>
-    <t>LENMINI B.L.W.</t>
-  </si>
-  <si>
-    <t>MEEDENIYA M.M.H.</t>
-  </si>
-  <si>
-    <t>RANAWAKA R.A.G.K.</t>
-  </si>
-  <si>
-    <t>INDUWARA M.L.A.S.</t>
-  </si>
-  <si>
-    <t>ABEYWARNA D.H.</t>
-  </si>
-  <si>
     <t>PALIHENA H.H.</t>
   </si>
   <si>
@@ -331,25 +325,40 @@
     <t>HIMASARA W.V.M.J.</t>
   </si>
   <si>
+    <t>HANSINDU M.M.A.D.</t>
+  </si>
+  <si>
+    <t>UBEYSEKARA V.T.T.</t>
+  </si>
+  <si>
+    <t>GUNASEKARA H.M.</t>
+  </si>
+  <si>
     <t>SANTHOSH S.</t>
   </si>
   <si>
-    <t>HANSINDU M.M.A.D.</t>
-  </si>
-  <si>
-    <t>UBEYSEKARA V.T.T.</t>
-  </si>
-  <si>
-    <t>GUNASEKARA H.M.</t>
-  </si>
-  <si>
     <t>ERANGA W.A.O.</t>
   </si>
   <si>
+    <t>HENDENIYA H.M.J.C.</t>
+  </si>
+  <si>
     <t>SAMARANAYAKA H.D.J.D.</t>
   </si>
   <si>
-    <t>HENDENIYA H.M.J.C.</t>
+    <t>WIJETHILAKA J.S.</t>
+  </si>
+  <si>
+    <t>MANATUNGA K.D.</t>
+  </si>
+  <si>
+    <t>IMBULPITIYA B.N.</t>
+  </si>
+  <si>
+    <t>AMARASINGHE A.A.D.K.</t>
+  </si>
+  <si>
+    <t>FERNANDO LTJ</t>
   </si>
   <si>
     <t>PIYUMAL N.P.P.</t>
@@ -358,31 +367,16 @@
     <t>THARUSHIKA G.K.E.</t>
   </si>
   <si>
-    <t>MANATUNGA K.D.</t>
-  </si>
-  <si>
-    <t>IMBULPITIYA B.N.</t>
-  </si>
-  <si>
-    <t>WIJETHILAKA J.S.</t>
-  </si>
-  <si>
-    <t>AMARASINGHE A.A.D.K.</t>
-  </si>
-  <si>
-    <t>FERNANDO LTJ</t>
+    <t>GUNARATHNA K.T.M.B.</t>
+  </si>
+  <si>
+    <t>HAKAM M.R.A.</t>
+  </si>
+  <si>
+    <t>JAYAKODY J.A.C.P.</t>
   </si>
   <si>
     <t>SAMARASEKARA S.M.R.P.</t>
-  </si>
-  <si>
-    <t>GUNARATHNA K.T.M.B.</t>
-  </si>
-  <si>
-    <t>HAKAM M.R.A.</t>
-  </si>
-  <si>
-    <t>JAYAKODY J.A.C.P.</t>
   </si>
   <si>
     <t>NUWANAKA W.A.S.</t>
@@ -391,8 +385,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -429,21 +423,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -481,7 +467,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -515,7 +501,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -550,10 +535,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -726,17 +710,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -759,7 +740,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
@@ -782,7 +763,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2</v>
       </c>
@@ -805,7 +786,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
@@ -828,7 +809,7 @@
         <v>3.9903</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>4</v>
       </c>
@@ -845,13 +826,13 @@
         <v>4</v>
       </c>
       <c r="F5">
-        <v>3.9609000000000001</v>
+        <v>3.9609</v>
       </c>
       <c r="G5">
         <v>3.9855</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>5</v>
       </c>
@@ -868,13 +849,13 @@
         <v>4</v>
       </c>
       <c r="F6">
-        <v>3.9609000000000001</v>
+        <v>3.9609</v>
       </c>
       <c r="G6">
         <v>3.9855</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>6</v>
       </c>
@@ -891,13 +872,13 @@
         <v>4</v>
       </c>
       <c r="F7">
-        <v>3.9609000000000001</v>
+        <v>3.9609</v>
       </c>
       <c r="G7">
         <v>3.9855</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>7</v>
       </c>
@@ -920,7 +901,7 @@
         <v>3.9855</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>8</v>
       </c>
@@ -937,18 +918,18 @@
         <v>4</v>
       </c>
       <c r="F9">
-        <v>3.9609000000000001</v>
+        <v>3.9609</v>
       </c>
       <c r="G9">
         <v>3.9855</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>230138</v>
+        <v>230548</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
@@ -960,18 +941,18 @@
         <v>4</v>
       </c>
       <c r="F10">
-        <v>3.9571000000000001</v>
+        <v>3.9609</v>
       </c>
       <c r="G10">
-        <v>3.9849999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.9855</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>230548</v>
+        <v>230138</v>
       </c>
       <c r="C11" t="s">
         <v>16</v>
@@ -983,13 +964,13 @@
         <v>4</v>
       </c>
       <c r="F11">
-        <v>3.9609000000000001</v>
+        <v>3.9571</v>
       </c>
       <c r="G11">
-        <v>3.9847000000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.985</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1009,10 +990,10 @@
         <v>3.95</v>
       </c>
       <c r="G12">
-        <v>3.9832999999999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.9842</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1029,13 +1010,13 @@
         <v>4</v>
       </c>
       <c r="F13">
-        <v>3.9249999999999998</v>
+        <v>3.925</v>
       </c>
       <c r="G13">
         <v>3.9714</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1052,13 +1033,13 @@
         <v>4</v>
       </c>
       <c r="F14">
-        <v>3.9249999999999998</v>
+        <v>3.925</v>
       </c>
       <c r="G14">
         <v>3.9714</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1069,19 +1050,19 @@
         <v>20</v>
       </c>
       <c r="D15">
-        <v>3.9357000000000002</v>
+        <v>3.9357</v>
       </c>
       <c r="E15">
         <v>4</v>
       </c>
       <c r="F15">
-        <v>3.9550000000000001</v>
+        <v>3.955</v>
       </c>
       <c r="G15">
-        <v>3.9710000000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.971</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1092,19 +1073,19 @@
         <v>21</v>
       </c>
       <c r="D16">
-        <v>3.9357000000000002</v>
+        <v>3.9357</v>
       </c>
       <c r="E16">
         <v>4</v>
       </c>
       <c r="F16">
-        <v>3.9609000000000001</v>
+        <v>3.9609</v>
       </c>
       <c r="G16">
-        <v>3.9710000000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.971</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1124,10 +1105,10 @@
         <v>3.9217</v>
       </c>
       <c r="G17">
-        <v>3.9695</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.971</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1150,7 +1131,7 @@
         <v>3.9661</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1170,10 +1151,10 @@
         <v>3.9</v>
       </c>
       <c r="G19">
-        <v>3.9632000000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.965</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1193,10 +1174,10 @@
         <v>3.9</v>
       </c>
       <c r="G20">
-        <v>3.9628999999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.9629</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1219,7 +1200,7 @@
         <v>3.9619</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1230,7 +1211,7 @@
         <v>27</v>
       </c>
       <c r="D22">
-        <v>3.9571000000000001</v>
+        <v>3.9571</v>
       </c>
       <c r="E22">
         <v>4</v>
@@ -1242,12 +1223,12 @@
         <v>3.9613</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23">
-        <v>230155</v>
+        <v>230508</v>
       </c>
       <c r="C23" t="s">
         <v>28</v>
@@ -1256,62 +1237,62 @@
         <v>4</v>
       </c>
       <c r="E23">
-        <v>3.9279999999999999</v>
+        <v>4</v>
       </c>
       <c r="F23">
-        <v>3.9571000000000001</v>
+        <v>3.8826</v>
       </c>
       <c r="G23">
-        <v>3.9550000000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.9565</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
-        <v>230258</v>
+        <v>230155</v>
       </c>
       <c r="C24" t="s">
         <v>29</v>
       </c>
       <c r="D24">
-        <v>3.9357000000000002</v>
+        <v>4</v>
       </c>
       <c r="E24">
-        <v>3.964</v>
+        <v>3.928</v>
       </c>
       <c r="F24">
-        <v>3.9571000000000001</v>
+        <v>3.9571</v>
       </c>
       <c r="G24">
-        <v>3.9550000000000001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.955</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25">
-        <v>230508</v>
+        <v>230258</v>
       </c>
       <c r="C25" t="s">
         <v>30</v>
       </c>
       <c r="D25">
-        <v>4</v>
+        <v>3.9357</v>
       </c>
       <c r="E25">
-        <v>4</v>
+        <v>3.964</v>
       </c>
       <c r="F25">
-        <v>3.8826000000000001</v>
+        <v>3.9571</v>
       </c>
       <c r="G25">
-        <v>3.9542000000000002</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.955</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1328,13 +1309,13 @@
         <v>4</v>
       </c>
       <c r="F26">
-        <v>3.8738999999999999</v>
+        <v>3.8739</v>
       </c>
       <c r="G26">
-        <v>3.9531999999999998</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.9532</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1351,13 +1332,13 @@
         <v>4</v>
       </c>
       <c r="F27">
-        <v>3.8696000000000002</v>
+        <v>3.8696</v>
       </c>
       <c r="G27">
         <v>3.9516</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1371,16 +1352,16 @@
         <v>4</v>
       </c>
       <c r="E28">
-        <v>3.9571000000000001</v>
+        <v>3.9571</v>
       </c>
       <c r="F28">
         <v>3.895</v>
       </c>
       <c r="G28">
-        <v>3.9468000000000001</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.9468</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1397,59 +1378,59 @@
         <v>4</v>
       </c>
       <c r="F29">
-        <v>3.8614999999999999</v>
+        <v>3.8615</v>
       </c>
       <c r="G29">
-        <v>3.9445999999999999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.9446</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30">
-        <v>230468</v>
+        <v>230566</v>
       </c>
       <c r="C30" t="s">
         <v>35</v>
       </c>
       <c r="D30">
-        <v>3.9142999999999999</v>
+        <v>3.9571</v>
       </c>
       <c r="E30">
         <v>4</v>
       </c>
       <c r="F30">
-        <v>3.8957000000000002</v>
+        <v>3.8846</v>
       </c>
       <c r="G30">
-        <v>3.9419</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.9446</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31">
-        <v>230566</v>
+        <v>230468</v>
       </c>
       <c r="C31" t="s">
         <v>36</v>
       </c>
       <c r="D31">
-        <v>3.9571000000000001</v>
+        <v>3.9143</v>
       </c>
       <c r="E31">
         <v>4</v>
       </c>
       <c r="F31">
-        <v>3.8845999999999998</v>
+        <v>3.8957</v>
       </c>
       <c r="G31">
         <v>3.9419</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1472,7 +1453,7 @@
         <v>3.9371</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1486,7 +1467,7 @@
         <v>4</v>
       </c>
       <c r="E33">
-        <v>3.9279999999999999</v>
+        <v>3.928</v>
       </c>
       <c r="F33">
         <v>3.9</v>
@@ -1495,7 +1476,7 @@
         <v>3.9339</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1515,10 +1496,10 @@
         <v>3.79</v>
       </c>
       <c r="G34">
-        <v>3.9323000000000001</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.9323</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1529,19 +1510,19 @@
         <v>40</v>
       </c>
       <c r="D35">
-        <v>3.9357000000000002</v>
+        <v>3.9357</v>
       </c>
       <c r="E35">
         <v>3.964</v>
       </c>
       <c r="F35">
-        <v>3.8738999999999999</v>
+        <v>3.8739</v>
       </c>
       <c r="G35">
-        <v>3.9241999999999999</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.9242</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1558,13 +1539,13 @@
         <v>4</v>
       </c>
       <c r="F36">
-        <v>3.7913000000000001</v>
+        <v>3.7913</v>
       </c>
       <c r="G36">
-        <v>3.9186000000000001</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.9226</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1575,19 +1556,19 @@
         <v>42</v>
       </c>
       <c r="D37">
-        <v>3.9571000000000001</v>
+        <v>3.9571</v>
       </c>
       <c r="E37">
-        <v>3.9590999999999998</v>
+        <v>3.964</v>
       </c>
       <c r="F37">
-        <v>3.8477999999999999</v>
+        <v>3.8478</v>
       </c>
       <c r="G37">
-        <v>3.9152999999999998</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.9194</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1601,16 +1582,16 @@
         <v>4</v>
       </c>
       <c r="E38">
-        <v>3.9159999999999999</v>
+        <v>3.916</v>
       </c>
       <c r="F38">
-        <v>3.8624999999999998</v>
+        <v>3.8625</v>
       </c>
       <c r="G38">
-        <v>3.9142999999999999</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.9143</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1624,21 +1605,21 @@
         <v>4</v>
       </c>
       <c r="E39">
-        <v>3.9318</v>
+        <v>3.94</v>
       </c>
       <c r="F39">
         <v>3.8304</v>
       </c>
       <c r="G39">
-        <v>3.9085000000000001</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.9129</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40">
-        <v>230724</v>
+        <v>230100</v>
       </c>
       <c r="C40" t="s">
         <v>45</v>
@@ -1647,21 +1628,21 @@
         <v>4</v>
       </c>
       <c r="E40">
-        <v>3.9045000000000001</v>
+        <v>4</v>
       </c>
       <c r="F40">
-        <v>3.8477999999999999</v>
+        <v>3.7217</v>
       </c>
       <c r="G40">
-        <v>3.9051</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.8968</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41">
-        <v>230100</v>
+        <v>230724</v>
       </c>
       <c r="C41" t="s">
         <v>46</v>
@@ -1670,16 +1651,16 @@
         <v>4</v>
       </c>
       <c r="E41">
-        <v>4</v>
+        <v>3.88</v>
       </c>
       <c r="F41">
-        <v>3.7216999999999998</v>
+        <v>3.8478</v>
       </c>
       <c r="G41">
-        <v>3.8967999999999998</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.8952</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1693,7 +1674,7 @@
         <v>4</v>
       </c>
       <c r="E42">
-        <v>3.9159999999999999</v>
+        <v>3.916</v>
       </c>
       <c r="F42">
         <v>3.8043</v>
@@ -1702,7 +1683,7 @@
         <v>3.8935</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1725,7 +1706,7 @@
         <v>3.8855</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1742,13 +1723,13 @@
         <v>3.964</v>
       </c>
       <c r="F44">
-        <v>3.7143000000000002</v>
+        <v>3.7143</v>
       </c>
       <c r="G44">
-        <v>3.8849999999999998</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.885</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1765,13 +1746,13 @@
         <v>3.952</v>
       </c>
       <c r="F45">
-        <v>3.7303999999999999</v>
+        <v>3.7304</v>
       </c>
       <c r="G45">
-        <v>3.8805999999999998</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.8806</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1782,19 +1763,19 @@
         <v>51</v>
       </c>
       <c r="D46">
-        <v>3.9357000000000002</v>
+        <v>3.9357</v>
       </c>
       <c r="E46">
         <v>4</v>
       </c>
       <c r="F46">
-        <v>3.7130000000000001</v>
+        <v>3.713</v>
       </c>
       <c r="G46">
         <v>3.879</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1805,19 +1786,19 @@
         <v>52</v>
       </c>
       <c r="D47">
-        <v>3.9357000000000002</v>
+        <v>3.9357</v>
       </c>
       <c r="E47">
         <v>4</v>
       </c>
       <c r="F47">
-        <v>3.7042999999999999</v>
+        <v>3.7043</v>
       </c>
       <c r="G47">
-        <v>3.8757999999999999</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.8758</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1828,65 +1809,65 @@
         <v>53</v>
       </c>
       <c r="D48">
-        <v>3.9571000000000001</v>
+        <v>3.9571</v>
       </c>
       <c r="E48">
         <v>3.88</v>
       </c>
       <c r="F48">
-        <v>3.8216999999999999</v>
+        <v>3.8217</v>
       </c>
       <c r="G48">
-        <v>3.8757999999999999</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.8758</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49">
-        <v>230659</v>
+        <v>230477</v>
       </c>
       <c r="C49" t="s">
         <v>54</v>
       </c>
       <c r="D49">
-        <v>3.8571</v>
+        <v>3.9357</v>
       </c>
       <c r="E49">
-        <v>3.9590999999999998</v>
+        <v>3.832</v>
       </c>
       <c r="F49">
-        <v>3.8043</v>
+        <v>3.8739</v>
       </c>
       <c r="G49">
-        <v>3.8746</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.871</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50">
-        <v>230477</v>
+        <v>230613</v>
       </c>
       <c r="C50" t="s">
         <v>55</v>
       </c>
       <c r="D50">
-        <v>3.9357000000000002</v>
+        <v>4</v>
       </c>
       <c r="E50">
-        <v>3.8319999999999999</v>
+        <v>3.952</v>
       </c>
       <c r="F50">
-        <v>3.8738999999999999</v>
+        <v>3.7</v>
       </c>
       <c r="G50">
-        <v>3.871</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.8694</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1897,24 +1878,24 @@
         <v>56</v>
       </c>
       <c r="D51">
-        <v>3.9571000000000001</v>
+        <v>3.9571</v>
       </c>
       <c r="E51">
-        <v>4</v>
+        <v>3.964</v>
       </c>
       <c r="F51">
-        <v>3.6714000000000002</v>
+        <v>3.6714</v>
       </c>
       <c r="G51">
-        <v>3.8683999999999998</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.86</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52">
-        <v>230613</v>
+        <v>230058</v>
       </c>
       <c r="C52" t="s">
         <v>57</v>
@@ -1923,85 +1904,85 @@
         <v>4</v>
       </c>
       <c r="E52">
-        <v>3.9455</v>
+        <v>3.916</v>
       </c>
       <c r="F52">
-        <v>3.7</v>
+        <v>3.713</v>
       </c>
       <c r="G52">
-        <v>3.8626999999999998</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.8597</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53">
-        <v>230058</v>
+        <v>230065</v>
       </c>
       <c r="C53" t="s">
         <v>58</v>
       </c>
       <c r="D53">
-        <v>4</v>
+        <v>3.8929</v>
       </c>
       <c r="E53">
-        <v>3.9159999999999999</v>
+        <v>3.844</v>
       </c>
       <c r="F53">
-        <v>3.7130000000000001</v>
+        <v>3.85</v>
       </c>
       <c r="G53">
-        <v>3.8597000000000001</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.8576</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54">
-        <v>230065</v>
+        <v>230045</v>
       </c>
       <c r="C54" t="s">
         <v>59</v>
       </c>
       <c r="D54">
-        <v>3.8929</v>
+        <v>4</v>
       </c>
       <c r="E54">
-        <v>3.8439999999999999</v>
+        <v>3.916</v>
       </c>
       <c r="F54">
-        <v>3.85</v>
+        <v>3.7043</v>
       </c>
       <c r="G54">
-        <v>3.8576000000000001</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.8565</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55">
-        <v>230045</v>
+        <v>230539</v>
       </c>
       <c r="C55" t="s">
         <v>60</v>
       </c>
       <c r="D55">
-        <v>4</v>
+        <v>3.9357</v>
       </c>
       <c r="E55">
-        <v>3.9159999999999999</v>
+        <v>4</v>
       </c>
       <c r="F55">
-        <v>3.7042999999999999</v>
+        <v>3.6522</v>
       </c>
       <c r="G55">
         <v>3.8565</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2015,39 +1996,39 @@
         <v>4</v>
       </c>
       <c r="E56">
-        <v>3.8919999999999999</v>
+        <v>3.892</v>
       </c>
       <c r="F56">
-        <v>3.7216999999999998</v>
+        <v>3.7217</v>
       </c>
       <c r="G56">
-        <v>3.8532000000000002</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.8532</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57">
-        <v>230539</v>
+        <v>230659</v>
       </c>
       <c r="C57" t="s">
         <v>62</v>
       </c>
       <c r="D57">
-        <v>3.9357000000000002</v>
+        <v>3.8571</v>
       </c>
       <c r="E57">
-        <v>4</v>
+        <v>3.88</v>
       </c>
       <c r="F57">
-        <v>3.6522000000000001</v>
+        <v>3.8043</v>
       </c>
       <c r="G57">
-        <v>3.8492000000000002</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.8468</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2058,116 +2039,116 @@
         <v>63</v>
       </c>
       <c r="D58">
-        <v>3.9357000000000002</v>
+        <v>3.9357</v>
       </c>
       <c r="E58">
-        <v>3.9159999999999999</v>
+        <v>3.916</v>
       </c>
       <c r="F58">
-        <v>3.6905000000000001</v>
+        <v>3.6905</v>
       </c>
       <c r="G58">
-        <v>3.8416999999999999</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.8417</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59">
-        <v>230180</v>
+        <v>230500</v>
       </c>
       <c r="C59" t="s">
         <v>64</v>
       </c>
       <c r="D59">
-        <v>3.9357000000000002</v>
+        <v>3.9571</v>
       </c>
       <c r="E59">
-        <v>3.8319999999999999</v>
+        <v>3.916</v>
       </c>
       <c r="F59">
-        <v>3.7783000000000002</v>
+        <v>3.6783</v>
       </c>
       <c r="G59">
-        <v>3.8355000000000001</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.8371</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60">
-        <v>230218</v>
+        <v>230180</v>
       </c>
       <c r="C60" t="s">
         <v>65</v>
       </c>
       <c r="D60">
-        <v>3.9357000000000002</v>
+        <v>3.9357</v>
       </c>
       <c r="E60">
-        <v>3.8178999999999998</v>
+        <v>3.832</v>
       </c>
       <c r="F60">
-        <v>3.78</v>
+        <v>3.7783</v>
       </c>
       <c r="G60">
-        <v>3.8323</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.8355</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61">
-        <v>230500</v>
+        <v>230629</v>
       </c>
       <c r="C61" t="s">
         <v>66</v>
       </c>
       <c r="D61">
-        <v>3.9571000000000001</v>
+        <v>3.9571</v>
       </c>
       <c r="E61">
-        <v>3.9045000000000001</v>
+        <v>3.916</v>
       </c>
       <c r="F61">
-        <v>3.6783000000000001</v>
+        <v>3.6739</v>
       </c>
       <c r="G61">
-        <v>3.8288000000000002</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.8355</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62">
-        <v>230629</v>
+        <v>230218</v>
       </c>
       <c r="C62" t="s">
         <v>67</v>
       </c>
       <c r="D62">
-        <v>3.9571000000000001</v>
+        <v>3.9357</v>
       </c>
       <c r="E62">
-        <v>3.9045000000000001</v>
+        <v>3.8179</v>
       </c>
       <c r="F62">
-        <v>3.6739000000000002</v>
+        <v>3.78</v>
       </c>
       <c r="G62">
-        <v>3.8271000000000002</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.8323</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63">
-        <v>230470</v>
+        <v>230502</v>
       </c>
       <c r="C63" t="s">
         <v>68</v>
@@ -2176,90 +2157,90 @@
         <v>4</v>
       </c>
       <c r="E63">
-        <v>4</v>
+        <v>3.952</v>
       </c>
       <c r="F63">
-        <v>3.5261</v>
+        <v>3.587</v>
       </c>
       <c r="G63">
-        <v>3.8241999999999998</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.8274</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64">
-        <v>230353</v>
+        <v>230470</v>
       </c>
       <c r="C64" t="s">
         <v>69</v>
       </c>
       <c r="D64">
-        <v>3.9</v>
+        <v>4</v>
       </c>
       <c r="E64">
-        <v>3.964</v>
+        <v>4</v>
       </c>
       <c r="F64">
-        <v>3.613</v>
+        <v>3.5261</v>
       </c>
       <c r="G64">
-        <v>3.8193999999999999</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.8242</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65">
-        <v>230502</v>
+        <v>230353</v>
       </c>
       <c r="C65" t="s">
         <v>70</v>
       </c>
       <c r="D65">
-        <v>4</v>
+        <v>3.9</v>
       </c>
       <c r="E65">
-        <v>3.9455</v>
+        <v>3.964</v>
       </c>
       <c r="F65">
-        <v>3.5870000000000002</v>
+        <v>3.613</v>
       </c>
       <c r="G65">
-        <v>3.8186</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.8194</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66">
-        <v>230726</v>
+        <v>230525</v>
       </c>
       <c r="C66" t="s">
         <v>71</v>
       </c>
       <c r="D66">
-        <v>3.8929</v>
+        <v>4</v>
       </c>
       <c r="E66">
-        <v>3.9045000000000001</v>
+        <v>4</v>
       </c>
       <c r="F66">
-        <v>3.6608999999999998</v>
+        <v>3.5</v>
       </c>
       <c r="G66">
-        <v>3.8068</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.8145</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67">
-        <v>230525</v>
+        <v>230063</v>
       </c>
       <c r="C67" t="s">
         <v>72</v>
@@ -2268,177 +2249,177 @@
         <v>4</v>
       </c>
       <c r="E67">
-        <v>4</v>
+        <v>3.916</v>
       </c>
       <c r="F67">
-        <v>3.5</v>
+        <v>3.5609</v>
       </c>
       <c r="G67">
-        <v>3.8050999999999999</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.8032</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68">
-        <v>230063</v>
+        <v>230164</v>
       </c>
       <c r="C68" t="s">
         <v>73</v>
       </c>
       <c r="D68">
-        <v>4</v>
+        <v>3.9571</v>
       </c>
       <c r="E68">
-        <v>3.9159999999999999</v>
+        <v>3.88</v>
       </c>
       <c r="F68">
-        <v>3.5609000000000002</v>
+        <v>3.6261</v>
       </c>
       <c r="G68">
-        <v>3.8031999999999999</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.8032</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69">
-        <v>230164</v>
+        <v>230585</v>
       </c>
       <c r="C69" t="s">
         <v>74</v>
       </c>
       <c r="D69">
-        <v>3.9571000000000001</v>
+        <v>3.9357</v>
       </c>
       <c r="E69">
-        <v>3.88</v>
+        <v>3.964</v>
       </c>
       <c r="F69">
-        <v>3.6261000000000001</v>
+        <v>3.5435</v>
       </c>
       <c r="G69">
-        <v>3.8031999999999999</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.8016</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70">
-        <v>230070</v>
+        <v>230726</v>
       </c>
       <c r="C70" t="s">
         <v>75</v>
       </c>
       <c r="D70">
-        <v>3.9571000000000001</v>
+        <v>3.8929</v>
       </c>
       <c r="E70">
-        <v>3.8239999999999998</v>
+        <v>3.88</v>
       </c>
       <c r="F70">
-        <v>3.6652</v>
+        <v>3.6609</v>
       </c>
       <c r="G70">
-        <v>3.7951999999999999</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.8016</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71">
-        <v>230016</v>
+        <v>230507</v>
       </c>
       <c r="C71" t="s">
         <v>76</v>
       </c>
       <c r="D71">
-        <v>4</v>
+        <v>3.8571</v>
       </c>
       <c r="E71">
-        <v>3.9142999999999999</v>
+        <v>3.8821</v>
       </c>
       <c r="F71">
-        <v>3.48</v>
+        <v>3.645</v>
       </c>
       <c r="G71">
-        <v>3.7934999999999999</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="B72">
-        <v>230280</v>
+        <v>230070</v>
       </c>
       <c r="C72" t="s">
         <v>77</v>
       </c>
       <c r="D72">
-        <v>3.85</v>
+        <v>3.9571</v>
       </c>
       <c r="E72">
-        <v>3.9159999999999999</v>
+        <v>3.824</v>
       </c>
       <c r="F72">
-        <v>3.6</v>
+        <v>3.6652</v>
       </c>
       <c r="G72">
-        <v>3.7932000000000001</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.7952</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73">
-        <v>230585</v>
+        <v>230016</v>
       </c>
       <c r="C73" t="s">
         <v>78</v>
       </c>
       <c r="D73">
-        <v>3.9357000000000002</v>
+        <v>4</v>
       </c>
       <c r="E73">
-        <v>3.9590999999999998</v>
+        <v>3.9143</v>
       </c>
       <c r="F73">
-        <v>3.5434999999999999</v>
+        <v>3.48</v>
       </c>
       <c r="G73">
-        <v>3.7915000000000001</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.7935</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
       <c r="A74">
         <v>73</v>
       </c>
       <c r="B74">
-        <v>230507</v>
+        <v>230280</v>
       </c>
       <c r="C74" t="s">
         <v>79</v>
       </c>
       <c r="D74">
-        <v>3.8571</v>
+        <v>3.85</v>
       </c>
       <c r="E74">
-        <v>3.8679999999999999</v>
+        <v>3.916</v>
       </c>
       <c r="F74">
-        <v>3.645</v>
+        <v>3.6</v>
       </c>
       <c r="G74">
-        <v>3.7898000000000001</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.7932</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2449,19 +2430,19 @@
         <v>80</v>
       </c>
       <c r="D75">
-        <v>3.9571000000000001</v>
+        <v>3.9571</v>
       </c>
       <c r="E75">
-        <v>3.7959999999999998</v>
+        <v>3.796</v>
       </c>
       <c r="F75">
-        <v>3.6783000000000001</v>
+        <v>3.6783</v>
       </c>
       <c r="G75">
         <v>3.7887</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2472,19 +2453,19 @@
         <v>81</v>
       </c>
       <c r="D76">
-        <v>3.9357000000000002</v>
+        <v>3.9357</v>
       </c>
       <c r="E76">
-        <v>3.9455</v>
+        <v>3.952</v>
       </c>
       <c r="F76">
-        <v>3.4956999999999998</v>
+        <v>3.4957</v>
       </c>
       <c r="G76">
-        <v>3.7677999999999998</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.779</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2495,19 +2476,19 @@
         <v>82</v>
       </c>
       <c r="D77">
-        <v>3.9357000000000002</v>
+        <v>3.9357</v>
       </c>
       <c r="E77">
-        <v>3.8317999999999999</v>
+        <v>3.852</v>
       </c>
       <c r="F77">
-        <v>3.5912999999999999</v>
+        <v>3.5913</v>
       </c>
       <c r="G77">
-        <v>3.7627000000000002</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.7742</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2521,16 +2502,16 @@
         <v>4</v>
       </c>
       <c r="E78">
-        <v>3.8679999999999999</v>
+        <v>3.868</v>
       </c>
       <c r="F78">
-        <v>3.4550000000000001</v>
+        <v>3.455</v>
       </c>
       <c r="G78">
-        <v>3.7593000000000001</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.7593</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2553,7 +2534,7 @@
         <v>3.7565</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2567,16 +2548,16 @@
         <v>3.85</v>
       </c>
       <c r="E80">
-        <v>3.6840000000000002</v>
+        <v>3.684</v>
       </c>
       <c r="F80">
-        <v>3.7652000000000001</v>
+        <v>3.7652</v>
       </c>
       <c r="G80">
-        <v>3.7515999999999998</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.7516</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2599,53 +2580,53 @@
         <v>3.746</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7">
       <c r="A82">
         <v>81</v>
       </c>
       <c r="B82">
-        <v>230727</v>
+        <v>230473</v>
       </c>
       <c r="C82" t="s">
         <v>87</v>
       </c>
       <c r="D82">
-        <v>3.7856999999999998</v>
+        <v>3.8929</v>
       </c>
       <c r="E82">
-        <v>3.8679999999999999</v>
+        <v>3.916</v>
       </c>
       <c r="F82">
-        <v>3.54</v>
+        <v>3.4435</v>
       </c>
       <c r="G82">
-        <v>3.7372999999999998</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.7355</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
       <c r="A83">
         <v>82</v>
       </c>
       <c r="B83">
-        <v>230473</v>
+        <v>230727</v>
       </c>
       <c r="C83" t="s">
         <v>88</v>
       </c>
       <c r="D83">
-        <v>3.8929</v>
+        <v>3.7857</v>
       </c>
       <c r="E83">
-        <v>3.9159999999999999</v>
+        <v>3.85</v>
       </c>
       <c r="F83">
-        <v>3.4434999999999998</v>
+        <v>3.54</v>
       </c>
       <c r="G83">
         <v>3.7355</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2656,10 +2637,10 @@
         <v>89</v>
       </c>
       <c r="D84">
-        <v>3.9142999999999999</v>
+        <v>3.9143</v>
       </c>
       <c r="E84">
-        <v>3.7959999999999998</v>
+        <v>3.796</v>
       </c>
       <c r="F84">
         <v>3.5583</v>
@@ -2668,7 +2649,7 @@
         <v>3.7317</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2682,67 +2663,67 @@
         <v>3.8929</v>
       </c>
       <c r="E85">
-        <v>3.8319999999999999</v>
+        <v>3.832</v>
       </c>
       <c r="F85">
-        <v>3.5087000000000002</v>
+        <v>3.5087</v>
       </c>
       <c r="G85">
         <v>3.7258</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7">
       <c r="A86">
         <v>85</v>
       </c>
       <c r="B86">
-        <v>230520</v>
+        <v>230077</v>
       </c>
       <c r="C86" t="s">
         <v>91</v>
       </c>
       <c r="D86">
-        <v>3.85</v>
+        <v>3.7857</v>
       </c>
       <c r="E86">
-        <v>3.85</v>
+        <v>3.7536</v>
       </c>
       <c r="F86">
-        <v>3.4950000000000001</v>
+        <v>3.619</v>
       </c>
       <c r="G86">
-        <v>3.7231999999999998</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.7159</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
       <c r="A87">
         <v>86</v>
       </c>
       <c r="B87">
-        <v>230077</v>
+        <v>230444</v>
       </c>
       <c r="C87" t="s">
         <v>92</v>
       </c>
       <c r="D87">
-        <v>3.7856999999999998</v>
+        <v>3.7857</v>
       </c>
       <c r="E87">
-        <v>3.7536</v>
+        <v>3.625</v>
       </c>
       <c r="F87">
-        <v>3.6190000000000002</v>
+        <v>3.7571</v>
       </c>
       <c r="G87">
-        <v>3.7159</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.7048</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
       <c r="A88">
         <v>87</v>
       </c>
       <c r="B88">
-        <v>230495</v>
+        <v>230375</v>
       </c>
       <c r="C88" t="s">
         <v>93</v>
@@ -2751,67 +2732,67 @@
         <v>3.85</v>
       </c>
       <c r="E88">
-        <v>3.9182000000000001</v>
+        <v>3.712</v>
       </c>
       <c r="F88">
-        <v>3.4174000000000002</v>
+        <v>3.6</v>
       </c>
       <c r="G88">
-        <v>3.7067999999999999</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.7016</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
       <c r="A89">
         <v>88</v>
       </c>
       <c r="B89">
-        <v>230444</v>
+        <v>230407</v>
       </c>
       <c r="C89" t="s">
         <v>94</v>
       </c>
       <c r="D89">
-        <v>3.7856999999999998</v>
+        <v>4</v>
       </c>
       <c r="E89">
-        <v>3.625</v>
+        <v>3.748</v>
       </c>
       <c r="F89">
-        <v>3.7570999999999999</v>
+        <v>3.4696</v>
       </c>
       <c r="G89">
-        <v>3.7048000000000001</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.7016</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
       <c r="A90">
         <v>89</v>
       </c>
       <c r="B90">
-        <v>230375</v>
+        <v>230527</v>
       </c>
       <c r="C90" t="s">
         <v>95</v>
       </c>
       <c r="D90">
-        <v>3.85</v>
+        <v>4</v>
       </c>
       <c r="E90">
-        <v>3.7120000000000002</v>
+        <v>3.844</v>
       </c>
       <c r="F90">
-        <v>3.6</v>
+        <v>3.3391</v>
       </c>
       <c r="G90">
-        <v>3.7016</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.6919</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
       <c r="A91">
         <v>90</v>
       </c>
       <c r="B91">
-        <v>230407</v>
+        <v>230261</v>
       </c>
       <c r="C91" t="s">
         <v>96</v>
@@ -2820,67 +2801,67 @@
         <v>4</v>
       </c>
       <c r="E91">
-        <v>3.7480000000000002</v>
+        <v>3.768</v>
       </c>
       <c r="F91">
-        <v>3.4695999999999998</v>
+        <v>3.425</v>
       </c>
       <c r="G91">
-        <v>3.7016</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.6889</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
       <c r="A92">
         <v>91</v>
       </c>
       <c r="B92">
-        <v>230527</v>
+        <v>230013</v>
       </c>
       <c r="C92" t="s">
         <v>97</v>
       </c>
       <c r="D92">
-        <v>4</v>
+        <v>3.85</v>
       </c>
       <c r="E92">
-        <v>3.8635999999999999</v>
+        <v>3.648</v>
       </c>
       <c r="F92">
-        <v>3.3391000000000002</v>
+        <v>3.6385</v>
       </c>
       <c r="G92">
-        <v>3.6915</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.6877</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
       <c r="A93">
         <v>92</v>
       </c>
       <c r="B93">
-        <v>230261</v>
+        <v>230495</v>
       </c>
       <c r="C93" t="s">
         <v>98</v>
       </c>
       <c r="D93">
-        <v>4</v>
+        <v>3.85</v>
       </c>
       <c r="E93">
-        <v>3.7679999999999998</v>
+        <v>3.844</v>
       </c>
       <c r="F93">
-        <v>3.4249999999999998</v>
+        <v>3.4174</v>
       </c>
       <c r="G93">
-        <v>3.6888999999999998</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.6871</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
       <c r="A94">
         <v>93</v>
       </c>
       <c r="B94">
-        <v>230013</v>
+        <v>230520</v>
       </c>
       <c r="C94" t="s">
         <v>99</v>
@@ -2889,16 +2870,16 @@
         <v>3.85</v>
       </c>
       <c r="E94">
-        <v>3.6480000000000001</v>
+        <v>3.748</v>
       </c>
       <c r="F94">
-        <v>3.6385000000000001</v>
+        <v>3.495</v>
       </c>
       <c r="G94">
-        <v>3.6877</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.6864</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
       <c r="A95">
         <v>94</v>
       </c>
@@ -2909,19 +2890,19 @@
         <v>100</v>
       </c>
       <c r="D95">
-        <v>3.9571000000000001</v>
+        <v>3.9571</v>
       </c>
       <c r="E95">
-        <v>3.7360000000000002</v>
+        <v>3.736</v>
       </c>
       <c r="F95">
-        <v>3.4651999999999998</v>
+        <v>3.4652</v>
       </c>
       <c r="G95">
-        <v>3.6855000000000002</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.6855</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
       <c r="A96">
         <v>95</v>
       </c>
@@ -2932,19 +2913,19 @@
         <v>101</v>
       </c>
       <c r="D96">
-        <v>3.9357000000000002</v>
+        <v>3.9357</v>
       </c>
       <c r="E96">
-        <v>3.8182</v>
+        <v>3.804</v>
       </c>
       <c r="F96">
         <v>3.4</v>
       </c>
       <c r="G96">
-        <v>3.6831</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.6839</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
       <c r="A97">
         <v>96</v>
       </c>
@@ -2955,70 +2936,70 @@
         <v>102</v>
       </c>
       <c r="D97">
-        <v>3.9357000000000002</v>
+        <v>3.9357</v>
       </c>
       <c r="E97">
-        <v>3.6640000000000001</v>
+        <v>3.664</v>
       </c>
       <c r="F97">
-        <v>3.5434999999999999</v>
+        <v>3.5435</v>
       </c>
       <c r="G97">
-        <v>3.6806000000000001</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.6806</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
       <c r="A98">
         <v>97</v>
       </c>
       <c r="B98">
-        <v>230581</v>
+        <v>230229</v>
       </c>
       <c r="C98" t="s">
         <v>103</v>
       </c>
       <c r="D98">
-        <v>3.7928999999999999</v>
+        <v>3.85</v>
       </c>
       <c r="E98">
-        <v>3.6840000000000002</v>
+        <v>3.784</v>
       </c>
       <c r="F98">
-        <v>3.5470999999999999</v>
+        <v>3.4</v>
       </c>
       <c r="G98">
-        <v>3.6696</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.665</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
       <c r="A99">
         <v>98</v>
       </c>
       <c r="B99">
-        <v>230229</v>
+        <v>230650</v>
       </c>
       <c r="C99" t="s">
         <v>104</v>
       </c>
       <c r="D99">
-        <v>3.85</v>
+        <v>4</v>
       </c>
       <c r="E99">
-        <v>3.7839999999999998</v>
+        <v>3.732</v>
       </c>
       <c r="F99">
-        <v>3.4</v>
+        <v>3.3739</v>
       </c>
       <c r="G99">
-        <v>3.665</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.6597</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
       <c r="A100">
         <v>99</v>
       </c>
       <c r="B100">
-        <v>230650</v>
+        <v>230208</v>
       </c>
       <c r="C100" t="s">
         <v>105</v>
@@ -3027,39 +3008,39 @@
         <v>4</v>
       </c>
       <c r="E100">
-        <v>3.7364000000000002</v>
+        <v>3.636</v>
       </c>
       <c r="F100">
-        <v>3.3738999999999999</v>
+        <v>3.4609</v>
       </c>
       <c r="G100">
-        <v>3.6576</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.6532</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7">
       <c r="A101">
         <v>100</v>
       </c>
       <c r="B101">
-        <v>230208</v>
+        <v>230581</v>
       </c>
       <c r="C101" t="s">
         <v>106</v>
       </c>
       <c r="D101">
-        <v>4</v>
+        <v>3.7929</v>
       </c>
       <c r="E101">
-        <v>3.6360000000000001</v>
+        <v>3.6429</v>
       </c>
       <c r="F101">
-        <v>3.4609000000000001</v>
+        <v>3.5471</v>
       </c>
       <c r="G101">
-        <v>3.6532</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.6508</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7">
       <c r="A102">
         <v>101</v>
       </c>
@@ -3070,116 +3051,116 @@
         <v>107</v>
       </c>
       <c r="D102">
-        <v>3.9571000000000001</v>
+        <v>3.9571</v>
       </c>
       <c r="E102">
-        <v>3.6960000000000002</v>
+        <v>3.696</v>
       </c>
       <c r="F102">
-        <v>3.4043000000000001</v>
+        <v>3.4043</v>
       </c>
       <c r="G102">
-        <v>3.6467999999999998</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.6468</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7">
       <c r="A103">
         <v>102</v>
       </c>
       <c r="B103">
-        <v>230563</v>
+        <v>230238</v>
       </c>
       <c r="C103" t="s">
         <v>108</v>
       </c>
       <c r="D103">
-        <v>3.8929</v>
+        <v>3.7643</v>
       </c>
       <c r="E103">
-        <v>3.8090999999999999</v>
+        <v>3.4786</v>
       </c>
       <c r="F103">
-        <v>3.3043</v>
+        <v>3.75</v>
       </c>
       <c r="G103">
-        <v>3.6322000000000001</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.6267</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7">
       <c r="A104">
         <v>103</v>
       </c>
       <c r="B104">
-        <v>230238</v>
+        <v>230563</v>
       </c>
       <c r="C104" t="s">
         <v>109</v>
       </c>
       <c r="D104">
-        <v>3.7643</v>
+        <v>3.8929</v>
       </c>
       <c r="E104">
-        <v>3.4786000000000001</v>
+        <v>3.748</v>
       </c>
       <c r="F104">
-        <v>3.75</v>
+        <v>3.3043</v>
       </c>
       <c r="G104">
-        <v>3.6267</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.6161</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7">
       <c r="A105">
         <v>104</v>
       </c>
       <c r="B105">
-        <v>230493</v>
+        <v>230730</v>
       </c>
       <c r="C105" t="s">
         <v>110</v>
       </c>
       <c r="D105">
-        <v>3.9357000000000002</v>
+        <v>4</v>
       </c>
       <c r="E105">
-        <v>3.6947000000000001</v>
+        <v>3.656</v>
       </c>
       <c r="F105">
-        <v>3.3348</v>
+        <v>3.1706</v>
       </c>
       <c r="G105">
-        <v>3.6071</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.5946</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7">
       <c r="A106">
         <v>105</v>
       </c>
       <c r="B106">
-        <v>230636</v>
+        <v>230395</v>
       </c>
       <c r="C106" t="s">
         <v>111</v>
       </c>
       <c r="D106">
-        <v>3.8929</v>
+        <v>3.85</v>
       </c>
       <c r="E106">
-        <v>3.7364000000000002</v>
+        <v>3.684</v>
       </c>
       <c r="F106">
-        <v>3.2783000000000002</v>
+        <v>3.3348</v>
       </c>
       <c r="G106">
-        <v>3.5949</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.5919</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7">
       <c r="A107">
         <v>106</v>
       </c>
       <c r="B107">
-        <v>230395</v>
+        <v>230259</v>
       </c>
       <c r="C107" t="s">
         <v>112</v>
@@ -3188,21 +3169,21 @@
         <v>3.85</v>
       </c>
       <c r="E107">
-        <v>3.6840000000000002</v>
+        <v>3.5679</v>
       </c>
       <c r="F107">
-        <v>3.3348</v>
+        <v>3.4476</v>
       </c>
       <c r="G107">
-        <v>3.5918999999999999</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.5905</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7">
       <c r="A108">
         <v>107</v>
       </c>
       <c r="B108">
-        <v>230259</v>
+        <v>230033</v>
       </c>
       <c r="C108" t="s">
         <v>113</v>
@@ -3211,21 +3192,21 @@
         <v>3.85</v>
       </c>
       <c r="E108">
-        <v>3.5678999999999998</v>
+        <v>3.636</v>
       </c>
       <c r="F108">
-        <v>3.4476</v>
+        <v>3.3478</v>
       </c>
       <c r="G108">
-        <v>3.5905</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.5774</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7">
       <c r="A109">
         <v>108</v>
       </c>
       <c r="B109">
-        <v>230730</v>
+        <v>230183</v>
       </c>
       <c r="C109" t="s">
         <v>114</v>
@@ -3234,90 +3215,90 @@
         <v>4</v>
       </c>
       <c r="E109">
-        <v>3.65</v>
+        <v>3.536</v>
       </c>
       <c r="F109">
-        <v>3.1705999999999999</v>
+        <v>3.2529</v>
       </c>
       <c r="G109">
-        <v>3.5886999999999998</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.5661</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7">
       <c r="A110">
         <v>109</v>
       </c>
       <c r="B110">
-        <v>230033</v>
+        <v>230493</v>
       </c>
       <c r="C110" t="s">
         <v>115</v>
       </c>
       <c r="D110">
-        <v>3.85</v>
+        <v>3.9357</v>
       </c>
       <c r="E110">
-        <v>3.6360000000000001</v>
+        <v>3.5591</v>
       </c>
       <c r="F110">
-        <v>3.3477999999999999</v>
+        <v>3.3348</v>
       </c>
       <c r="G110">
-        <v>3.5773999999999999</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.561</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
       <c r="A111">
         <v>110</v>
       </c>
       <c r="B111">
-        <v>230183</v>
+        <v>230636</v>
       </c>
       <c r="C111" t="s">
         <v>116</v>
       </c>
       <c r="D111">
-        <v>4</v>
+        <v>3.8929</v>
       </c>
       <c r="E111">
-        <v>3.536</v>
+        <v>3.612</v>
       </c>
       <c r="F111">
-        <v>3.2528999999999999</v>
+        <v>3.2783</v>
       </c>
       <c r="G111">
-        <v>3.5661</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.5516</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7">
       <c r="A112">
         <v>111</v>
       </c>
       <c r="B112">
-        <v>230564</v>
+        <v>230203</v>
       </c>
       <c r="C112" t="s">
         <v>117</v>
       </c>
       <c r="D112">
-        <v>3.8714</v>
+        <v>3.85</v>
       </c>
       <c r="E112">
-        <v>3.5727000000000002</v>
+        <v>3.488</v>
       </c>
       <c r="F112">
-        <v>3.2216999999999998</v>
+        <v>3.25</v>
       </c>
       <c r="G112">
-        <v>3.5068000000000001</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.5018</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7">
       <c r="A113">
         <v>112</v>
       </c>
       <c r="B113">
-        <v>230203</v>
+        <v>230224</v>
       </c>
       <c r="C113" t="s">
         <v>118</v>
@@ -3326,21 +3307,21 @@
         <v>3.85</v>
       </c>
       <c r="E113">
-        <v>3.488</v>
+        <v>3.528</v>
       </c>
       <c r="F113">
-        <v>3.25</v>
+        <v>3.2217</v>
       </c>
       <c r="G113">
-        <v>3.5017999999999998</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.4871</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7">
       <c r="A114">
         <v>113</v>
       </c>
       <c r="B114">
-        <v>230224</v>
+        <v>230268</v>
       </c>
       <c r="C114" t="s">
         <v>119</v>
@@ -3349,39 +3330,39 @@
         <v>3.85</v>
       </c>
       <c r="E114">
-        <v>3.528</v>
+        <v>3.62</v>
       </c>
       <c r="F114">
-        <v>3.2216999999999998</v>
+        <v>3.0957</v>
       </c>
       <c r="G114">
-        <v>3.4870999999999999</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.4774</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7">
       <c r="A115">
         <v>114</v>
       </c>
       <c r="B115">
-        <v>230268</v>
+        <v>230564</v>
       </c>
       <c r="C115" t="s">
         <v>120</v>
       </c>
       <c r="D115">
-        <v>3.85</v>
+        <v>3.8714</v>
       </c>
       <c r="E115">
-        <v>3.62</v>
+        <v>3.468</v>
       </c>
       <c r="F115">
-        <v>3.0956999999999999</v>
+        <v>3.2217</v>
       </c>
       <c r="G115">
-        <v>3.4773999999999998</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.4677</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7">
       <c r="A116">
         <v>115</v>
       </c>
@@ -3392,16 +3373,16 @@
         <v>121</v>
       </c>
       <c r="D116">
-        <v>3.8071000000000002</v>
+        <v>3.8071</v>
       </c>
       <c r="E116">
-        <v>3.3178999999999998</v>
+        <v>3.3179</v>
       </c>
       <c r="F116">
         <v>2.835</v>
       </c>
       <c r="G116">
-        <v>3.2726000000000002</v>
+        <v>3.2726</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I-we credit value adjusted to 0
</commit_message>
<xml_diff>
--- a/output/CGPA_Results.xlsx
+++ b/output/CGPA_Results.xlsx
@@ -55,6 +55,9 @@
     <t>BANDARA W.D.A.C.</t>
   </si>
   <si>
+    <t>DHANANJAYA K.T.G.T.N.</t>
+  </si>
+  <si>
     <t>NETTIKUMARA N.A.H.G.</t>
   </si>
   <si>
@@ -64,322 +67,319 @@
     <t>RATNAYAKE R.M.S.H.</t>
   </si>
   <si>
-    <t>DHANANJAYA K.T.G.T.N.</t>
+    <t>ILANKOON I.M.M.K.B.</t>
+  </si>
+  <si>
+    <t>KARIYAWASAM J.H.D.</t>
+  </si>
+  <si>
+    <t>COLOMBAGE D.M.</t>
+  </si>
+  <si>
+    <t>KUMARA K.B.R.</t>
+  </si>
+  <si>
+    <t>RATHNAYAKE M.A.G.K.N.</t>
+  </si>
+  <si>
+    <t>PERERA K.W.A.O.V.</t>
+  </si>
+  <si>
+    <t>WANIGASUNDARA W.M.H.</t>
+  </si>
+  <si>
+    <t>KUMARASINGHE M.N.</t>
+  </si>
+  <si>
+    <t>DE MEL D.J.</t>
+  </si>
+  <si>
+    <t>PEIRIS E.A.S.S.</t>
+  </si>
+  <si>
+    <t>RAHUL B.</t>
+  </si>
+  <si>
+    <t>DISSANAYAKA D.M.D.P.</t>
+  </si>
+  <si>
+    <t>IMADUWAGE O.N.H.</t>
+  </si>
+  <si>
+    <t>MALDENIYA P.A.D.G.R.</t>
+  </si>
+  <si>
+    <t>FERNANDO W.H.D.</t>
+  </si>
+  <si>
+    <t>DISSANAYAKE G.R.G.K.</t>
+  </si>
+  <si>
+    <t>PERERA U.I.H.</t>
+  </si>
+  <si>
+    <t>SAMARASINGHE S.M.R.R.</t>
+  </si>
+  <si>
+    <t>PATHIRANA P.T.S.</t>
+  </si>
+  <si>
+    <t>ARACHCHI A.D.I.D.</t>
+  </si>
+  <si>
+    <t>GARUSINGHE S.B.</t>
+  </si>
+  <si>
+    <t>KEERAWELLA K.P.C.P.</t>
+  </si>
+  <si>
+    <t>DHARMAKEERTHI P.K.G.C.L.</t>
+  </si>
+  <si>
+    <t>RANASINGHE D.P.H.</t>
+  </si>
+  <si>
+    <t>RASANJANA W.P.G.R.A.</t>
+  </si>
+  <si>
+    <t>KARUNARATHNA G.K.T.</t>
+  </si>
+  <si>
+    <t>WEDAMESTRIGE A.N.</t>
+  </si>
+  <si>
+    <t>CHANDRAKUMARA H.A.D.C.</t>
+  </si>
+  <si>
+    <t>WIJESEKARA W.A.G.S.</t>
+  </si>
+  <si>
+    <t>MUNASINGHE A.I.</t>
+  </si>
+  <si>
+    <t>AMARATHUNGE A.M.N.L.</t>
+  </si>
+  <si>
+    <t>DESHAN W.U.</t>
+  </si>
+  <si>
+    <t>KARUNANAYAKE A.H.D.</t>
+  </si>
+  <si>
+    <t>JAYAWEERA N.S.</t>
+  </si>
+  <si>
+    <t>DILHAN W.A.</t>
+  </si>
+  <si>
+    <t>GUNASEKARA L.U.A.</t>
+  </si>
+  <si>
+    <t>PERERA H.A.J.I.</t>
+  </si>
+  <si>
+    <t>SHEHAN M.N.N.</t>
+  </si>
+  <si>
+    <t>WEERASINGHE J.A.H.R.</t>
+  </si>
+  <si>
+    <t>AROSHANA H.A.P.</t>
+  </si>
+  <si>
+    <t>ANTHONY C.S.B.</t>
+  </si>
+  <si>
+    <t>RATHEESHAN A.R.</t>
+  </si>
+  <si>
+    <t>GUNASEKARA K.S.</t>
+  </si>
+  <si>
+    <t>UPEKSHANI T.S.</t>
+  </si>
+  <si>
+    <t>PITIWADUGE D.N.</t>
+  </si>
+  <si>
+    <t>PRISHMIKA H.W.N.</t>
+  </si>
+  <si>
+    <t>FERNANDO H.M.D.</t>
+  </si>
+  <si>
+    <t>TENNAKOON U.G.R.B.</t>
+  </si>
+  <si>
+    <t>GUNATHUNGA U.A.</t>
+  </si>
+  <si>
+    <t>PRIYADARSHANA S.A.D.</t>
+  </si>
+  <si>
+    <t>PEIRIS T.S.R.</t>
+  </si>
+  <si>
+    <t>KUMARA P.K.M.P.</t>
+  </si>
+  <si>
+    <t>RANATHUNGA R.J.K.O.H.</t>
+  </si>
+  <si>
+    <t>ATHUKORALA U.R.</t>
+  </si>
+  <si>
+    <t>DISSANAYAKE R.K.T.</t>
+  </si>
+  <si>
+    <t>SARUKA U.</t>
+  </si>
+  <si>
+    <t>WIJESINGHE U.G.S.K.D.</t>
+  </si>
+  <si>
+    <t>RAHMAN M.F.A.</t>
+  </si>
+  <si>
+    <t>BALASOORIYA B.R.B.D.</t>
+  </si>
+  <si>
+    <t>ABISHEK L.</t>
+  </si>
+  <si>
+    <t>GAMAGE SK</t>
   </si>
   <si>
     <t>WEERAKOON A.H.T.M.</t>
   </si>
   <si>
-    <t>ILANKOON I.M.M.K.B.</t>
-  </si>
-  <si>
-    <t>KARIYAWASAM J.H.D.</t>
-  </si>
-  <si>
-    <t>COLOMBAGE D.M.</t>
-  </si>
-  <si>
-    <t>KUMARA K.B.R.</t>
-  </si>
-  <si>
-    <t>RATHNAYAKE M.A.G.K.N.</t>
-  </si>
-  <si>
-    <t>PERERA K.W.A.O.V.</t>
-  </si>
-  <si>
-    <t>WANIGASUNDARA W.M.H.</t>
-  </si>
-  <si>
-    <t>KUMARASINGHE M.N.</t>
-  </si>
-  <si>
-    <t>PEIRIS E.A.S.S.</t>
-  </si>
-  <si>
-    <t>DE MEL D.J.</t>
-  </si>
-  <si>
-    <t>RAHUL B.</t>
-  </si>
-  <si>
-    <t>DISSANAYAKA D.M.D.P.</t>
-  </si>
-  <si>
-    <t>IMADUWAGE O.N.H.</t>
-  </si>
-  <si>
-    <t>MALDENIYA P.A.D.G.R.</t>
-  </si>
-  <si>
-    <t>FERNANDO W.H.D.</t>
-  </si>
-  <si>
-    <t>DISSANAYAKE G.R.G.K.</t>
-  </si>
-  <si>
-    <t>PERERA U.I.H.</t>
-  </si>
-  <si>
-    <t>SAMARASINGHE S.M.R.R.</t>
-  </si>
-  <si>
-    <t>PATHIRANA P.T.S.</t>
-  </si>
-  <si>
-    <t>ARACHCHI A.D.I.D.</t>
-  </si>
-  <si>
-    <t>GARUSINGHE S.B.</t>
-  </si>
-  <si>
-    <t>KEERAWELLA K.P.C.P.</t>
-  </si>
-  <si>
-    <t>DHARMAKEERTHI P.K.G.C.L.</t>
-  </si>
-  <si>
-    <t>RANASINGHE D.P.H.</t>
-  </si>
-  <si>
-    <t>RASANJANA W.P.G.R.A.</t>
-  </si>
-  <si>
-    <t>KARUNARATHNA G.K.T.</t>
-  </si>
-  <si>
-    <t>WEDAMESTRIGE A.N.</t>
-  </si>
-  <si>
-    <t>CHANDRAKUMARA H.A.D.C.</t>
-  </si>
-  <si>
-    <t>WIJESEKARA W.A.G.S.</t>
-  </si>
-  <si>
-    <t>MUNASINGHE A.I.</t>
-  </si>
-  <si>
-    <t>AMARATHUNGE A.M.N.L.</t>
-  </si>
-  <si>
-    <t>DESHAN W.U.</t>
-  </si>
-  <si>
-    <t>KARUNANAYAKE A.H.D.</t>
-  </si>
-  <si>
-    <t>JAYAWEERA N.S.</t>
-  </si>
-  <si>
-    <t>DILHAN W.A.</t>
-  </si>
-  <si>
-    <t>GUNASEKARA L.U.A.</t>
-  </si>
-  <si>
-    <t>PERERA H.A.J.I.</t>
-  </si>
-  <si>
-    <t>SHEHAN M.N.N.</t>
-  </si>
-  <si>
-    <t>WEERASINGHE J.A.H.R.</t>
-  </si>
-  <si>
-    <t>AROSHANA H.A.P.</t>
+    <t>RANAWAKA R.A.C.D.</t>
+  </si>
+  <si>
+    <t>UMAIR A.</t>
+  </si>
+  <si>
+    <t>ARACHCHIGE M. A. D. T. S.</t>
+  </si>
+  <si>
+    <t>WIJESINGHE W.A.P.W.</t>
+  </si>
+  <si>
+    <t>KAUSHALYA R.G.S.P.</t>
+  </si>
+  <si>
+    <t>ADHIKARI A.H.C.S.</t>
+  </si>
+  <si>
+    <t>PERAMUNAGE D.S.</t>
+  </si>
+  <si>
+    <t>ABEYWARDHANA T.C.W.</t>
+  </si>
+  <si>
+    <t>DILHARA D.S.</t>
+  </si>
+  <si>
+    <t>BANDARA K.M.N.D.</t>
+  </si>
+  <si>
+    <t>NIRMANI W.T.</t>
+  </si>
+  <si>
+    <t>LENMINI B.L.W.</t>
+  </si>
+  <si>
+    <t>MEEDENIYA M.M.H.</t>
+  </si>
+  <si>
+    <t>RANAWAKA R.A.G.K.</t>
+  </si>
+  <si>
+    <t>INDUWARA M.L.A.S.</t>
+  </si>
+  <si>
+    <t>ABEYWARNA D.H.</t>
+  </si>
+  <si>
+    <t>PRABHARSHA H.W.D.</t>
+  </si>
+  <si>
+    <t>PALIHENA H.H.</t>
+  </si>
+  <si>
+    <t>WITHANAGE G.D.N.</t>
+  </si>
+  <si>
+    <t>HIMASARA W.V.M.J.</t>
   </si>
   <si>
     <t>AYANAJA N.B.G.M.</t>
   </si>
   <si>
-    <t>ANTHONY C.S.B.</t>
-  </si>
-  <si>
-    <t>RATHEESHAN A.R.</t>
-  </si>
-  <si>
-    <t>GUNASEKARA K.S.</t>
-  </si>
-  <si>
-    <t>UPEKSHANI T.S.</t>
-  </si>
-  <si>
-    <t>PITIWADUGE D.N.</t>
-  </si>
-  <si>
-    <t>PRISHMIKA H.W.N.</t>
-  </si>
-  <si>
-    <t>FERNANDO H.M.D.</t>
-  </si>
-  <si>
-    <t>TENNAKOON U.G.R.B.</t>
-  </si>
-  <si>
-    <t>GUNATHUNGA U.A.</t>
-  </si>
-  <si>
-    <t>PRIYADARSHANA S.A.D.</t>
-  </si>
-  <si>
-    <t>PEIRIS T.S.R.</t>
-  </si>
-  <si>
-    <t>KUMARA P.K.M.P.</t>
-  </si>
-  <si>
-    <t>RANATHUNGA R.J.K.O.H.</t>
-  </si>
-  <si>
-    <t>ATHUKORALA U.R.</t>
-  </si>
-  <si>
-    <t>DISSANAYAKE R.K.T.</t>
-  </si>
-  <si>
-    <t>SARUKA U.</t>
-  </si>
-  <si>
-    <t>WIJESINGHE U.G.S.K.D.</t>
-  </si>
-  <si>
-    <t>RAHMAN M.F.A.</t>
-  </si>
-  <si>
-    <t>BALASOORIYA B.R.B.D.</t>
-  </si>
-  <si>
-    <t>ABISHEK L.</t>
+    <t>HANSINDU M.M.A.D.</t>
+  </si>
+  <si>
+    <t>UBEYSEKARA V.T.T.</t>
+  </si>
+  <si>
+    <t>GUNASEKARA H.M.</t>
+  </si>
+  <si>
+    <t>ERANGA W.A.O.</t>
+  </si>
+  <si>
+    <t>SAMARANAYAKA H.D.J.D.</t>
   </si>
   <si>
     <t>JAYASINGHE J.A.P.R.</t>
   </si>
   <si>
-    <t>GAMAGE SK</t>
-  </si>
-  <si>
-    <t>RANAWAKA R.A.C.D.</t>
-  </si>
-  <si>
-    <t>UMAIR A.</t>
+    <t>MANATUNGA K.D.</t>
+  </si>
+  <si>
+    <t>IMBULPITIYA B.N.</t>
   </si>
   <si>
     <t>AHAMED A.M.S.</t>
   </si>
   <si>
-    <t>ARACHCHIGE M. A. D. T. S.</t>
-  </si>
-  <si>
-    <t>KAUSHALYA R.G.S.P.</t>
-  </si>
-  <si>
-    <t>ADHIKARI A.H.C.S.</t>
-  </si>
-  <si>
-    <t>PERAMUNAGE D.S.</t>
-  </si>
-  <si>
-    <t>WIJESINGHE W.A.P.W.</t>
-  </si>
-  <si>
-    <t>ABEYWARDHANA T.C.W.</t>
-  </si>
-  <si>
-    <t>DILHARA D.S.</t>
-  </si>
-  <si>
-    <t>BANDARA K.M.N.D.</t>
-  </si>
-  <si>
-    <t>NIRMANI W.T.</t>
-  </si>
-  <si>
-    <t>LENMINI B.L.W.</t>
-  </si>
-  <si>
-    <t>MEEDENIYA M.M.H.</t>
-  </si>
-  <si>
-    <t>RANAWAKA R.A.G.K.</t>
-  </si>
-  <si>
-    <t>INDUWARA M.L.A.S.</t>
-  </si>
-  <si>
-    <t>ABEYWARNA D.H.</t>
-  </si>
-  <si>
-    <t>PRABHARSHA H.W.D.</t>
+    <t>AMARASINGHE A.A.D.K.</t>
+  </si>
+  <si>
+    <t>THARUSHIKA G.K.E.</t>
   </si>
   <si>
     <t>RANASINGHE A.G.N.S.</t>
   </si>
   <si>
-    <t>PALIHENA H.H.</t>
-  </si>
-  <si>
-    <t>WITHANAGE G.D.N.</t>
-  </si>
-  <si>
-    <t>HIMASARA W.V.M.J.</t>
-  </si>
-  <si>
-    <t>HANSINDU M.M.A.D.</t>
-  </si>
-  <si>
-    <t>UBEYSEKARA V.T.T.</t>
-  </si>
-  <si>
-    <t>GUNASEKARA H.M.</t>
+    <t>HAKAM M.R.A.</t>
+  </si>
+  <si>
+    <t>JAYAKODY J.A.C.P.</t>
   </si>
   <si>
     <t>SANTHOSH S.</t>
   </si>
   <si>
-    <t>ERANGA W.A.O.</t>
+    <t>SAMARASEKARA S.M.R.P.</t>
   </si>
   <si>
     <t>HENDENIYA H.M.J.C.</t>
   </si>
   <si>
-    <t>SAMARANAYAKA H.D.J.D.</t>
+    <t>PIYUMAL N.P.P.</t>
+  </si>
+  <si>
+    <t>GUNARATHNA K.T.M.B.</t>
+  </si>
+  <si>
+    <t>NUWANAKA W.A.S.</t>
   </si>
   <si>
     <t>WIJETHILAKA J.S.</t>
   </si>
   <si>
-    <t>MANATUNGA K.D.</t>
-  </si>
-  <si>
-    <t>IMBULPITIYA B.N.</t>
-  </si>
-  <si>
-    <t>AMARASINGHE A.A.D.K.</t>
-  </si>
-  <si>
     <t>FERNANDO LTJ</t>
-  </si>
-  <si>
-    <t>PIYUMAL N.P.P.</t>
-  </si>
-  <si>
-    <t>THARUSHIKA G.K.E.</t>
-  </si>
-  <si>
-    <t>GUNARATHNA K.T.M.B.</t>
-  </si>
-  <si>
-    <t>HAKAM M.R.A.</t>
-  </si>
-  <si>
-    <t>JAYAKODY J.A.C.P.</t>
-  </si>
-  <si>
-    <t>SAMARASEKARA S.M.R.P.</t>
-  </si>
-  <si>
-    <t>NUWANAKA W.A.S.</t>
   </si>
 </sst>
 </file>
@@ -803,10 +803,10 @@
         <v>4</v>
       </c>
       <c r="F4">
-        <v>3.9739</v>
+        <v>3.973</v>
       </c>
       <c r="G4">
-        <v>3.9903</v>
+        <v>3.99</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -826,10 +826,10 @@
         <v>4</v>
       </c>
       <c r="F5">
-        <v>3.9609</v>
+        <v>3.96</v>
       </c>
       <c r="G5">
-        <v>3.9855</v>
+        <v>3.985</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -849,10 +849,10 @@
         <v>4</v>
       </c>
       <c r="F6">
-        <v>3.9609</v>
+        <v>3.96</v>
       </c>
       <c r="G6">
-        <v>3.9855</v>
+        <v>3.985</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -872,10 +872,10 @@
         <v>4</v>
       </c>
       <c r="F7">
-        <v>3.9609</v>
+        <v>3.96</v>
       </c>
       <c r="G7">
-        <v>3.9855</v>
+        <v>3.985</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -883,7 +883,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>230436</v>
+        <v>230138</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
@@ -892,13 +892,13 @@
         <v>4</v>
       </c>
       <c r="E8">
-        <v>3.964</v>
+        <v>4</v>
       </c>
       <c r="F8">
-        <v>4</v>
+        <v>3.957</v>
       </c>
       <c r="G8">
-        <v>3.9855</v>
+        <v>3.985</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -906,7 +906,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>230476</v>
+        <v>230436</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
@@ -915,13 +915,13 @@
         <v>4</v>
       </c>
       <c r="E9">
-        <v>4</v>
+        <v>3.964</v>
       </c>
       <c r="F9">
-        <v>3.9609</v>
+        <v>4</v>
       </c>
       <c r="G9">
-        <v>3.9855</v>
+        <v>3.985</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -929,7 +929,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>230548</v>
+        <v>230476</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
@@ -941,10 +941,10 @@
         <v>4</v>
       </c>
       <c r="F10">
-        <v>3.9609</v>
+        <v>3.96</v>
       </c>
       <c r="G10">
-        <v>3.9855</v>
+        <v>3.985</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -952,7 +952,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>230138</v>
+        <v>230548</v>
       </c>
       <c r="C11" t="s">
         <v>16</v>
@@ -964,7 +964,7 @@
         <v>4</v>
       </c>
       <c r="F11">
-        <v>3.9571</v>
+        <v>3.96</v>
       </c>
       <c r="G11">
         <v>3.985</v>
@@ -975,7 +975,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>230689</v>
+        <v>230256</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
@@ -987,10 +987,10 @@
         <v>4</v>
       </c>
       <c r="F12">
-        <v>3.95</v>
+        <v>3.925</v>
       </c>
       <c r="G12">
-        <v>3.9842</v>
+        <v>3.971</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -998,7 +998,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>230256</v>
+        <v>230318</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
@@ -1010,10 +1010,10 @@
         <v>4</v>
       </c>
       <c r="F13">
-        <v>3.925</v>
+        <v>3.924</v>
       </c>
       <c r="G13">
-        <v>3.9714</v>
+        <v>3.971</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1021,22 +1021,22 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>230318</v>
+        <v>230108</v>
       </c>
       <c r="C14" t="s">
         <v>19</v>
       </c>
       <c r="D14">
-        <v>4</v>
+        <v>3.935</v>
       </c>
       <c r="E14">
         <v>4</v>
       </c>
       <c r="F14">
-        <v>3.925</v>
+        <v>3.954</v>
       </c>
       <c r="G14">
-        <v>3.9714</v>
+        <v>3.97</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1044,22 +1044,22 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>230108</v>
+        <v>230352</v>
       </c>
       <c r="C15" t="s">
         <v>20</v>
       </c>
       <c r="D15">
-        <v>3.9357</v>
+        <v>3.935</v>
       </c>
       <c r="E15">
         <v>4</v>
       </c>
       <c r="F15">
-        <v>3.955</v>
+        <v>3.96</v>
       </c>
       <c r="G15">
-        <v>3.971</v>
+        <v>3.97</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1067,22 +1067,22 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>230352</v>
+        <v>230544</v>
       </c>
       <c r="C16" t="s">
         <v>21</v>
       </c>
       <c r="D16">
-        <v>3.9357</v>
+        <v>4</v>
       </c>
       <c r="E16">
         <v>4</v>
       </c>
       <c r="F16">
-        <v>3.9609</v>
+        <v>3.921</v>
       </c>
       <c r="G16">
-        <v>3.971</v>
+        <v>3.97</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1090,22 +1090,22 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>230544</v>
+        <v>230481</v>
       </c>
       <c r="C17" t="s">
         <v>22</v>
       </c>
       <c r="D17">
-        <v>4</v>
+        <v>3.85</v>
       </c>
       <c r="E17">
         <v>4</v>
       </c>
       <c r="F17">
-        <v>3.9217</v>
+        <v>4</v>
       </c>
       <c r="G17">
-        <v>3.971</v>
+        <v>3.966</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1113,22 +1113,22 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>230481</v>
+        <v>230680</v>
       </c>
       <c r="C18" t="s">
         <v>23</v>
       </c>
       <c r="D18">
-        <v>3.85</v>
+        <v>4</v>
       </c>
       <c r="E18">
         <v>4</v>
       </c>
       <c r="F18">
-        <v>4</v>
+        <v>3.9</v>
       </c>
       <c r="G18">
-        <v>3.9661</v>
+        <v>3.965</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1136,7 +1136,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>230680</v>
+        <v>230355</v>
       </c>
       <c r="C19" t="s">
         <v>24</v>
@@ -1151,7 +1151,7 @@
         <v>3.9</v>
       </c>
       <c r="G19">
-        <v>3.965</v>
+        <v>3.962</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1159,22 +1159,22 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>230355</v>
+        <v>230121</v>
       </c>
       <c r="C20" t="s">
         <v>25</v>
       </c>
       <c r="D20">
-        <v>4</v>
+        <v>3.957</v>
       </c>
       <c r="E20">
         <v>4</v>
       </c>
       <c r="F20">
-        <v>3.9</v>
+        <v>3.921</v>
       </c>
       <c r="G20">
-        <v>3.9629</v>
+        <v>3.961</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1194,10 +1194,10 @@
         <v>3.964</v>
       </c>
       <c r="F21">
-        <v>3.9375</v>
+        <v>3.937</v>
       </c>
       <c r="G21">
-        <v>3.9619</v>
+        <v>3.961</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1205,22 +1205,22 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>230121</v>
+        <v>230508</v>
       </c>
       <c r="C22" t="s">
         <v>27</v>
       </c>
       <c r="D22">
-        <v>3.9571</v>
+        <v>4</v>
       </c>
       <c r="E22">
         <v>4</v>
       </c>
       <c r="F22">
-        <v>3.9217</v>
+        <v>3.882</v>
       </c>
       <c r="G22">
-        <v>3.9613</v>
+        <v>3.956</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1228,7 +1228,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>230508</v>
+        <v>230155</v>
       </c>
       <c r="C23" t="s">
         <v>28</v>
@@ -1237,13 +1237,13 @@
         <v>4</v>
       </c>
       <c r="E23">
-        <v>4</v>
+        <v>3.927</v>
       </c>
       <c r="F23">
-        <v>3.8826</v>
+        <v>3.957</v>
       </c>
       <c r="G23">
-        <v>3.9565</v>
+        <v>3.954</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1251,22 +1251,22 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>230155</v>
+        <v>230258</v>
       </c>
       <c r="C24" t="s">
         <v>29</v>
       </c>
       <c r="D24">
-        <v>4</v>
+        <v>3.935</v>
       </c>
       <c r="E24">
-        <v>3.928</v>
+        <v>3.964</v>
       </c>
       <c r="F24">
-        <v>3.9571</v>
+        <v>3.957</v>
       </c>
       <c r="G24">
-        <v>3.955</v>
+        <v>3.954</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1274,22 +1274,22 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>230258</v>
+        <v>230390</v>
       </c>
       <c r="C25" t="s">
         <v>30</v>
       </c>
       <c r="D25">
-        <v>3.9357</v>
+        <v>4</v>
       </c>
       <c r="E25">
-        <v>3.964</v>
+        <v>4</v>
       </c>
       <c r="F25">
-        <v>3.9571</v>
+        <v>3.873</v>
       </c>
       <c r="G25">
-        <v>3.955</v>
+        <v>3.953</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1297,7 +1297,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>230390</v>
+        <v>230186</v>
       </c>
       <c r="C26" t="s">
         <v>31</v>
@@ -1309,10 +1309,10 @@
         <v>4</v>
       </c>
       <c r="F26">
-        <v>3.8739</v>
+        <v>3.869</v>
       </c>
       <c r="G26">
-        <v>3.9532</v>
+        <v>3.951</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1320,7 +1320,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>230186</v>
+        <v>230159</v>
       </c>
       <c r="C27" t="s">
         <v>32</v>
@@ -1329,13 +1329,13 @@
         <v>4</v>
       </c>
       <c r="E27">
-        <v>4</v>
+        <v>3.957</v>
       </c>
       <c r="F27">
-        <v>3.8696</v>
+        <v>3.895</v>
       </c>
       <c r="G27">
-        <v>3.9516</v>
+        <v>3.946</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1343,7 +1343,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>230159</v>
+        <v>230486</v>
       </c>
       <c r="C28" t="s">
         <v>33</v>
@@ -1352,13 +1352,13 @@
         <v>4</v>
       </c>
       <c r="E28">
-        <v>3.9571</v>
+        <v>4</v>
       </c>
       <c r="F28">
-        <v>3.895</v>
+        <v>3.861</v>
       </c>
       <c r="G28">
-        <v>3.9468</v>
+        <v>3.944</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1366,22 +1366,22 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>230486</v>
+        <v>230566</v>
       </c>
       <c r="C29" t="s">
         <v>34</v>
       </c>
       <c r="D29">
-        <v>4</v>
+        <v>3.957</v>
       </c>
       <c r="E29">
         <v>4</v>
       </c>
       <c r="F29">
-        <v>3.8615</v>
+        <v>3.884</v>
       </c>
       <c r="G29">
-        <v>3.9446</v>
+        <v>3.944</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1389,22 +1389,22 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>230566</v>
+        <v>230468</v>
       </c>
       <c r="C30" t="s">
         <v>35</v>
       </c>
       <c r="D30">
-        <v>3.9571</v>
+        <v>3.914</v>
       </c>
       <c r="E30">
         <v>4</v>
       </c>
       <c r="F30">
-        <v>3.8846</v>
+        <v>3.895</v>
       </c>
       <c r="G30">
-        <v>3.9446</v>
+        <v>3.941</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1412,22 +1412,22 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>230468</v>
+        <v>230051</v>
       </c>
       <c r="C31" t="s">
         <v>36</v>
       </c>
       <c r="D31">
-        <v>3.9143</v>
+        <v>4</v>
       </c>
       <c r="E31">
         <v>4</v>
       </c>
       <c r="F31">
-        <v>3.8957</v>
+        <v>3.83</v>
       </c>
       <c r="G31">
-        <v>3.9419</v>
+        <v>3.937</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1435,7 +1435,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>230051</v>
+        <v>230197</v>
       </c>
       <c r="C32" t="s">
         <v>37</v>
@@ -1444,13 +1444,13 @@
         <v>4</v>
       </c>
       <c r="E32">
-        <v>4</v>
+        <v>3.928</v>
       </c>
       <c r="F32">
-        <v>3.8304</v>
+        <v>3.899</v>
       </c>
       <c r="G32">
-        <v>3.9371</v>
+        <v>3.933</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1458,7 +1458,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>230197</v>
+        <v>230332</v>
       </c>
       <c r="C33" t="s">
         <v>38</v>
@@ -1467,13 +1467,13 @@
         <v>4</v>
       </c>
       <c r="E33">
-        <v>3.928</v>
+        <v>4</v>
       </c>
       <c r="F33">
-        <v>3.9</v>
+        <v>3.79</v>
       </c>
       <c r="G33">
-        <v>3.9339</v>
+        <v>3.932</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1481,22 +1481,22 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>230332</v>
+        <v>230140</v>
       </c>
       <c r="C34" t="s">
         <v>39</v>
       </c>
       <c r="D34">
-        <v>4</v>
+        <v>3.935</v>
       </c>
       <c r="E34">
-        <v>4</v>
+        <v>3.964</v>
       </c>
       <c r="F34">
-        <v>3.79</v>
+        <v>3.873</v>
       </c>
       <c r="G34">
-        <v>3.9323</v>
+        <v>3.924</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1504,22 +1504,22 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>230140</v>
+        <v>230521</v>
       </c>
       <c r="C35" t="s">
         <v>40</v>
       </c>
       <c r="D35">
-        <v>3.9357</v>
+        <v>4</v>
       </c>
       <c r="E35">
-        <v>3.964</v>
+        <v>4</v>
       </c>
       <c r="F35">
-        <v>3.8739</v>
+        <v>3.791</v>
       </c>
       <c r="G35">
-        <v>3.9242</v>
+        <v>3.922</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1527,22 +1527,22 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>230521</v>
+        <v>230536</v>
       </c>
       <c r="C36" t="s">
         <v>41</v>
       </c>
       <c r="D36">
-        <v>4</v>
+        <v>3.957</v>
       </c>
       <c r="E36">
-        <v>4</v>
+        <v>3.964</v>
       </c>
       <c r="F36">
-        <v>3.7913</v>
+        <v>3.847</v>
       </c>
       <c r="G36">
-        <v>3.9226</v>
+        <v>3.919</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1550,22 +1550,22 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>230536</v>
+        <v>230322</v>
       </c>
       <c r="C37" t="s">
         <v>42</v>
       </c>
       <c r="D37">
-        <v>3.9571</v>
+        <v>4</v>
       </c>
       <c r="E37">
-        <v>3.964</v>
+        <v>3.916</v>
       </c>
       <c r="F37">
-        <v>3.8478</v>
+        <v>3.862</v>
       </c>
       <c r="G37">
-        <v>3.9194</v>
+        <v>3.914</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1573,7 +1573,7 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>230322</v>
+        <v>230687</v>
       </c>
       <c r="C38" t="s">
         <v>43</v>
@@ -1582,13 +1582,13 @@
         <v>4</v>
       </c>
       <c r="E38">
-        <v>3.916</v>
+        <v>3.94</v>
       </c>
       <c r="F38">
-        <v>3.8625</v>
+        <v>3.83</v>
       </c>
       <c r="G38">
-        <v>3.9143</v>
+        <v>3.912</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1596,7 +1596,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>230687</v>
+        <v>230100</v>
       </c>
       <c r="C39" t="s">
         <v>44</v>
@@ -1605,13 +1605,13 @@
         <v>4</v>
       </c>
       <c r="E39">
-        <v>3.94</v>
+        <v>4</v>
       </c>
       <c r="F39">
-        <v>3.8304</v>
+        <v>3.721</v>
       </c>
       <c r="G39">
-        <v>3.9129</v>
+        <v>3.896</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1619,7 +1619,7 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>230100</v>
+        <v>230724</v>
       </c>
       <c r="C40" t="s">
         <v>45</v>
@@ -1628,13 +1628,13 @@
         <v>4</v>
       </c>
       <c r="E40">
-        <v>4</v>
+        <v>3.88</v>
       </c>
       <c r="F40">
-        <v>3.7217</v>
+        <v>3.847</v>
       </c>
       <c r="G40">
-        <v>3.8968</v>
+        <v>3.895</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1642,7 +1642,7 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>230724</v>
+        <v>230417</v>
       </c>
       <c r="C41" t="s">
         <v>46</v>
@@ -1651,13 +1651,13 @@
         <v>4</v>
       </c>
       <c r="E41">
-        <v>3.88</v>
+        <v>3.916</v>
       </c>
       <c r="F41">
-        <v>3.8478</v>
+        <v>3.804</v>
       </c>
       <c r="G41">
-        <v>3.8952</v>
+        <v>3.893</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -1665,7 +1665,7 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>230417</v>
+        <v>230038</v>
       </c>
       <c r="C42" t="s">
         <v>47</v>
@@ -1674,13 +1674,13 @@
         <v>4</v>
       </c>
       <c r="E42">
-        <v>3.916</v>
+        <v>4</v>
       </c>
       <c r="F42">
-        <v>3.8043</v>
+        <v>3.691</v>
       </c>
       <c r="G42">
-        <v>3.8935</v>
+        <v>3.885</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1688,7 +1688,7 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>230038</v>
+        <v>230130</v>
       </c>
       <c r="C43" t="s">
         <v>48</v>
@@ -1697,13 +1697,13 @@
         <v>4</v>
       </c>
       <c r="E43">
-        <v>4</v>
+        <v>3.964</v>
       </c>
       <c r="F43">
-        <v>3.6913</v>
+        <v>3.714</v>
       </c>
       <c r="G43">
-        <v>3.8855</v>
+        <v>3.885</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -1711,7 +1711,7 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>230130</v>
+        <v>230321</v>
       </c>
       <c r="C44" t="s">
         <v>49</v>
@@ -1720,13 +1720,13 @@
         <v>4</v>
       </c>
       <c r="E44">
-        <v>3.964</v>
+        <v>3.952</v>
       </c>
       <c r="F44">
-        <v>3.7143</v>
+        <v>3.73</v>
       </c>
       <c r="G44">
-        <v>3.885</v>
+        <v>3.88</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1734,22 +1734,22 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>230321</v>
+        <v>230300</v>
       </c>
       <c r="C45" t="s">
         <v>50</v>
       </c>
       <c r="D45">
-        <v>4</v>
+        <v>3.935</v>
       </c>
       <c r="E45">
-        <v>3.952</v>
+        <v>4</v>
       </c>
       <c r="F45">
-        <v>3.7304</v>
+        <v>3.713</v>
       </c>
       <c r="G45">
-        <v>3.8806</v>
+        <v>3.879</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -1757,22 +1757,22 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>230300</v>
+        <v>230145</v>
       </c>
       <c r="C46" t="s">
         <v>51</v>
       </c>
       <c r="D46">
-        <v>3.9357</v>
+        <v>3.935</v>
       </c>
       <c r="E46">
         <v>4</v>
       </c>
       <c r="F46">
-        <v>3.713</v>
+        <v>3.704</v>
       </c>
       <c r="G46">
-        <v>3.879</v>
+        <v>3.875</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -1780,22 +1780,22 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>230145</v>
+        <v>230212</v>
       </c>
       <c r="C47" t="s">
         <v>52</v>
       </c>
       <c r="D47">
-        <v>3.9357</v>
+        <v>3.957</v>
       </c>
       <c r="E47">
-        <v>4</v>
+        <v>3.88</v>
       </c>
       <c r="F47">
-        <v>3.7043</v>
+        <v>3.821</v>
       </c>
       <c r="G47">
-        <v>3.8758</v>
+        <v>3.875</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -1803,22 +1803,22 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>230212</v>
+        <v>230477</v>
       </c>
       <c r="C48" t="s">
         <v>53</v>
       </c>
       <c r="D48">
-        <v>3.9571</v>
+        <v>3.935</v>
       </c>
       <c r="E48">
-        <v>3.88</v>
+        <v>3.832</v>
       </c>
       <c r="F48">
-        <v>3.8217</v>
+        <v>3.873</v>
       </c>
       <c r="G48">
-        <v>3.8758</v>
+        <v>3.87</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -1826,22 +1826,22 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>230477</v>
+        <v>230613</v>
       </c>
       <c r="C49" t="s">
         <v>54</v>
       </c>
       <c r="D49">
-        <v>3.9357</v>
+        <v>4</v>
       </c>
       <c r="E49">
-        <v>3.832</v>
+        <v>3.952</v>
       </c>
       <c r="F49">
-        <v>3.8739</v>
+        <v>3.699</v>
       </c>
       <c r="G49">
-        <v>3.871</v>
+        <v>3.869</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -1849,22 +1849,22 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>230613</v>
+        <v>230697</v>
       </c>
       <c r="C50" t="s">
         <v>55</v>
       </c>
       <c r="D50">
-        <v>4</v>
+        <v>3.957</v>
       </c>
       <c r="E50">
-        <v>3.952</v>
+        <v>3.964</v>
       </c>
       <c r="F50">
-        <v>3.7</v>
+        <v>3.671</v>
       </c>
       <c r="G50">
-        <v>3.8694</v>
+        <v>3.86</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -1872,22 +1872,22 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>230697</v>
+        <v>230058</v>
       </c>
       <c r="C51" t="s">
         <v>56</v>
       </c>
       <c r="D51">
-        <v>3.9571</v>
+        <v>4</v>
       </c>
       <c r="E51">
-        <v>3.964</v>
+        <v>3.916</v>
       </c>
       <c r="F51">
-        <v>3.6714</v>
+        <v>3.713</v>
       </c>
       <c r="G51">
-        <v>3.86</v>
+        <v>3.859</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -1895,7 +1895,7 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>230058</v>
+        <v>230045</v>
       </c>
       <c r="C52" t="s">
         <v>57</v>
@@ -1907,10 +1907,10 @@
         <v>3.916</v>
       </c>
       <c r="F52">
-        <v>3.713</v>
+        <v>3.704</v>
       </c>
       <c r="G52">
-        <v>3.8597</v>
+        <v>3.856</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -1918,22 +1918,22 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>230065</v>
+        <v>230539</v>
       </c>
       <c r="C53" t="s">
         <v>58</v>
       </c>
       <c r="D53">
-        <v>3.8929</v>
+        <v>3.935</v>
       </c>
       <c r="E53">
-        <v>3.844</v>
+        <v>4</v>
       </c>
       <c r="F53">
-        <v>3.85</v>
+        <v>3.652</v>
       </c>
       <c r="G53">
-        <v>3.8576</v>
+        <v>3.856</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -1941,7 +1941,7 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>230045</v>
+        <v>230211</v>
       </c>
       <c r="C54" t="s">
         <v>59</v>
@@ -1950,13 +1950,13 @@
         <v>4</v>
       </c>
       <c r="E54">
-        <v>3.916</v>
+        <v>3.892</v>
       </c>
       <c r="F54">
-        <v>3.7043</v>
+        <v>3.721</v>
       </c>
       <c r="G54">
-        <v>3.8565</v>
+        <v>3.853</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -1964,22 +1964,22 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>230539</v>
+        <v>230659</v>
       </c>
       <c r="C55" t="s">
         <v>60</v>
       </c>
       <c r="D55">
-        <v>3.9357</v>
+        <v>3.857</v>
       </c>
       <c r="E55">
-        <v>4</v>
+        <v>3.88</v>
       </c>
       <c r="F55">
-        <v>3.6522</v>
+        <v>3.804</v>
       </c>
       <c r="G55">
-        <v>3.8565</v>
+        <v>3.846</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -1987,22 +1987,22 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>230211</v>
+        <v>230492</v>
       </c>
       <c r="C56" t="s">
         <v>61</v>
       </c>
       <c r="D56">
-        <v>4</v>
+        <v>3.935</v>
       </c>
       <c r="E56">
-        <v>3.892</v>
+        <v>3.916</v>
       </c>
       <c r="F56">
-        <v>3.7217</v>
+        <v>3.69</v>
       </c>
       <c r="G56">
-        <v>3.8532</v>
+        <v>3.841</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -2010,22 +2010,22 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>230659</v>
+        <v>230500</v>
       </c>
       <c r="C57" t="s">
         <v>62</v>
       </c>
       <c r="D57">
-        <v>3.8571</v>
+        <v>3.957</v>
       </c>
       <c r="E57">
-        <v>3.88</v>
+        <v>3.916</v>
       </c>
       <c r="F57">
-        <v>3.8043</v>
+        <v>3.678</v>
       </c>
       <c r="G57">
-        <v>3.8468</v>
+        <v>3.837</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -2033,22 +2033,22 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>230492</v>
+        <v>230180</v>
       </c>
       <c r="C58" t="s">
         <v>63</v>
       </c>
       <c r="D58">
-        <v>3.9357</v>
+        <v>3.935</v>
       </c>
       <c r="E58">
-        <v>3.916</v>
+        <v>3.832</v>
       </c>
       <c r="F58">
-        <v>3.6905</v>
+        <v>3.778</v>
       </c>
       <c r="G58">
-        <v>3.8417</v>
+        <v>3.835</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -2056,22 +2056,22 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>230500</v>
+        <v>230629</v>
       </c>
       <c r="C59" t="s">
         <v>64</v>
       </c>
       <c r="D59">
-        <v>3.9571</v>
+        <v>3.957</v>
       </c>
       <c r="E59">
         <v>3.916</v>
       </c>
       <c r="F59">
-        <v>3.6783</v>
+        <v>3.673</v>
       </c>
       <c r="G59">
-        <v>3.8371</v>
+        <v>3.835</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -2079,22 +2079,22 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>230180</v>
+        <v>230218</v>
       </c>
       <c r="C60" t="s">
         <v>65</v>
       </c>
       <c r="D60">
-        <v>3.9357</v>
+        <v>3.935</v>
       </c>
       <c r="E60">
+        <v>3.817</v>
+      </c>
+      <c r="F60">
+        <v>3.78</v>
+      </c>
+      <c r="G60">
         <v>3.832</v>
-      </c>
-      <c r="F60">
-        <v>3.7783</v>
-      </c>
-      <c r="G60">
-        <v>3.8355</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -2102,22 +2102,22 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>230629</v>
+        <v>230502</v>
       </c>
       <c r="C61" t="s">
         <v>66</v>
       </c>
       <c r="D61">
-        <v>3.9571</v>
+        <v>4</v>
       </c>
       <c r="E61">
-        <v>3.916</v>
+        <v>3.952</v>
       </c>
       <c r="F61">
-        <v>3.6739</v>
+        <v>3.586</v>
       </c>
       <c r="G61">
-        <v>3.8355</v>
+        <v>3.827</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -2125,22 +2125,22 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>230218</v>
+        <v>230470</v>
       </c>
       <c r="C62" t="s">
         <v>67</v>
       </c>
       <c r="D62">
-        <v>3.9357</v>
+        <v>4</v>
       </c>
       <c r="E62">
-        <v>3.8179</v>
+        <v>4</v>
       </c>
       <c r="F62">
-        <v>3.78</v>
+        <v>3.526</v>
       </c>
       <c r="G62">
-        <v>3.8323</v>
+        <v>3.824</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -2148,22 +2148,22 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>230502</v>
+        <v>230353</v>
       </c>
       <c r="C63" t="s">
         <v>68</v>
       </c>
       <c r="D63">
-        <v>4</v>
+        <v>3.9</v>
       </c>
       <c r="E63">
-        <v>3.952</v>
+        <v>3.964</v>
       </c>
       <c r="F63">
-        <v>3.587</v>
+        <v>3.613</v>
       </c>
       <c r="G63">
-        <v>3.8274</v>
+        <v>3.819</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -2171,7 +2171,7 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <v>230470</v>
+        <v>230525</v>
       </c>
       <c r="C64" t="s">
         <v>69</v>
@@ -2183,10 +2183,10 @@
         <v>4</v>
       </c>
       <c r="F64">
-        <v>3.5261</v>
+        <v>3.5</v>
       </c>
       <c r="G64">
-        <v>3.8242</v>
+        <v>3.814</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -2194,22 +2194,22 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>230353</v>
+        <v>230063</v>
       </c>
       <c r="C65" t="s">
         <v>70</v>
       </c>
       <c r="D65">
-        <v>3.9</v>
+        <v>4</v>
       </c>
       <c r="E65">
-        <v>3.964</v>
+        <v>3.916</v>
       </c>
       <c r="F65">
-        <v>3.613</v>
+        <v>3.56</v>
       </c>
       <c r="G65">
-        <v>3.8194</v>
+        <v>3.803</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -2217,22 +2217,22 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <v>230525</v>
+        <v>230164</v>
       </c>
       <c r="C66" t="s">
         <v>71</v>
       </c>
       <c r="D66">
-        <v>4</v>
+        <v>3.957</v>
       </c>
       <c r="E66">
-        <v>4</v>
+        <v>3.88</v>
       </c>
       <c r="F66">
-        <v>3.5</v>
+        <v>3.626</v>
       </c>
       <c r="G66">
-        <v>3.8145</v>
+        <v>3.803</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -2240,22 +2240,22 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <v>230063</v>
+        <v>230585</v>
       </c>
       <c r="C67" t="s">
         <v>72</v>
       </c>
       <c r="D67">
-        <v>4</v>
+        <v>3.935</v>
       </c>
       <c r="E67">
-        <v>3.916</v>
+        <v>3.964</v>
       </c>
       <c r="F67">
-        <v>3.5609</v>
+        <v>3.543</v>
       </c>
       <c r="G67">
-        <v>3.8032</v>
+        <v>3.801</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -2263,22 +2263,22 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <v>230164</v>
+        <v>230726</v>
       </c>
       <c r="C68" t="s">
         <v>73</v>
       </c>
       <c r="D68">
-        <v>3.9571</v>
+        <v>3.892</v>
       </c>
       <c r="E68">
         <v>3.88</v>
       </c>
       <c r="F68">
-        <v>3.6261</v>
+        <v>3.66</v>
       </c>
       <c r="G68">
-        <v>3.8032</v>
+        <v>3.801</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -2286,22 +2286,22 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <v>230585</v>
+        <v>230507</v>
       </c>
       <c r="C69" t="s">
         <v>74</v>
       </c>
       <c r="D69">
-        <v>3.9357</v>
+        <v>3.857</v>
       </c>
       <c r="E69">
-        <v>3.964</v>
+        <v>3.882</v>
       </c>
       <c r="F69">
-        <v>3.5435</v>
+        <v>3.645</v>
       </c>
       <c r="G69">
-        <v>3.8016</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -2309,22 +2309,22 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <v>230726</v>
+        <v>230070</v>
       </c>
       <c r="C70" t="s">
         <v>75</v>
       </c>
       <c r="D70">
-        <v>3.8929</v>
+        <v>3.957</v>
       </c>
       <c r="E70">
-        <v>3.88</v>
+        <v>3.824</v>
       </c>
       <c r="F70">
-        <v>3.6609</v>
+        <v>3.665</v>
       </c>
       <c r="G70">
-        <v>3.8016</v>
+        <v>3.795</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -2332,22 +2332,22 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>230507</v>
+        <v>230016</v>
       </c>
       <c r="C71" t="s">
         <v>76</v>
       </c>
       <c r="D71">
-        <v>3.8571</v>
+        <v>4</v>
       </c>
       <c r="E71">
-        <v>3.8821</v>
+        <v>3.914</v>
       </c>
       <c r="F71">
-        <v>3.645</v>
+        <v>3.479</v>
       </c>
       <c r="G71">
-        <v>3.8</v>
+        <v>3.793</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -2355,22 +2355,22 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <v>230070</v>
+        <v>230195</v>
       </c>
       <c r="C72" t="s">
         <v>77</v>
       </c>
       <c r="D72">
-        <v>3.9571</v>
+        <v>3.957</v>
       </c>
       <c r="E72">
-        <v>3.824</v>
+        <v>3.796</v>
       </c>
       <c r="F72">
-        <v>3.6652</v>
+        <v>3.678</v>
       </c>
       <c r="G72">
-        <v>3.7952</v>
+        <v>3.788</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -2378,7 +2378,7 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <v>230016</v>
+        <v>230689</v>
       </c>
       <c r="C73" t="s">
         <v>78</v>
@@ -2387,13 +2387,13 @@
         <v>4</v>
       </c>
       <c r="E73">
-        <v>3.9143</v>
+        <v>4</v>
       </c>
       <c r="F73">
-        <v>3.48</v>
+        <v>3.385</v>
       </c>
       <c r="G73">
-        <v>3.7935</v>
+        <v>3.784</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -2401,22 +2401,22 @@
         <v>73</v>
       </c>
       <c r="B74">
-        <v>230280</v>
+        <v>230526</v>
       </c>
       <c r="C74" t="s">
         <v>79</v>
       </c>
       <c r="D74">
-        <v>3.85</v>
+        <v>3.935</v>
       </c>
       <c r="E74">
-        <v>3.916</v>
+        <v>3.952</v>
       </c>
       <c r="F74">
-        <v>3.6</v>
+        <v>3.495</v>
       </c>
       <c r="G74">
-        <v>3.7932</v>
+        <v>3.779</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -2424,22 +2424,22 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <v>230195</v>
+        <v>230654</v>
       </c>
       <c r="C75" t="s">
         <v>80</v>
       </c>
       <c r="D75">
-        <v>3.9571</v>
+        <v>3.935</v>
       </c>
       <c r="E75">
-        <v>3.796</v>
+        <v>3.852</v>
       </c>
       <c r="F75">
-        <v>3.6783</v>
+        <v>3.591</v>
       </c>
       <c r="G75">
-        <v>3.7887</v>
+        <v>3.774</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -2447,22 +2447,22 @@
         <v>75</v>
       </c>
       <c r="B76">
-        <v>230526</v>
+        <v>230052</v>
       </c>
       <c r="C76" t="s">
         <v>81</v>
       </c>
       <c r="D76">
-        <v>3.9357</v>
+        <v>3.75</v>
       </c>
       <c r="E76">
-        <v>3.952</v>
+        <v>3.85</v>
       </c>
       <c r="F76">
-        <v>3.4957</v>
+        <v>3.63</v>
       </c>
       <c r="G76">
-        <v>3.779</v>
+        <v>3.756</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -2470,22 +2470,22 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <v>230654</v>
+        <v>230727</v>
       </c>
       <c r="C77" t="s">
         <v>82</v>
       </c>
       <c r="D77">
-        <v>3.9357</v>
+        <v>3.785</v>
       </c>
       <c r="E77">
-        <v>3.852</v>
+        <v>3.892</v>
       </c>
       <c r="F77">
-        <v>3.5913</v>
+        <v>3.54</v>
       </c>
       <c r="G77">
-        <v>3.7742</v>
+        <v>3.754</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -2493,22 +2493,22 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <v>230020</v>
+        <v>230327</v>
       </c>
       <c r="C78" t="s">
         <v>83</v>
       </c>
       <c r="D78">
-        <v>4</v>
+        <v>3.85</v>
       </c>
       <c r="E78">
-        <v>3.868</v>
+        <v>3.683</v>
       </c>
       <c r="F78">
-        <v>3.455</v>
+        <v>3.765</v>
       </c>
       <c r="G78">
-        <v>3.7593</v>
+        <v>3.751</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -2516,22 +2516,22 @@
         <v>78</v>
       </c>
       <c r="B79">
-        <v>230052</v>
+        <v>230017</v>
       </c>
       <c r="C79" t="s">
         <v>84</v>
       </c>
       <c r="D79">
-        <v>3.75</v>
+        <v>3.9</v>
       </c>
       <c r="E79">
-        <v>3.85</v>
+        <v>3.952</v>
       </c>
       <c r="F79">
-        <v>3.63</v>
+        <v>3.441</v>
       </c>
       <c r="G79">
-        <v>3.7565</v>
+        <v>3.746</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -2539,22 +2539,22 @@
         <v>79</v>
       </c>
       <c r="B80">
-        <v>230327</v>
+        <v>230473</v>
       </c>
       <c r="C80" t="s">
         <v>85</v>
       </c>
       <c r="D80">
-        <v>3.85</v>
+        <v>3.892</v>
       </c>
       <c r="E80">
-        <v>3.684</v>
+        <v>3.916</v>
       </c>
       <c r="F80">
-        <v>3.7652</v>
+        <v>3.443</v>
       </c>
       <c r="G80">
-        <v>3.7516</v>
+        <v>3.735</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -2562,22 +2562,22 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <v>230017</v>
+        <v>230012</v>
       </c>
       <c r="C81" t="s">
         <v>86</v>
       </c>
       <c r="D81">
-        <v>3.9</v>
+        <v>3.914</v>
       </c>
       <c r="E81">
-        <v>3.952</v>
+        <v>3.796</v>
       </c>
       <c r="F81">
-        <v>3.4417</v>
+        <v>3.558</v>
       </c>
       <c r="G81">
-        <v>3.746</v>
+        <v>3.731</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -2585,22 +2585,22 @@
         <v>81</v>
       </c>
       <c r="B82">
-        <v>230473</v>
+        <v>230147</v>
       </c>
       <c r="C82" t="s">
         <v>87</v>
       </c>
       <c r="D82">
-        <v>3.8929</v>
+        <v>3.892</v>
       </c>
       <c r="E82">
-        <v>3.916</v>
+        <v>3.832</v>
       </c>
       <c r="F82">
-        <v>3.4435</v>
+        <v>3.508</v>
       </c>
       <c r="G82">
-        <v>3.7355</v>
+        <v>3.725</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -2608,22 +2608,22 @@
         <v>82</v>
       </c>
       <c r="B83">
-        <v>230727</v>
+        <v>230077</v>
       </c>
       <c r="C83" t="s">
         <v>88</v>
       </c>
       <c r="D83">
-        <v>3.7857</v>
+        <v>3.785</v>
       </c>
       <c r="E83">
-        <v>3.85</v>
+        <v>3.753</v>
       </c>
       <c r="F83">
-        <v>3.54</v>
+        <v>3.619</v>
       </c>
       <c r="G83">
-        <v>3.7355</v>
+        <v>3.715</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -2631,22 +2631,22 @@
         <v>83</v>
       </c>
       <c r="B84">
-        <v>230012</v>
+        <v>230444</v>
       </c>
       <c r="C84" t="s">
         <v>89</v>
       </c>
       <c r="D84">
-        <v>3.9143</v>
+        <v>3.785</v>
       </c>
       <c r="E84">
-        <v>3.796</v>
+        <v>3.625</v>
       </c>
       <c r="F84">
-        <v>3.5583</v>
+        <v>3.757</v>
       </c>
       <c r="G84">
-        <v>3.7317</v>
+        <v>3.704</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -2654,22 +2654,22 @@
         <v>84</v>
       </c>
       <c r="B85">
-        <v>230147</v>
+        <v>230375</v>
       </c>
       <c r="C85" t="s">
         <v>90</v>
       </c>
       <c r="D85">
-        <v>3.8929</v>
+        <v>3.85</v>
       </c>
       <c r="E85">
-        <v>3.832</v>
+        <v>3.712</v>
       </c>
       <c r="F85">
-        <v>3.5087</v>
+        <v>3.599</v>
       </c>
       <c r="G85">
-        <v>3.7258</v>
+        <v>3.701</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -2677,22 +2677,22 @@
         <v>85</v>
       </c>
       <c r="B86">
-        <v>230077</v>
+        <v>230407</v>
       </c>
       <c r="C86" t="s">
         <v>91</v>
       </c>
       <c r="D86">
-        <v>3.7857</v>
+        <v>4</v>
       </c>
       <c r="E86">
-        <v>3.7536</v>
+        <v>3.747</v>
       </c>
       <c r="F86">
-        <v>3.619</v>
+        <v>3.469</v>
       </c>
       <c r="G86">
-        <v>3.7159</v>
+        <v>3.701</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -2700,22 +2700,22 @@
         <v>86</v>
       </c>
       <c r="B87">
-        <v>230444</v>
+        <v>230527</v>
       </c>
       <c r="C87" t="s">
         <v>92</v>
       </c>
       <c r="D87">
-        <v>3.7857</v>
+        <v>4</v>
       </c>
       <c r="E87">
-        <v>3.625</v>
+        <v>3.844</v>
       </c>
       <c r="F87">
-        <v>3.7571</v>
+        <v>3.339</v>
       </c>
       <c r="G87">
-        <v>3.7048</v>
+        <v>3.691</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -2723,22 +2723,22 @@
         <v>87</v>
       </c>
       <c r="B88">
-        <v>230375</v>
+        <v>230261</v>
       </c>
       <c r="C88" t="s">
         <v>93</v>
       </c>
       <c r="D88">
-        <v>3.85</v>
+        <v>4</v>
       </c>
       <c r="E88">
-        <v>3.712</v>
+        <v>3.768</v>
       </c>
       <c r="F88">
-        <v>3.6</v>
+        <v>3.424</v>
       </c>
       <c r="G88">
-        <v>3.7016</v>
+        <v>3.688</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -2746,22 +2746,22 @@
         <v>88</v>
       </c>
       <c r="B89">
-        <v>230407</v>
+        <v>230013</v>
       </c>
       <c r="C89" t="s">
         <v>94</v>
       </c>
       <c r="D89">
-        <v>4</v>
+        <v>3.85</v>
       </c>
       <c r="E89">
-        <v>3.748</v>
+        <v>3.647</v>
       </c>
       <c r="F89">
-        <v>3.4696</v>
+        <v>3.638</v>
       </c>
       <c r="G89">
-        <v>3.7016</v>
+        <v>3.687</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -2769,22 +2769,22 @@
         <v>89</v>
       </c>
       <c r="B90">
-        <v>230527</v>
+        <v>230495</v>
       </c>
       <c r="C90" t="s">
         <v>95</v>
       </c>
       <c r="D90">
-        <v>4</v>
+        <v>3.85</v>
       </c>
       <c r="E90">
         <v>3.844</v>
       </c>
       <c r="F90">
-        <v>3.3391</v>
+        <v>3.417</v>
       </c>
       <c r="G90">
-        <v>3.6919</v>
+        <v>3.687</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -2792,22 +2792,22 @@
         <v>90</v>
       </c>
       <c r="B91">
-        <v>230261</v>
+        <v>230458</v>
       </c>
       <c r="C91" t="s">
         <v>96</v>
       </c>
       <c r="D91">
-        <v>4</v>
+        <v>3.957</v>
       </c>
       <c r="E91">
-        <v>3.768</v>
+        <v>3.736</v>
       </c>
       <c r="F91">
-        <v>3.425</v>
+        <v>3.465</v>
       </c>
       <c r="G91">
-        <v>3.6889</v>
+        <v>3.685</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -2815,22 +2815,22 @@
         <v>91</v>
       </c>
       <c r="B92">
-        <v>230013</v>
+        <v>230735</v>
       </c>
       <c r="C92" t="s">
         <v>97</v>
       </c>
       <c r="D92">
-        <v>3.85</v>
+        <v>3.935</v>
       </c>
       <c r="E92">
-        <v>3.648</v>
+        <v>3.804</v>
       </c>
       <c r="F92">
-        <v>3.6385</v>
+        <v>3.399</v>
       </c>
       <c r="G92">
-        <v>3.6877</v>
+        <v>3.683</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -2838,22 +2838,22 @@
         <v>92</v>
       </c>
       <c r="B93">
-        <v>230495</v>
+        <v>230248</v>
       </c>
       <c r="C93" t="s">
         <v>98</v>
       </c>
       <c r="D93">
-        <v>3.85</v>
+        <v>3.935</v>
       </c>
       <c r="E93">
-        <v>3.844</v>
+        <v>3.663</v>
       </c>
       <c r="F93">
-        <v>3.4174</v>
+        <v>3.543</v>
       </c>
       <c r="G93">
-        <v>3.6871</v>
+        <v>3.68</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -2861,22 +2861,22 @@
         <v>93</v>
       </c>
       <c r="B94">
-        <v>230520</v>
+        <v>230065</v>
       </c>
       <c r="C94" t="s">
         <v>99</v>
       </c>
       <c r="D94">
-        <v>3.85</v>
+        <v>3.892</v>
       </c>
       <c r="E94">
-        <v>3.748</v>
+        <v>3.844</v>
       </c>
       <c r="F94">
-        <v>3.495</v>
+        <v>3.347</v>
       </c>
       <c r="G94">
-        <v>3.6864</v>
+        <v>3.67</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -2884,22 +2884,22 @@
         <v>94</v>
       </c>
       <c r="B95">
-        <v>230458</v>
+        <v>230229</v>
       </c>
       <c r="C95" t="s">
         <v>100</v>
       </c>
       <c r="D95">
-        <v>3.9571</v>
+        <v>3.85</v>
       </c>
       <c r="E95">
-        <v>3.736</v>
+        <v>3.784</v>
       </c>
       <c r="F95">
-        <v>3.4652</v>
+        <v>3.4</v>
       </c>
       <c r="G95">
-        <v>3.6855</v>
+        <v>3.665</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -2907,22 +2907,22 @@
         <v>95</v>
       </c>
       <c r="B96">
-        <v>230735</v>
+        <v>230650</v>
       </c>
       <c r="C96" t="s">
         <v>101</v>
       </c>
       <c r="D96">
-        <v>3.9357</v>
+        <v>4</v>
       </c>
       <c r="E96">
-        <v>3.804</v>
+        <v>3.732</v>
       </c>
       <c r="F96">
-        <v>3.4</v>
+        <v>3.373</v>
       </c>
       <c r="G96">
-        <v>3.6839</v>
+        <v>3.659</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -2930,22 +2930,22 @@
         <v>96</v>
       </c>
       <c r="B97">
-        <v>230248</v>
+        <v>230208</v>
       </c>
       <c r="C97" t="s">
         <v>102</v>
       </c>
       <c r="D97">
-        <v>3.9357</v>
+        <v>4</v>
       </c>
       <c r="E97">
-        <v>3.664</v>
+        <v>3.636</v>
       </c>
       <c r="F97">
-        <v>3.5435</v>
+        <v>3.46</v>
       </c>
       <c r="G97">
-        <v>3.6806</v>
+        <v>3.653</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -2953,22 +2953,22 @@
         <v>97</v>
       </c>
       <c r="B98">
-        <v>230229</v>
+        <v>230175</v>
       </c>
       <c r="C98" t="s">
         <v>103</v>
       </c>
       <c r="D98">
-        <v>3.85</v>
+        <v>3.957</v>
       </c>
       <c r="E98">
-        <v>3.784</v>
+        <v>3.696</v>
       </c>
       <c r="F98">
-        <v>3.4</v>
+        <v>3.404</v>
       </c>
       <c r="G98">
-        <v>3.665</v>
+        <v>3.646</v>
       </c>
     </row>
     <row r="99" spans="1:7">
@@ -2976,22 +2976,22 @@
         <v>98</v>
       </c>
       <c r="B99">
-        <v>230650</v>
+        <v>230563</v>
       </c>
       <c r="C99" t="s">
         <v>104</v>
       </c>
       <c r="D99">
-        <v>4</v>
+        <v>3.892</v>
       </c>
       <c r="E99">
-        <v>3.732</v>
+        <v>3.747</v>
       </c>
       <c r="F99">
-        <v>3.3739</v>
+        <v>3.304</v>
       </c>
       <c r="G99">
-        <v>3.6597</v>
+        <v>3.616</v>
       </c>
     </row>
     <row r="100" spans="1:7">
@@ -2999,22 +2999,22 @@
         <v>99</v>
       </c>
       <c r="B100">
-        <v>230208</v>
+        <v>230280</v>
       </c>
       <c r="C100" t="s">
         <v>105</v>
       </c>
       <c r="D100">
-        <v>4</v>
+        <v>3.85</v>
       </c>
       <c r="E100">
-        <v>3.636</v>
+        <v>3.916</v>
       </c>
       <c r="F100">
-        <v>3.4609</v>
+        <v>3.13</v>
       </c>
       <c r="G100">
-        <v>3.6532</v>
+        <v>3.609</v>
       </c>
     </row>
     <row r="101" spans="1:7">
@@ -3022,22 +3022,22 @@
         <v>100</v>
       </c>
       <c r="B101">
-        <v>230581</v>
+        <v>230395</v>
       </c>
       <c r="C101" t="s">
         <v>106</v>
       </c>
       <c r="D101">
-        <v>3.7929</v>
+        <v>3.85</v>
       </c>
       <c r="E101">
-        <v>3.6429</v>
+        <v>3.683</v>
       </c>
       <c r="F101">
-        <v>3.5471</v>
+        <v>3.334</v>
       </c>
       <c r="G101">
-        <v>3.6508</v>
+        <v>3.591</v>
       </c>
     </row>
     <row r="102" spans="1:7">
@@ -3045,22 +3045,22 @@
         <v>101</v>
       </c>
       <c r="B102">
-        <v>230175</v>
+        <v>230259</v>
       </c>
       <c r="C102" t="s">
         <v>107</v>
       </c>
       <c r="D102">
-        <v>3.9571</v>
+        <v>3.85</v>
       </c>
       <c r="E102">
-        <v>3.696</v>
+        <v>3.567</v>
       </c>
       <c r="F102">
-        <v>3.4043</v>
+        <v>3.447</v>
       </c>
       <c r="G102">
-        <v>3.6468</v>
+        <v>3.59</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -3068,22 +3068,22 @@
         <v>102</v>
       </c>
       <c r="B103">
-        <v>230238</v>
+        <v>230020</v>
       </c>
       <c r="C103" t="s">
         <v>108</v>
       </c>
       <c r="D103">
-        <v>3.7643</v>
+        <v>4</v>
       </c>
       <c r="E103">
-        <v>3.4786</v>
+        <v>3.868</v>
       </c>
       <c r="F103">
-        <v>3.75</v>
+        <v>3.004</v>
       </c>
       <c r="G103">
-        <v>3.6267</v>
+        <v>3.577</v>
       </c>
     </row>
     <row r="104" spans="1:7">
@@ -3091,22 +3091,22 @@
         <v>103</v>
       </c>
       <c r="B104">
-        <v>230563</v>
+        <v>230033</v>
       </c>
       <c r="C104" t="s">
         <v>109</v>
       </c>
       <c r="D104">
-        <v>3.8929</v>
+        <v>3.85</v>
       </c>
       <c r="E104">
-        <v>3.748</v>
+        <v>3.635</v>
       </c>
       <c r="F104">
-        <v>3.3043</v>
+        <v>3.347</v>
       </c>
       <c r="G104">
-        <v>3.6161</v>
+        <v>3.577</v>
       </c>
     </row>
     <row r="105" spans="1:7">
@@ -3114,22 +3114,22 @@
         <v>104</v>
       </c>
       <c r="B105">
-        <v>230730</v>
+        <v>230636</v>
       </c>
       <c r="C105" t="s">
         <v>110</v>
       </c>
       <c r="D105">
-        <v>4</v>
+        <v>3.892</v>
       </c>
       <c r="E105">
-        <v>3.656</v>
+        <v>3.612</v>
       </c>
       <c r="F105">
-        <v>3.1706</v>
+        <v>3.278</v>
       </c>
       <c r="G105">
-        <v>3.5946</v>
+        <v>3.551</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -3137,7 +3137,7 @@
         <v>105</v>
       </c>
       <c r="B106">
-        <v>230395</v>
+        <v>230520</v>
       </c>
       <c r="C106" t="s">
         <v>111</v>
@@ -3146,13 +3146,13 @@
         <v>3.85</v>
       </c>
       <c r="E106">
-        <v>3.684</v>
+        <v>3.747</v>
       </c>
       <c r="F106">
-        <v>3.3348</v>
+        <v>3.039</v>
       </c>
       <c r="G106">
-        <v>3.5919</v>
+        <v>3.508</v>
       </c>
     </row>
     <row r="107" spans="1:7">
@@ -3160,7 +3160,7 @@
         <v>106</v>
       </c>
       <c r="B107">
-        <v>230259</v>
+        <v>230224</v>
       </c>
       <c r="C107" t="s">
         <v>112</v>
@@ -3169,13 +3169,13 @@
         <v>3.85</v>
       </c>
       <c r="E107">
-        <v>3.5679</v>
+        <v>3.528</v>
       </c>
       <c r="F107">
-        <v>3.4476</v>
+        <v>3.221</v>
       </c>
       <c r="G107">
-        <v>3.5905</v>
+        <v>3.487</v>
       </c>
     </row>
     <row r="108" spans="1:7">
@@ -3183,7 +3183,7 @@
         <v>107</v>
       </c>
       <c r="B108">
-        <v>230033</v>
+        <v>230268</v>
       </c>
       <c r="C108" t="s">
         <v>113</v>
@@ -3192,13 +3192,13 @@
         <v>3.85</v>
       </c>
       <c r="E108">
-        <v>3.636</v>
+        <v>3.62</v>
       </c>
       <c r="F108">
-        <v>3.3478</v>
+        <v>3.095</v>
       </c>
       <c r="G108">
-        <v>3.5774</v>
+        <v>3.477</v>
       </c>
     </row>
     <row r="109" spans="1:7">
@@ -3206,22 +3206,22 @@
         <v>108</v>
       </c>
       <c r="B109">
-        <v>230183</v>
+        <v>230581</v>
       </c>
       <c r="C109" t="s">
         <v>114</v>
       </c>
       <c r="D109">
-        <v>4</v>
+        <v>3.792</v>
       </c>
       <c r="E109">
-        <v>3.536</v>
+        <v>3.642</v>
       </c>
       <c r="F109">
-        <v>3.2529</v>
+        <v>3.014</v>
       </c>
       <c r="G109">
-        <v>3.5661</v>
+        <v>3.474</v>
       </c>
     </row>
     <row r="110" spans="1:7">
@@ -3229,22 +3229,22 @@
         <v>109</v>
       </c>
       <c r="B110">
-        <v>230493</v>
+        <v>230564</v>
       </c>
       <c r="C110" t="s">
         <v>115</v>
       </c>
       <c r="D110">
-        <v>3.9357</v>
+        <v>3.871</v>
       </c>
       <c r="E110">
-        <v>3.5591</v>
+        <v>3.468</v>
       </c>
       <c r="F110">
-        <v>3.3348</v>
+        <v>3.221</v>
       </c>
       <c r="G110">
-        <v>3.561</v>
+        <v>3.467</v>
       </c>
     </row>
     <row r="111" spans="1:7">
@@ -3252,22 +3252,22 @@
         <v>110</v>
       </c>
       <c r="B111">
-        <v>230636</v>
+        <v>230238</v>
       </c>
       <c r="C111" t="s">
         <v>116</v>
       </c>
       <c r="D111">
-        <v>3.8929</v>
+        <v>3.764</v>
       </c>
       <c r="E111">
-        <v>3.612</v>
+        <v>3.478</v>
       </c>
       <c r="F111">
-        <v>3.2783</v>
+        <v>3.214</v>
       </c>
       <c r="G111">
-        <v>3.5516</v>
+        <v>3.453</v>
       </c>
     </row>
     <row r="112" spans="1:7">
@@ -3275,22 +3275,22 @@
         <v>111</v>
       </c>
       <c r="B112">
-        <v>230203</v>
+        <v>230493</v>
       </c>
       <c r="C112" t="s">
         <v>117</v>
       </c>
       <c r="D112">
-        <v>3.85</v>
+        <v>3.935</v>
       </c>
       <c r="E112">
-        <v>3.488</v>
+        <v>3.132</v>
       </c>
       <c r="F112">
-        <v>3.25</v>
+        <v>3.334</v>
       </c>
       <c r="G112">
-        <v>3.5018</v>
+        <v>3.388</v>
       </c>
     </row>
     <row r="113" spans="1:7">
@@ -3298,7 +3298,7 @@
         <v>112</v>
       </c>
       <c r="B113">
-        <v>230224</v>
+        <v>230203</v>
       </c>
       <c r="C113" t="s">
         <v>118</v>
@@ -3307,13 +3307,13 @@
         <v>3.85</v>
       </c>
       <c r="E113">
-        <v>3.528</v>
+        <v>3.487</v>
       </c>
       <c r="F113">
-        <v>3.2217</v>
+        <v>2.785</v>
       </c>
       <c r="G113">
-        <v>3.4871</v>
+        <v>3.326</v>
       </c>
     </row>
     <row r="114" spans="1:7">
@@ -3321,22 +3321,22 @@
         <v>113</v>
       </c>
       <c r="B114">
-        <v>230268</v>
+        <v>230449</v>
       </c>
       <c r="C114" t="s">
         <v>119</v>
       </c>
       <c r="D114">
-        <v>3.85</v>
+        <v>3.807</v>
       </c>
       <c r="E114">
-        <v>3.62</v>
+        <v>3.317</v>
       </c>
       <c r="F114">
-        <v>3.0957</v>
+        <v>2.835</v>
       </c>
       <c r="G114">
-        <v>3.4774</v>
+        <v>3.272</v>
       </c>
     </row>
     <row r="115" spans="1:7">
@@ -3344,22 +3344,22 @@
         <v>114</v>
       </c>
       <c r="B115">
-        <v>230564</v>
+        <v>230730</v>
       </c>
       <c r="C115" t="s">
         <v>120</v>
       </c>
       <c r="D115">
-        <v>3.8714</v>
+        <v>4</v>
       </c>
       <c r="E115">
-        <v>3.468</v>
+        <v>3.656</v>
       </c>
       <c r="F115">
-        <v>3.2217</v>
+        <v>2.343</v>
       </c>
       <c r="G115">
-        <v>3.4677</v>
+        <v>3.246</v>
       </c>
     </row>
     <row r="116" spans="1:7">
@@ -3367,22 +3367,22 @@
         <v>115</v>
       </c>
       <c r="B116">
-        <v>230449</v>
+        <v>230183</v>
       </c>
       <c r="C116" t="s">
         <v>121</v>
       </c>
       <c r="D116">
-        <v>3.8071</v>
+        <v>4</v>
       </c>
       <c r="E116">
-        <v>3.3179</v>
+        <v>3.536</v>
       </c>
       <c r="F116">
-        <v>2.835</v>
+        <v>2.404</v>
       </c>
       <c r="G116">
-        <v>3.2726</v>
+        <v>3.22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update output Excel files for all semesters
</commit_message>
<xml_diff>
--- a/output/CGPA_Results.xlsx
+++ b/output/CGPA_Results.xlsx
@@ -46,6 +46,9 @@
     <t>ELAPATHA C.D.</t>
   </si>
   <si>
+    <t>NETTIKUMARA N.A.H.G.</t>
+  </si>
+  <si>
     <t>ADIKARAM D.M.G.H.</t>
   </si>
   <si>
@@ -55,16 +58,16 @@
     <t>BANDARA W.D.A.C.</t>
   </si>
   <si>
+    <t>PERERA G.M.B.</t>
+  </si>
+  <si>
+    <t>RATNAYAKE R.M.S.H.</t>
+  </si>
+  <si>
     <t>DHANANJAYA K.T.G.T.N.</t>
   </si>
   <si>
-    <t>NETTIKUMARA N.A.H.G.</t>
-  </si>
-  <si>
-    <t>PERERA G.M.B.</t>
-  </si>
-  <si>
-    <t>RATNAYAKE R.M.S.H.</t>
+    <t>COLOMBAGE D.M.</t>
   </si>
   <si>
     <t>ILANKOON I.M.M.K.B.</t>
@@ -73,9 +76,6 @@
     <t>KARIYAWASAM J.H.D.</t>
   </si>
   <si>
-    <t>COLOMBAGE D.M.</t>
-  </si>
-  <si>
     <t>KUMARA K.B.R.</t>
   </si>
   <si>
@@ -91,12 +91,12 @@
     <t>KUMARASINGHE M.N.</t>
   </si>
   <si>
+    <t>PEIRIS E.A.S.S.</t>
+  </si>
+  <si>
     <t>DE MEL D.J.</t>
   </si>
   <si>
-    <t>PEIRIS E.A.S.S.</t>
-  </si>
-  <si>
     <t>RAHUL B.</t>
   </si>
   <si>
@@ -124,12 +124,12 @@
     <t>PATHIRANA P.T.S.</t>
   </si>
   <si>
+    <t>GARUSINGHE S.B.</t>
+  </si>
+  <si>
     <t>ARACHCHI A.D.I.D.</t>
   </si>
   <si>
-    <t>GARUSINGHE S.B.</t>
-  </si>
-  <si>
     <t>KEERAWELLA K.P.C.P.</t>
   </si>
   <si>
@@ -148,21 +148,24 @@
     <t>WEDAMESTRIGE A.N.</t>
   </si>
   <si>
+    <t>MUNASINGHE A.I.</t>
+  </si>
+  <si>
     <t>CHANDRAKUMARA H.A.D.C.</t>
   </si>
   <si>
     <t>WIJESEKARA W.A.G.S.</t>
   </si>
   <si>
-    <t>MUNASINGHE A.I.</t>
-  </si>
-  <si>
     <t>AMARATHUNGE A.M.N.L.</t>
   </si>
   <si>
     <t>DESHAN W.U.</t>
   </si>
   <si>
+    <t>GUNASEKARA L.U.A.</t>
+  </si>
+  <si>
     <t>KARUNANAYAKE A.H.D.</t>
   </si>
   <si>
@@ -172,19 +175,19 @@
     <t>DILHAN W.A.</t>
   </si>
   <si>
-    <t>GUNASEKARA L.U.A.</t>
-  </si>
-  <si>
     <t>PERERA H.A.J.I.</t>
   </si>
   <si>
     <t>SHEHAN M.N.N.</t>
   </si>
   <si>
+    <t>AROSHANA H.A.P.</t>
+  </si>
+  <si>
     <t>WEERASINGHE J.A.H.R.</t>
   </si>
   <si>
-    <t>AROSHANA H.A.P.</t>
+    <t>GUNASEKARA K.S.</t>
   </si>
   <si>
     <t>ANTHONY C.S.B.</t>
@@ -193,9 +196,6 @@
     <t>RATHEESHAN A.R.</t>
   </si>
   <si>
-    <t>GUNASEKARA K.S.</t>
-  </si>
-  <si>
     <t>UPEKSHANI T.S.</t>
   </si>
   <si>
@@ -283,13 +283,13 @@
     <t>BANDARA K.M.N.D.</t>
   </si>
   <si>
+    <t>MEEDENIYA M.M.H.</t>
+  </si>
+  <si>
     <t>NIRMANI W.T.</t>
   </si>
   <si>
     <t>LENMINI B.L.W.</t>
-  </si>
-  <si>
-    <t>MEEDENIYA M.M.H.</t>
   </si>
   <si>
     <t>RANAWAKA R.A.G.K.</t>
@@ -814,7 +814,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>230018</v>
+        <v>230436</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -823,13 +823,13 @@
         <v>4</v>
       </c>
       <c r="E5">
-        <v>4</v>
+        <v>3.975</v>
       </c>
       <c r="F5">
-        <v>3.96</v>
+        <v>4</v>
       </c>
       <c r="G5">
-        <v>3.985</v>
+        <v>3.99</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -837,7 +837,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>230074</v>
+        <v>230018</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -860,7 +860,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>230082</v>
+        <v>230074</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
@@ -883,7 +883,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>230138</v>
+        <v>230082</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
@@ -895,7 +895,7 @@
         <v>4</v>
       </c>
       <c r="F8">
-        <v>3.957</v>
+        <v>3.96</v>
       </c>
       <c r="G8">
         <v>3.985</v>
@@ -906,7 +906,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>230436</v>
+        <v>230476</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
@@ -915,10 +915,10 @@
         <v>4</v>
       </c>
       <c r="E9">
-        <v>3.964</v>
+        <v>4</v>
       </c>
       <c r="F9">
-        <v>4</v>
+        <v>3.96</v>
       </c>
       <c r="G9">
         <v>3.985</v>
@@ -929,7 +929,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>230476</v>
+        <v>230548</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
@@ -952,7 +952,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>230548</v>
+        <v>230138</v>
       </c>
       <c r="C11" t="s">
         <v>16</v>
@@ -964,10 +964,10 @@
         <v>4</v>
       </c>
       <c r="F11">
-        <v>3.96</v>
+        <v>3.957</v>
       </c>
       <c r="G11">
-        <v>3.985</v>
+        <v>3.984</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -975,22 +975,22 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>230256</v>
+        <v>230108</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
       </c>
       <c r="D12">
-        <v>4</v>
+        <v>3.935</v>
       </c>
       <c r="E12">
         <v>4</v>
       </c>
       <c r="F12">
-        <v>3.925</v>
+        <v>3.954</v>
       </c>
       <c r="G12">
-        <v>3.971</v>
+        <v>3.97</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -998,7 +998,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>230318</v>
+        <v>230256</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
@@ -1010,10 +1010,10 @@
         <v>4</v>
       </c>
       <c r="F13">
-        <v>3.924</v>
+        <v>3.925</v>
       </c>
       <c r="G13">
-        <v>3.971</v>
+        <v>3.97</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1021,19 +1021,19 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>230108</v>
+        <v>230318</v>
       </c>
       <c r="C14" t="s">
         <v>19</v>
       </c>
       <c r="D14">
-        <v>3.935</v>
+        <v>4</v>
       </c>
       <c r="E14">
         <v>4</v>
       </c>
       <c r="F14">
-        <v>3.954</v>
+        <v>3.924</v>
       </c>
       <c r="G14">
         <v>3.97</v>
@@ -1105,7 +1105,7 @@
         <v>4</v>
       </c>
       <c r="G17">
-        <v>3.966</v>
+        <v>3.965</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1128,7 +1128,7 @@
         <v>3.9</v>
       </c>
       <c r="G18">
-        <v>3.965</v>
+        <v>3.964</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1159,19 +1159,19 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>230121</v>
+        <v>230469</v>
       </c>
       <c r="C20" t="s">
         <v>25</v>
       </c>
       <c r="D20">
-        <v>3.957</v>
+        <v>4</v>
       </c>
       <c r="E20">
-        <v>4</v>
+        <v>3.962</v>
       </c>
       <c r="F20">
-        <v>3.921</v>
+        <v>3.937</v>
       </c>
       <c r="G20">
         <v>3.961</v>
@@ -1182,22 +1182,22 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>230469</v>
+        <v>230121</v>
       </c>
       <c r="C21" t="s">
         <v>26</v>
       </c>
       <c r="D21">
-        <v>4</v>
+        <v>3.957</v>
       </c>
       <c r="E21">
-        <v>3.964</v>
+        <v>4</v>
       </c>
       <c r="F21">
-        <v>3.937</v>
+        <v>3.921</v>
       </c>
       <c r="G21">
-        <v>3.961</v>
+        <v>3.96</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1220,7 +1220,7 @@
         <v>3.882</v>
       </c>
       <c r="G22">
-        <v>3.956</v>
+        <v>3.955</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1237,7 +1237,7 @@
         <v>4</v>
       </c>
       <c r="E23">
-        <v>3.927</v>
+        <v>3.924</v>
       </c>
       <c r="F23">
         <v>3.957</v>
@@ -1260,7 +1260,7 @@
         <v>3.935</v>
       </c>
       <c r="E24">
-        <v>3.964</v>
+        <v>3.962</v>
       </c>
       <c r="F24">
         <v>3.957</v>
@@ -1289,7 +1289,7 @@
         <v>3.873</v>
       </c>
       <c r="G25">
-        <v>3.953</v>
+        <v>3.952</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1312,7 +1312,7 @@
         <v>3.869</v>
       </c>
       <c r="G26">
-        <v>3.951</v>
+        <v>3.95</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1329,13 +1329,13 @@
         <v>4</v>
       </c>
       <c r="E27">
-        <v>3.957</v>
+        <v>3.955</v>
       </c>
       <c r="F27">
         <v>3.895</v>
       </c>
       <c r="G27">
-        <v>3.946</v>
+        <v>3.945</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1358,7 +1358,7 @@
         <v>3.861</v>
       </c>
       <c r="G28">
-        <v>3.944</v>
+        <v>3.943</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1381,7 +1381,7 @@
         <v>3.884</v>
       </c>
       <c r="G29">
-        <v>3.944</v>
+        <v>3.943</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1404,7 +1404,7 @@
         <v>3.895</v>
       </c>
       <c r="G30">
-        <v>3.941</v>
+        <v>3.94</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1412,7 +1412,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>230051</v>
+        <v>230197</v>
       </c>
       <c r="C31" t="s">
         <v>36</v>
@@ -1421,10 +1421,10 @@
         <v>4</v>
       </c>
       <c r="E31">
-        <v>4</v>
+        <v>3.937</v>
       </c>
       <c r="F31">
-        <v>3.83</v>
+        <v>3.899</v>
       </c>
       <c r="G31">
         <v>3.937</v>
@@ -1435,7 +1435,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>230197</v>
+        <v>230051</v>
       </c>
       <c r="C32" t="s">
         <v>37</v>
@@ -1444,13 +1444,13 @@
         <v>4</v>
       </c>
       <c r="E32">
-        <v>3.928</v>
+        <v>4</v>
       </c>
       <c r="F32">
-        <v>3.899</v>
+        <v>3.83</v>
       </c>
       <c r="G32">
-        <v>3.933</v>
+        <v>3.936</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1473,7 +1473,7 @@
         <v>3.79</v>
       </c>
       <c r="G33">
-        <v>3.932</v>
+        <v>3.931</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1490,13 +1490,13 @@
         <v>3.935</v>
       </c>
       <c r="E34">
-        <v>3.964</v>
+        <v>3.962</v>
       </c>
       <c r="F34">
         <v>3.873</v>
       </c>
       <c r="G34">
-        <v>3.924</v>
+        <v>3.922</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1519,7 +1519,7 @@
         <v>3.791</v>
       </c>
       <c r="G35">
-        <v>3.922</v>
+        <v>3.921</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1536,13 +1536,13 @@
         <v>3.957</v>
       </c>
       <c r="E36">
-        <v>3.964</v>
+        <v>3.962</v>
       </c>
       <c r="F36">
         <v>3.847</v>
       </c>
       <c r="G36">
-        <v>3.919</v>
+        <v>3.918</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1559,13 +1559,13 @@
         <v>4</v>
       </c>
       <c r="E37">
-        <v>3.916</v>
+        <v>3.912</v>
       </c>
       <c r="F37">
         <v>3.862</v>
       </c>
       <c r="G37">
-        <v>3.914</v>
+        <v>3.912</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1582,13 +1582,13 @@
         <v>4</v>
       </c>
       <c r="E38">
-        <v>3.94</v>
+        <v>3.937</v>
       </c>
       <c r="F38">
         <v>3.83</v>
       </c>
       <c r="G38">
-        <v>3.912</v>
+        <v>3.911</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1596,7 +1596,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>230100</v>
+        <v>230417</v>
       </c>
       <c r="C39" t="s">
         <v>44</v>
@@ -1605,13 +1605,13 @@
         <v>4</v>
       </c>
       <c r="E39">
-        <v>4</v>
+        <v>3.941</v>
       </c>
       <c r="F39">
-        <v>3.721</v>
+        <v>3.804</v>
       </c>
       <c r="G39">
-        <v>3.896</v>
+        <v>3.903</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1619,7 +1619,7 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>230724</v>
+        <v>230100</v>
       </c>
       <c r="C40" t="s">
         <v>45</v>
@@ -1628,10 +1628,10 @@
         <v>4</v>
       </c>
       <c r="E40">
-        <v>3.88</v>
+        <v>4</v>
       </c>
       <c r="F40">
-        <v>3.847</v>
+        <v>3.721</v>
       </c>
       <c r="G40">
         <v>3.895</v>
@@ -1642,7 +1642,7 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>230417</v>
+        <v>230724</v>
       </c>
       <c r="C41" t="s">
         <v>46</v>
@@ -1651,10 +1651,10 @@
         <v>4</v>
       </c>
       <c r="E41">
-        <v>3.916</v>
+        <v>3.875</v>
       </c>
       <c r="F41">
-        <v>3.804</v>
+        <v>3.847</v>
       </c>
       <c r="G41">
         <v>3.893</v>
@@ -1680,7 +1680,7 @@
         <v>3.691</v>
       </c>
       <c r="G42">
-        <v>3.885</v>
+        <v>3.883</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1697,13 +1697,13 @@
         <v>4</v>
       </c>
       <c r="E43">
-        <v>3.964</v>
+        <v>3.962</v>
       </c>
       <c r="F43">
         <v>3.714</v>
       </c>
       <c r="G43">
-        <v>3.885</v>
+        <v>3.883</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -1711,22 +1711,22 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>230321</v>
+        <v>230212</v>
       </c>
       <c r="C44" t="s">
         <v>49</v>
       </c>
       <c r="D44">
-        <v>4</v>
+        <v>3.957</v>
       </c>
       <c r="E44">
-        <v>3.952</v>
+        <v>3.887</v>
       </c>
       <c r="F44">
-        <v>3.73</v>
+        <v>3.821</v>
       </c>
       <c r="G44">
-        <v>3.88</v>
+        <v>3.878</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1734,22 +1734,22 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>230300</v>
+        <v>230321</v>
       </c>
       <c r="C45" t="s">
         <v>50</v>
       </c>
       <c r="D45">
-        <v>3.935</v>
+        <v>4</v>
       </c>
       <c r="E45">
-        <v>4</v>
+        <v>3.949</v>
       </c>
       <c r="F45">
-        <v>3.713</v>
+        <v>3.73</v>
       </c>
       <c r="G45">
-        <v>3.879</v>
+        <v>3.878</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -1757,7 +1757,7 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>230145</v>
+        <v>230300</v>
       </c>
       <c r="C46" t="s">
         <v>51</v>
@@ -1769,10 +1769,10 @@
         <v>4</v>
       </c>
       <c r="F46">
-        <v>3.704</v>
+        <v>3.713</v>
       </c>
       <c r="G46">
-        <v>3.875</v>
+        <v>3.877</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -1780,22 +1780,22 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>230212</v>
+        <v>230145</v>
       </c>
       <c r="C47" t="s">
         <v>52</v>
       </c>
       <c r="D47">
-        <v>3.957</v>
+        <v>3.935</v>
       </c>
       <c r="E47">
-        <v>3.88</v>
+        <v>4</v>
       </c>
       <c r="F47">
-        <v>3.821</v>
+        <v>3.704</v>
       </c>
       <c r="G47">
-        <v>3.875</v>
+        <v>3.873</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -1812,13 +1812,13 @@
         <v>3.935</v>
       </c>
       <c r="E48">
-        <v>3.832</v>
+        <v>3.825</v>
       </c>
       <c r="F48">
         <v>3.873</v>
       </c>
       <c r="G48">
-        <v>3.87</v>
+        <v>3.868</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -1835,13 +1835,13 @@
         <v>4</v>
       </c>
       <c r="E49">
-        <v>3.952</v>
+        <v>3.949</v>
       </c>
       <c r="F49">
         <v>3.699</v>
       </c>
       <c r="G49">
-        <v>3.869</v>
+        <v>3.867</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -1849,22 +1849,22 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>230697</v>
+        <v>230058</v>
       </c>
       <c r="C50" t="s">
         <v>55</v>
       </c>
       <c r="D50">
-        <v>3.957</v>
+        <v>4</v>
       </c>
       <c r="E50">
-        <v>3.964</v>
+        <v>3.912</v>
       </c>
       <c r="F50">
-        <v>3.671</v>
+        <v>3.713</v>
       </c>
       <c r="G50">
-        <v>3.86</v>
+        <v>3.857</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -1872,22 +1872,22 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>230058</v>
+        <v>230697</v>
       </c>
       <c r="C51" t="s">
         <v>56</v>
       </c>
       <c r="D51">
-        <v>4</v>
+        <v>3.957</v>
       </c>
       <c r="E51">
-        <v>3.916</v>
+        <v>3.962</v>
       </c>
       <c r="F51">
-        <v>3.713</v>
+        <v>3.671</v>
       </c>
       <c r="G51">
-        <v>3.859</v>
+        <v>3.857</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -1895,7 +1895,7 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>230045</v>
+        <v>230211</v>
       </c>
       <c r="C52" t="s">
         <v>57</v>
@@ -1904,13 +1904,13 @@
         <v>4</v>
       </c>
       <c r="E52">
-        <v>3.916</v>
+        <v>3.9</v>
       </c>
       <c r="F52">
-        <v>3.704</v>
+        <v>3.721</v>
       </c>
       <c r="G52">
-        <v>3.856</v>
+        <v>3.855</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -1918,22 +1918,22 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>230539</v>
+        <v>230045</v>
       </c>
       <c r="C53" t="s">
         <v>58</v>
       </c>
       <c r="D53">
-        <v>3.935</v>
+        <v>4</v>
       </c>
       <c r="E53">
-        <v>4</v>
+        <v>3.912</v>
       </c>
       <c r="F53">
-        <v>3.652</v>
+        <v>3.704</v>
       </c>
       <c r="G53">
-        <v>3.856</v>
+        <v>3.854</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -1941,22 +1941,22 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>230211</v>
+        <v>230539</v>
       </c>
       <c r="C54" t="s">
         <v>59</v>
       </c>
       <c r="D54">
-        <v>4</v>
+        <v>3.935</v>
       </c>
       <c r="E54">
-        <v>3.892</v>
+        <v>4</v>
       </c>
       <c r="F54">
-        <v>3.721</v>
+        <v>3.652</v>
       </c>
       <c r="G54">
-        <v>3.853</v>
+        <v>3.854</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -1973,13 +1973,13 @@
         <v>3.857</v>
       </c>
       <c r="E55">
-        <v>3.88</v>
+        <v>3.875</v>
       </c>
       <c r="F55">
         <v>3.804</v>
       </c>
       <c r="G55">
-        <v>3.846</v>
+        <v>3.844</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -1996,13 +1996,13 @@
         <v>3.935</v>
       </c>
       <c r="E56">
-        <v>3.916</v>
+        <v>3.912</v>
       </c>
       <c r="F56">
         <v>3.69</v>
       </c>
       <c r="G56">
-        <v>3.841</v>
+        <v>3.838</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -2019,13 +2019,13 @@
         <v>3.957</v>
       </c>
       <c r="E57">
-        <v>3.916</v>
+        <v>3.912</v>
       </c>
       <c r="F57">
         <v>3.678</v>
       </c>
       <c r="G57">
-        <v>3.837</v>
+        <v>3.834</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -2042,13 +2042,13 @@
         <v>3.935</v>
       </c>
       <c r="E58">
-        <v>3.832</v>
+        <v>3.825</v>
       </c>
       <c r="F58">
         <v>3.778</v>
       </c>
       <c r="G58">
-        <v>3.835</v>
+        <v>3.832</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -2065,13 +2065,13 @@
         <v>3.957</v>
       </c>
       <c r="E59">
-        <v>3.916</v>
+        <v>3.912</v>
       </c>
       <c r="F59">
         <v>3.673</v>
       </c>
       <c r="G59">
-        <v>3.835</v>
+        <v>3.832</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -2088,13 +2088,13 @@
         <v>3.935</v>
       </c>
       <c r="E60">
-        <v>3.817</v>
+        <v>3.811</v>
       </c>
       <c r="F60">
         <v>3.78</v>
       </c>
       <c r="G60">
-        <v>3.832</v>
+        <v>3.829</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -2111,13 +2111,13 @@
         <v>4</v>
       </c>
       <c r="E61">
-        <v>3.952</v>
+        <v>3.949</v>
       </c>
       <c r="F61">
         <v>3.586</v>
       </c>
       <c r="G61">
-        <v>3.827</v>
+        <v>3.824</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -2140,7 +2140,7 @@
         <v>3.526</v>
       </c>
       <c r="G62">
-        <v>3.824</v>
+        <v>3.821</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -2157,13 +2157,13 @@
         <v>3.9</v>
       </c>
       <c r="E63">
-        <v>3.964</v>
+        <v>3.962</v>
       </c>
       <c r="F63">
         <v>3.613</v>
       </c>
       <c r="G63">
-        <v>3.819</v>
+        <v>3.816</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -2186,7 +2186,7 @@
         <v>3.5</v>
       </c>
       <c r="G64">
-        <v>3.814</v>
+        <v>3.811</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -2203,13 +2203,13 @@
         <v>4</v>
       </c>
       <c r="E65">
-        <v>3.916</v>
+        <v>3.912</v>
       </c>
       <c r="F65">
         <v>3.56</v>
       </c>
       <c r="G65">
-        <v>3.803</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -2226,13 +2226,13 @@
         <v>3.957</v>
       </c>
       <c r="E66">
-        <v>3.88</v>
+        <v>3.875</v>
       </c>
       <c r="F66">
         <v>3.626</v>
       </c>
       <c r="G66">
-        <v>3.803</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -2249,13 +2249,13 @@
         <v>3.935</v>
       </c>
       <c r="E67">
-        <v>3.964</v>
+        <v>3.962</v>
       </c>
       <c r="F67">
         <v>3.543</v>
       </c>
       <c r="G67">
-        <v>3.801</v>
+        <v>3.798</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -2272,13 +2272,13 @@
         <v>3.892</v>
       </c>
       <c r="E68">
-        <v>3.88</v>
+        <v>3.875</v>
       </c>
       <c r="F68">
         <v>3.66</v>
       </c>
       <c r="G68">
-        <v>3.801</v>
+        <v>3.798</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -2295,13 +2295,13 @@
         <v>3.857</v>
       </c>
       <c r="E69">
-        <v>3.882</v>
+        <v>3.877</v>
       </c>
       <c r="F69">
         <v>3.645</v>
       </c>
       <c r="G69">
-        <v>3.8</v>
+        <v>3.796</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -2318,13 +2318,13 @@
         <v>3.957</v>
       </c>
       <c r="E70">
-        <v>3.824</v>
+        <v>3.816</v>
       </c>
       <c r="F70">
         <v>3.665</v>
       </c>
       <c r="G70">
-        <v>3.795</v>
+        <v>3.791</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -2341,13 +2341,13 @@
         <v>4</v>
       </c>
       <c r="E71">
-        <v>3.914</v>
+        <v>3.911</v>
       </c>
       <c r="F71">
         <v>3.479</v>
       </c>
       <c r="G71">
-        <v>3.793</v>
+        <v>3.79</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -2364,13 +2364,13 @@
         <v>3.957</v>
       </c>
       <c r="E72">
-        <v>3.796</v>
+        <v>3.8</v>
       </c>
       <c r="F72">
         <v>3.678</v>
       </c>
       <c r="G72">
-        <v>3.788</v>
+        <v>3.79</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -2393,7 +2393,7 @@
         <v>3.385</v>
       </c>
       <c r="G73">
-        <v>3.784</v>
+        <v>3.781</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -2410,13 +2410,13 @@
         <v>3.935</v>
       </c>
       <c r="E74">
-        <v>3.952</v>
+        <v>3.949</v>
       </c>
       <c r="F74">
         <v>3.495</v>
       </c>
       <c r="G74">
-        <v>3.779</v>
+        <v>3.775</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -2433,13 +2433,13 @@
         <v>3.935</v>
       </c>
       <c r="E75">
-        <v>3.852</v>
+        <v>3.845</v>
       </c>
       <c r="F75">
         <v>3.591</v>
       </c>
       <c r="G75">
-        <v>3.774</v>
+        <v>3.77</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -2456,13 +2456,13 @@
         <v>3.75</v>
       </c>
       <c r="E76">
-        <v>3.85</v>
+        <v>3.844</v>
       </c>
       <c r="F76">
         <v>3.63</v>
       </c>
       <c r="G76">
-        <v>3.756</v>
+        <v>3.752</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -2479,13 +2479,13 @@
         <v>3.785</v>
       </c>
       <c r="E77">
-        <v>3.892</v>
+        <v>3.888</v>
       </c>
       <c r="F77">
         <v>3.54</v>
       </c>
       <c r="G77">
-        <v>3.754</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -2502,13 +2502,13 @@
         <v>3.85</v>
       </c>
       <c r="E78">
-        <v>3.683</v>
+        <v>3.67</v>
       </c>
       <c r="F78">
         <v>3.765</v>
       </c>
       <c r="G78">
-        <v>3.751</v>
+        <v>3.747</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -2525,13 +2525,13 @@
         <v>3.9</v>
       </c>
       <c r="E79">
-        <v>3.952</v>
+        <v>3.949</v>
       </c>
       <c r="F79">
         <v>3.441</v>
       </c>
       <c r="G79">
-        <v>3.746</v>
+        <v>3.741</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -2548,13 +2548,13 @@
         <v>3.892</v>
       </c>
       <c r="E80">
-        <v>3.916</v>
+        <v>3.912</v>
       </c>
       <c r="F80">
         <v>3.443</v>
       </c>
       <c r="G80">
-        <v>3.735</v>
+        <v>3.731</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -2571,13 +2571,13 @@
         <v>3.914</v>
       </c>
       <c r="E81">
-        <v>3.796</v>
+        <v>3.787</v>
       </c>
       <c r="F81">
         <v>3.558</v>
       </c>
       <c r="G81">
-        <v>3.731</v>
+        <v>3.727</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -2594,13 +2594,13 @@
         <v>3.892</v>
       </c>
       <c r="E82">
-        <v>3.832</v>
+        <v>3.825</v>
       </c>
       <c r="F82">
         <v>3.508</v>
       </c>
       <c r="G82">
-        <v>3.725</v>
+        <v>3.721</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -2617,13 +2617,13 @@
         <v>3.785</v>
       </c>
       <c r="E83">
-        <v>3.753</v>
+        <v>3.744</v>
       </c>
       <c r="F83">
         <v>3.619</v>
       </c>
       <c r="G83">
-        <v>3.715</v>
+        <v>3.711</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -2631,22 +2631,22 @@
         <v>83</v>
       </c>
       <c r="B84">
-        <v>230444</v>
+        <v>230407</v>
       </c>
       <c r="C84" t="s">
         <v>89</v>
       </c>
       <c r="D84">
-        <v>3.785</v>
+        <v>4</v>
       </c>
       <c r="E84">
-        <v>3.625</v>
+        <v>3.766</v>
       </c>
       <c r="F84">
-        <v>3.757</v>
+        <v>3.469</v>
       </c>
       <c r="G84">
-        <v>3.704</v>
+        <v>3.708</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -2654,22 +2654,22 @@
         <v>84</v>
       </c>
       <c r="B85">
-        <v>230375</v>
+        <v>230444</v>
       </c>
       <c r="C85" t="s">
         <v>90</v>
       </c>
       <c r="D85">
-        <v>3.85</v>
+        <v>3.785</v>
       </c>
       <c r="E85">
-        <v>3.712</v>
+        <v>3.622</v>
       </c>
       <c r="F85">
-        <v>3.599</v>
+        <v>3.757</v>
       </c>
       <c r="G85">
-        <v>3.701</v>
+        <v>3.704</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -2677,22 +2677,22 @@
         <v>85</v>
       </c>
       <c r="B86">
-        <v>230407</v>
+        <v>230375</v>
       </c>
       <c r="C86" t="s">
         <v>91</v>
       </c>
       <c r="D86">
-        <v>4</v>
+        <v>3.85</v>
       </c>
       <c r="E86">
-        <v>3.747</v>
+        <v>3.7</v>
       </c>
       <c r="F86">
-        <v>3.469</v>
+        <v>3.599</v>
       </c>
       <c r="G86">
-        <v>3.701</v>
+        <v>3.696</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -2709,13 +2709,13 @@
         <v>4</v>
       </c>
       <c r="E87">
-        <v>3.844</v>
+        <v>3.837</v>
       </c>
       <c r="F87">
         <v>3.339</v>
       </c>
       <c r="G87">
-        <v>3.691</v>
+        <v>3.686</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -2732,13 +2732,13 @@
         <v>4</v>
       </c>
       <c r="E88">
-        <v>3.768</v>
+        <v>3.758</v>
       </c>
       <c r="F88">
         <v>3.424</v>
       </c>
       <c r="G88">
-        <v>3.688</v>
+        <v>3.683</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -2755,13 +2755,13 @@
         <v>3.85</v>
       </c>
       <c r="E89">
-        <v>3.647</v>
+        <v>3.633</v>
       </c>
       <c r="F89">
         <v>3.638</v>
       </c>
       <c r="G89">
-        <v>3.687</v>
+        <v>3.682</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -2778,13 +2778,13 @@
         <v>3.85</v>
       </c>
       <c r="E90">
-        <v>3.844</v>
+        <v>3.837</v>
       </c>
       <c r="F90">
         <v>3.417</v>
       </c>
       <c r="G90">
-        <v>3.687</v>
+        <v>3.681</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -2801,13 +2801,13 @@
         <v>3.957</v>
       </c>
       <c r="E91">
-        <v>3.736</v>
+        <v>3.725</v>
       </c>
       <c r="F91">
         <v>3.465</v>
       </c>
       <c r="G91">
-        <v>3.685</v>
+        <v>3.68</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -2824,13 +2824,13 @@
         <v>3.935</v>
       </c>
       <c r="E92">
-        <v>3.804</v>
+        <v>3.795</v>
       </c>
       <c r="F92">
         <v>3.399</v>
       </c>
       <c r="G92">
-        <v>3.683</v>
+        <v>3.678</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -2847,13 +2847,13 @@
         <v>3.935</v>
       </c>
       <c r="E93">
-        <v>3.663</v>
+        <v>3.65</v>
       </c>
       <c r="F93">
         <v>3.543</v>
       </c>
       <c r="G93">
-        <v>3.68</v>
+        <v>3.675</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -2870,13 +2870,13 @@
         <v>3.892</v>
       </c>
       <c r="E94">
-        <v>3.844</v>
+        <v>3.837</v>
       </c>
       <c r="F94">
         <v>3.347</v>
       </c>
       <c r="G94">
-        <v>3.67</v>
+        <v>3.665</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -2893,13 +2893,13 @@
         <v>3.85</v>
       </c>
       <c r="E95">
-        <v>3.784</v>
+        <v>3.775</v>
       </c>
       <c r="F95">
         <v>3.4</v>
       </c>
       <c r="G95">
-        <v>3.665</v>
+        <v>3.659</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -2916,13 +2916,13 @@
         <v>4</v>
       </c>
       <c r="E96">
-        <v>3.732</v>
+        <v>3.72</v>
       </c>
       <c r="F96">
         <v>3.373</v>
       </c>
       <c r="G96">
-        <v>3.659</v>
+        <v>3.654</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -2939,13 +2939,13 @@
         <v>4</v>
       </c>
       <c r="E97">
-        <v>3.636</v>
+        <v>3.633</v>
       </c>
       <c r="F97">
         <v>3.46</v>
       </c>
       <c r="G97">
-        <v>3.653</v>
+        <v>3.652</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -2962,13 +2962,13 @@
         <v>3.957</v>
       </c>
       <c r="E98">
-        <v>3.696</v>
+        <v>3.695</v>
       </c>
       <c r="F98">
         <v>3.404</v>
       </c>
       <c r="G98">
-        <v>3.646</v>
+        <v>3.645</v>
       </c>
     </row>
     <row r="99" spans="1:7">
@@ -2985,13 +2985,13 @@
         <v>3.892</v>
       </c>
       <c r="E99">
-        <v>3.747</v>
+        <v>3.737</v>
       </c>
       <c r="F99">
         <v>3.304</v>
       </c>
       <c r="G99">
-        <v>3.616</v>
+        <v>3.609</v>
       </c>
     </row>
     <row r="100" spans="1:7">
@@ -3008,13 +3008,13 @@
         <v>3.85</v>
       </c>
       <c r="E100">
-        <v>3.916</v>
+        <v>3.912</v>
       </c>
       <c r="F100">
         <v>3.13</v>
       </c>
       <c r="G100">
-        <v>3.609</v>
+        <v>3.603</v>
       </c>
     </row>
     <row r="101" spans="1:7">
@@ -3031,13 +3031,13 @@
         <v>3.85</v>
       </c>
       <c r="E101">
-        <v>3.683</v>
+        <v>3.67</v>
       </c>
       <c r="F101">
         <v>3.334</v>
       </c>
       <c r="G101">
-        <v>3.591</v>
+        <v>3.585</v>
       </c>
     </row>
     <row r="102" spans="1:7">
@@ -3054,13 +3054,13 @@
         <v>3.85</v>
       </c>
       <c r="E102">
-        <v>3.567</v>
+        <v>3.551</v>
       </c>
       <c r="F102">
         <v>3.447</v>
       </c>
       <c r="G102">
-        <v>3.59</v>
+        <v>3.583</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -3077,13 +3077,13 @@
         <v>4</v>
       </c>
       <c r="E103">
-        <v>3.868</v>
+        <v>3.862</v>
       </c>
       <c r="F103">
         <v>3.004</v>
       </c>
       <c r="G103">
-        <v>3.577</v>
+        <v>3.57</v>
       </c>
     </row>
     <row r="104" spans="1:7">
@@ -3100,13 +3100,13 @@
         <v>3.85</v>
       </c>
       <c r="E104">
-        <v>3.635</v>
+        <v>3.62</v>
       </c>
       <c r="F104">
         <v>3.347</v>
       </c>
       <c r="G104">
-        <v>3.577</v>
+        <v>3.57</v>
       </c>
     </row>
     <row r="105" spans="1:7">
@@ -3123,13 +3123,13 @@
         <v>3.892</v>
       </c>
       <c r="E105">
-        <v>3.612</v>
+        <v>3.595</v>
       </c>
       <c r="F105">
         <v>3.278</v>
       </c>
       <c r="G105">
-        <v>3.551</v>
+        <v>3.544</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -3146,13 +3146,13 @@
         <v>3.85</v>
       </c>
       <c r="E106">
-        <v>3.747</v>
+        <v>3.737</v>
       </c>
       <c r="F106">
         <v>3.039</v>
       </c>
       <c r="G106">
-        <v>3.508</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="107" spans="1:7">
@@ -3169,13 +3169,13 @@
         <v>3.85</v>
       </c>
       <c r="E107">
-        <v>3.528</v>
+        <v>3.508</v>
       </c>
       <c r="F107">
         <v>3.221</v>
       </c>
       <c r="G107">
-        <v>3.487</v>
+        <v>3.478</v>
       </c>
     </row>
     <row r="108" spans="1:7">
@@ -3192,13 +3192,13 @@
         <v>3.85</v>
       </c>
       <c r="E108">
-        <v>3.62</v>
+        <v>3.604</v>
       </c>
       <c r="F108">
         <v>3.095</v>
       </c>
       <c r="G108">
-        <v>3.477</v>
+        <v>3.468</v>
       </c>
     </row>
     <row r="109" spans="1:7">
@@ -3215,13 +3215,13 @@
         <v>3.792</v>
       </c>
       <c r="E109">
-        <v>3.642</v>
+        <v>3.629</v>
       </c>
       <c r="F109">
         <v>3.014</v>
       </c>
       <c r="G109">
-        <v>3.474</v>
+        <v>3.465</v>
       </c>
     </row>
     <row r="110" spans="1:7">
@@ -3238,13 +3238,13 @@
         <v>3.871</v>
       </c>
       <c r="E110">
-        <v>3.468</v>
+        <v>3.445</v>
       </c>
       <c r="F110">
         <v>3.221</v>
       </c>
       <c r="G110">
-        <v>3.467</v>
+        <v>3.459</v>
       </c>
     </row>
     <row r="111" spans="1:7">
@@ -3261,13 +3261,13 @@
         <v>3.764</v>
       </c>
       <c r="E111">
-        <v>3.478</v>
+        <v>3.459</v>
       </c>
       <c r="F111">
         <v>3.214</v>
       </c>
       <c r="G111">
-        <v>3.453</v>
+        <v>3.445</v>
       </c>
     </row>
     <row r="112" spans="1:7">
@@ -3284,13 +3284,13 @@
         <v>3.935</v>
       </c>
       <c r="E112">
-        <v>3.132</v>
+        <v>3.095</v>
       </c>
       <c r="F112">
         <v>3.334</v>
       </c>
       <c r="G112">
-        <v>3.388</v>
+        <v>3.378</v>
       </c>
     </row>
     <row r="113" spans="1:7">
@@ -3307,13 +3307,13 @@
         <v>3.85</v>
       </c>
       <c r="E113">
-        <v>3.487</v>
+        <v>3.479</v>
       </c>
       <c r="F113">
         <v>2.785</v>
       </c>
       <c r="G113">
-        <v>3.326</v>
+        <v>3.32</v>
       </c>
     </row>
     <row r="114" spans="1:7">
@@ -3330,13 +3330,13 @@
         <v>3.807</v>
       </c>
       <c r="E114">
-        <v>3.317</v>
+        <v>3.292</v>
       </c>
       <c r="F114">
         <v>2.835</v>
       </c>
       <c r="G114">
-        <v>3.272</v>
+        <v>3.26</v>
       </c>
     </row>
     <row r="115" spans="1:7">
@@ -3353,13 +3353,13 @@
         <v>4</v>
       </c>
       <c r="E115">
-        <v>3.656</v>
+        <v>3.641</v>
       </c>
       <c r="F115">
         <v>2.343</v>
       </c>
       <c r="G115">
-        <v>3.246</v>
+        <v>3.234</v>
       </c>
     </row>
     <row r="116" spans="1:7">
@@ -3376,13 +3376,13 @@
         <v>4</v>
       </c>
       <c r="E116">
-        <v>3.536</v>
+        <v>3.516</v>
       </c>
       <c r="F116">
         <v>2.404</v>
       </c>
       <c r="G116">
-        <v>3.22</v>
+        <v>3.208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SGPA calc test commit
</commit_message>
<xml_diff>
--- a/output/CGPA_Results.xlsx
+++ b/output/CGPA_Results.xlsx
@@ -91,12 +91,12 @@
     <t>KUMARASINGHE M.N.</t>
   </si>
   <si>
+    <t>DE MEL D.J.</t>
+  </si>
+  <si>
     <t>PEIRIS E.A.S.S.</t>
   </si>
   <si>
-    <t>DE MEL D.J.</t>
-  </si>
-  <si>
     <t>RAHUL B.</t>
   </si>
   <si>
@@ -232,21 +232,21 @@
     <t>DISSANAYAKE R.K.T.</t>
   </si>
   <si>
+    <t>RAHMAN M.F.A.</t>
+  </si>
+  <si>
     <t>SARUKA U.</t>
   </si>
   <si>
     <t>WIJESINGHE U.G.S.K.D.</t>
   </si>
   <si>
-    <t>RAHMAN M.F.A.</t>
+    <t>ABISHEK L.</t>
   </si>
   <si>
     <t>BALASOORIYA B.R.B.D.</t>
   </si>
   <si>
-    <t>ABISHEK L.</t>
-  </si>
-  <si>
     <t>GAMAGE SK</t>
   </si>
   <si>
@@ -334,12 +334,12 @@
     <t>JAYASINGHE J.A.P.R.</t>
   </si>
   <si>
+    <t>IMBULPITIYA B.N.</t>
+  </si>
+  <si>
     <t>MANATUNGA K.D.</t>
   </si>
   <si>
-    <t>IMBULPITIYA B.N.</t>
-  </si>
-  <si>
     <t>AHAMED A.M.S.</t>
   </si>
   <si>
@@ -355,10 +355,10 @@
     <t>HAKAM M.R.A.</t>
   </si>
   <si>
+    <t>SANTHOSH S.</t>
+  </si>
+  <si>
     <t>JAYAKODY J.A.C.P.</t>
-  </si>
-  <si>
-    <t>SANTHOSH S.</t>
   </si>
   <si>
     <t>SAMARASEKARA S.M.R.P.</t>
@@ -823,7 +823,7 @@
         <v>4</v>
       </c>
       <c r="E5">
-        <v>3.975</v>
+        <v>3.973</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -1059,7 +1059,7 @@
         <v>3.96</v>
       </c>
       <c r="G15">
-        <v>3.97</v>
+        <v>3.969</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1082,7 +1082,7 @@
         <v>3.921</v>
       </c>
       <c r="G16">
-        <v>3.97</v>
+        <v>3.969</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1128,7 +1128,7 @@
         <v>3.9</v>
       </c>
       <c r="G18">
-        <v>3.964</v>
+        <v>3.963</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1151,7 +1151,7 @@
         <v>3.9</v>
       </c>
       <c r="G19">
-        <v>3.962</v>
+        <v>3.961</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1159,22 +1159,22 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>230469</v>
+        <v>230121</v>
       </c>
       <c r="C20" t="s">
         <v>25</v>
       </c>
       <c r="D20">
-        <v>4</v>
+        <v>3.957</v>
       </c>
       <c r="E20">
-        <v>3.962</v>
+        <v>4</v>
       </c>
       <c r="F20">
-        <v>3.937</v>
+        <v>3.921</v>
       </c>
       <c r="G20">
-        <v>3.961</v>
+        <v>3.96</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1182,19 +1182,19 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>230121</v>
+        <v>230469</v>
       </c>
       <c r="C21" t="s">
         <v>26</v>
       </c>
       <c r="D21">
-        <v>3.957</v>
+        <v>4</v>
       </c>
       <c r="E21">
-        <v>4</v>
+        <v>3.96</v>
       </c>
       <c r="F21">
-        <v>3.921</v>
+        <v>3.937</v>
       </c>
       <c r="G21">
         <v>3.96</v>
@@ -1237,13 +1237,13 @@
         <v>4</v>
       </c>
       <c r="E23">
-        <v>3.924</v>
+        <v>3.921</v>
       </c>
       <c r="F23">
         <v>3.957</v>
       </c>
       <c r="G23">
-        <v>3.954</v>
+        <v>3.953</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1260,13 +1260,13 @@
         <v>3.935</v>
       </c>
       <c r="E24">
-        <v>3.962</v>
+        <v>3.96</v>
       </c>
       <c r="F24">
         <v>3.957</v>
       </c>
       <c r="G24">
-        <v>3.954</v>
+        <v>3.953</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1289,7 +1289,7 @@
         <v>3.873</v>
       </c>
       <c r="G25">
-        <v>3.952</v>
+        <v>3.951</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1358,7 +1358,7 @@
         <v>3.861</v>
       </c>
       <c r="G28">
-        <v>3.943</v>
+        <v>3.942</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1381,7 +1381,7 @@
         <v>3.884</v>
       </c>
       <c r="G29">
-        <v>3.943</v>
+        <v>3.942</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1421,13 +1421,13 @@
         <v>4</v>
       </c>
       <c r="E31">
-        <v>3.937</v>
+        <v>3.934</v>
       </c>
       <c r="F31">
         <v>3.899</v>
       </c>
       <c r="G31">
-        <v>3.937</v>
+        <v>3.936</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1450,7 +1450,7 @@
         <v>3.83</v>
       </c>
       <c r="G32">
-        <v>3.936</v>
+        <v>3.935</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1490,13 +1490,13 @@
         <v>3.935</v>
       </c>
       <c r="E34">
-        <v>3.962</v>
+        <v>3.96</v>
       </c>
       <c r="F34">
         <v>3.873</v>
       </c>
       <c r="G34">
-        <v>3.922</v>
+        <v>3.921</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1519,7 +1519,7 @@
         <v>3.791</v>
       </c>
       <c r="G35">
-        <v>3.921</v>
+        <v>3.92</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1536,13 +1536,13 @@
         <v>3.957</v>
       </c>
       <c r="E36">
-        <v>3.962</v>
+        <v>3.96</v>
       </c>
       <c r="F36">
         <v>3.847</v>
       </c>
       <c r="G36">
-        <v>3.918</v>
+        <v>3.916</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1559,13 +1559,13 @@
         <v>4</v>
       </c>
       <c r="E37">
-        <v>3.912</v>
+        <v>3.908</v>
       </c>
       <c r="F37">
         <v>3.862</v>
       </c>
       <c r="G37">
-        <v>3.912</v>
+        <v>3.911</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1582,13 +1582,13 @@
         <v>4</v>
       </c>
       <c r="E38">
-        <v>3.937</v>
+        <v>3.934</v>
       </c>
       <c r="F38">
         <v>3.83</v>
       </c>
       <c r="G38">
-        <v>3.911</v>
+        <v>3.909</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1605,13 +1605,13 @@
         <v>4</v>
       </c>
       <c r="E39">
-        <v>3.941</v>
+        <v>3.939</v>
       </c>
       <c r="F39">
         <v>3.804</v>
       </c>
       <c r="G39">
-        <v>3.903</v>
+        <v>3.901</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1634,7 +1634,7 @@
         <v>3.721</v>
       </c>
       <c r="G40">
-        <v>3.895</v>
+        <v>3.893</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1651,13 +1651,13 @@
         <v>4</v>
       </c>
       <c r="E41">
-        <v>3.875</v>
+        <v>3.869</v>
       </c>
       <c r="F41">
         <v>3.847</v>
       </c>
       <c r="G41">
-        <v>3.893</v>
+        <v>3.891</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -1680,7 +1680,7 @@
         <v>3.691</v>
       </c>
       <c r="G42">
-        <v>3.883</v>
+        <v>3.881</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1697,13 +1697,13 @@
         <v>4</v>
       </c>
       <c r="E43">
-        <v>3.962</v>
+        <v>3.96</v>
       </c>
       <c r="F43">
         <v>3.714</v>
       </c>
       <c r="G43">
-        <v>3.883</v>
+        <v>3.881</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -1720,13 +1720,13 @@
         <v>3.957</v>
       </c>
       <c r="E44">
-        <v>3.887</v>
+        <v>3.882</v>
       </c>
       <c r="F44">
         <v>3.821</v>
       </c>
       <c r="G44">
-        <v>3.878</v>
+        <v>3.876</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1743,13 +1743,13 @@
         <v>4</v>
       </c>
       <c r="E45">
-        <v>3.949</v>
+        <v>3.947</v>
       </c>
       <c r="F45">
         <v>3.73</v>
       </c>
       <c r="G45">
-        <v>3.878</v>
+        <v>3.876</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -1772,7 +1772,7 @@
         <v>3.713</v>
       </c>
       <c r="G46">
-        <v>3.877</v>
+        <v>3.875</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -1795,7 +1795,7 @@
         <v>3.704</v>
       </c>
       <c r="G47">
-        <v>3.873</v>
+        <v>3.871</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -1812,13 +1812,13 @@
         <v>3.935</v>
       </c>
       <c r="E48">
-        <v>3.825</v>
+        <v>3.817</v>
       </c>
       <c r="F48">
         <v>3.873</v>
       </c>
       <c r="G48">
-        <v>3.868</v>
+        <v>3.866</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -1835,13 +1835,13 @@
         <v>4</v>
       </c>
       <c r="E49">
-        <v>3.949</v>
+        <v>3.947</v>
       </c>
       <c r="F49">
         <v>3.699</v>
       </c>
       <c r="G49">
-        <v>3.867</v>
+        <v>3.865</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -1858,13 +1858,13 @@
         <v>4</v>
       </c>
       <c r="E50">
-        <v>3.912</v>
+        <v>3.908</v>
       </c>
       <c r="F50">
         <v>3.713</v>
       </c>
       <c r="G50">
-        <v>3.857</v>
+        <v>3.855</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -1881,13 +1881,13 @@
         <v>3.957</v>
       </c>
       <c r="E51">
-        <v>3.962</v>
+        <v>3.96</v>
       </c>
       <c r="F51">
         <v>3.671</v>
       </c>
       <c r="G51">
-        <v>3.857</v>
+        <v>3.855</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -1904,13 +1904,13 @@
         <v>4</v>
       </c>
       <c r="E52">
-        <v>3.9</v>
+        <v>3.895</v>
       </c>
       <c r="F52">
         <v>3.721</v>
       </c>
       <c r="G52">
-        <v>3.855</v>
+        <v>3.853</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -1927,13 +1927,13 @@
         <v>4</v>
       </c>
       <c r="E53">
-        <v>3.912</v>
+        <v>3.908</v>
       </c>
       <c r="F53">
         <v>3.704</v>
       </c>
       <c r="G53">
-        <v>3.854</v>
+        <v>3.851</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -1956,7 +1956,7 @@
         <v>3.652</v>
       </c>
       <c r="G54">
-        <v>3.854</v>
+        <v>3.851</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -1973,13 +1973,13 @@
         <v>3.857</v>
       </c>
       <c r="E55">
-        <v>3.875</v>
+        <v>3.869</v>
       </c>
       <c r="F55">
         <v>3.804</v>
       </c>
       <c r="G55">
-        <v>3.844</v>
+        <v>3.841</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -1996,13 +1996,13 @@
         <v>3.935</v>
       </c>
       <c r="E56">
-        <v>3.912</v>
+        <v>3.908</v>
       </c>
       <c r="F56">
         <v>3.69</v>
       </c>
       <c r="G56">
-        <v>3.838</v>
+        <v>3.836</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -2019,13 +2019,13 @@
         <v>3.957</v>
       </c>
       <c r="E57">
-        <v>3.912</v>
+        <v>3.908</v>
       </c>
       <c r="F57">
         <v>3.678</v>
       </c>
       <c r="G57">
-        <v>3.834</v>
+        <v>3.831</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -2042,13 +2042,13 @@
         <v>3.935</v>
       </c>
       <c r="E58">
-        <v>3.825</v>
+        <v>3.817</v>
       </c>
       <c r="F58">
         <v>3.778</v>
       </c>
       <c r="G58">
-        <v>3.832</v>
+        <v>3.83</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -2065,13 +2065,13 @@
         <v>3.957</v>
       </c>
       <c r="E59">
-        <v>3.912</v>
+        <v>3.908</v>
       </c>
       <c r="F59">
         <v>3.673</v>
       </c>
       <c r="G59">
-        <v>3.832</v>
+        <v>3.83</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -2111,13 +2111,13 @@
         <v>4</v>
       </c>
       <c r="E61">
-        <v>3.949</v>
+        <v>3.947</v>
       </c>
       <c r="F61">
         <v>3.586</v>
       </c>
       <c r="G61">
-        <v>3.824</v>
+        <v>3.821</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -2140,7 +2140,7 @@
         <v>3.526</v>
       </c>
       <c r="G62">
-        <v>3.821</v>
+        <v>3.818</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -2157,13 +2157,13 @@
         <v>3.9</v>
       </c>
       <c r="E63">
-        <v>3.962</v>
+        <v>3.96</v>
       </c>
       <c r="F63">
         <v>3.613</v>
       </c>
       <c r="G63">
-        <v>3.816</v>
+        <v>3.813</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -2186,7 +2186,7 @@
         <v>3.5</v>
       </c>
       <c r="G64">
-        <v>3.811</v>
+        <v>3.808</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -2203,13 +2203,13 @@
         <v>4</v>
       </c>
       <c r="E65">
-        <v>3.912</v>
+        <v>3.908</v>
       </c>
       <c r="F65">
         <v>3.56</v>
       </c>
       <c r="G65">
-        <v>3.8</v>
+        <v>3.796</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -2226,13 +2226,13 @@
         <v>3.957</v>
       </c>
       <c r="E66">
-        <v>3.875</v>
+        <v>3.869</v>
       </c>
       <c r="F66">
         <v>3.626</v>
       </c>
       <c r="G66">
-        <v>3.8</v>
+        <v>3.796</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -2240,22 +2240,22 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <v>230585</v>
+        <v>230507</v>
       </c>
       <c r="C67" t="s">
         <v>72</v>
       </c>
       <c r="D67">
-        <v>3.935</v>
+        <v>3.857</v>
       </c>
       <c r="E67">
-        <v>3.962</v>
+        <v>3.877</v>
       </c>
       <c r="F67">
-        <v>3.543</v>
+        <v>3.645</v>
       </c>
       <c r="G67">
-        <v>3.798</v>
+        <v>3.796</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -2263,22 +2263,22 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <v>230726</v>
+        <v>230585</v>
       </c>
       <c r="C68" t="s">
         <v>73</v>
       </c>
       <c r="D68">
-        <v>3.892</v>
+        <v>3.935</v>
       </c>
       <c r="E68">
-        <v>3.875</v>
+        <v>3.96</v>
       </c>
       <c r="F68">
-        <v>3.66</v>
+        <v>3.543</v>
       </c>
       <c r="G68">
-        <v>3.798</v>
+        <v>3.795</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -2286,22 +2286,22 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <v>230507</v>
+        <v>230726</v>
       </c>
       <c r="C69" t="s">
         <v>74</v>
       </c>
       <c r="D69">
-        <v>3.857</v>
+        <v>3.892</v>
       </c>
       <c r="E69">
-        <v>3.877</v>
+        <v>3.869</v>
       </c>
       <c r="F69">
-        <v>3.645</v>
+        <v>3.66</v>
       </c>
       <c r="G69">
-        <v>3.796</v>
+        <v>3.795</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -2309,22 +2309,22 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <v>230070</v>
+        <v>230016</v>
       </c>
       <c r="C70" t="s">
         <v>75</v>
       </c>
       <c r="D70">
-        <v>3.957</v>
+        <v>4</v>
       </c>
       <c r="E70">
-        <v>3.816</v>
+        <v>3.911</v>
       </c>
       <c r="F70">
-        <v>3.665</v>
+        <v>3.479</v>
       </c>
       <c r="G70">
-        <v>3.791</v>
+        <v>3.79</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -2332,22 +2332,22 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>230016</v>
+        <v>230070</v>
       </c>
       <c r="C71" t="s">
         <v>76</v>
       </c>
       <c r="D71">
-        <v>4</v>
+        <v>3.957</v>
       </c>
       <c r="E71">
-        <v>3.911</v>
+        <v>3.808</v>
       </c>
       <c r="F71">
-        <v>3.479</v>
+        <v>3.665</v>
       </c>
       <c r="G71">
-        <v>3.79</v>
+        <v>3.788</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -2364,13 +2364,13 @@
         <v>3.957</v>
       </c>
       <c r="E72">
-        <v>3.8</v>
+        <v>3.791</v>
       </c>
       <c r="F72">
         <v>3.678</v>
       </c>
       <c r="G72">
-        <v>3.79</v>
+        <v>3.786</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -2393,7 +2393,7 @@
         <v>3.385</v>
       </c>
       <c r="G73">
-        <v>3.781</v>
+        <v>3.777</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -2410,13 +2410,13 @@
         <v>3.935</v>
       </c>
       <c r="E74">
-        <v>3.949</v>
+        <v>3.947</v>
       </c>
       <c r="F74">
         <v>3.495</v>
       </c>
       <c r="G74">
-        <v>3.775</v>
+        <v>3.771</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -2433,13 +2433,13 @@
         <v>3.935</v>
       </c>
       <c r="E75">
-        <v>3.845</v>
+        <v>3.839</v>
       </c>
       <c r="F75">
         <v>3.591</v>
       </c>
       <c r="G75">
-        <v>3.77</v>
+        <v>3.766</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -2502,13 +2502,13 @@
         <v>3.85</v>
       </c>
       <c r="E78">
-        <v>3.67</v>
+        <v>3.656</v>
       </c>
       <c r="F78">
         <v>3.765</v>
       </c>
       <c r="G78">
-        <v>3.747</v>
+        <v>3.743</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -2525,13 +2525,13 @@
         <v>3.9</v>
       </c>
       <c r="E79">
-        <v>3.949</v>
+        <v>3.947</v>
       </c>
       <c r="F79">
         <v>3.441</v>
       </c>
       <c r="G79">
-        <v>3.741</v>
+        <v>3.737</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -2548,13 +2548,13 @@
         <v>3.892</v>
       </c>
       <c r="E80">
-        <v>3.912</v>
+        <v>3.908</v>
       </c>
       <c r="F80">
         <v>3.443</v>
       </c>
       <c r="G80">
-        <v>3.731</v>
+        <v>3.726</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -2571,13 +2571,13 @@
         <v>3.914</v>
       </c>
       <c r="E81">
-        <v>3.787</v>
+        <v>3.778</v>
       </c>
       <c r="F81">
         <v>3.558</v>
       </c>
       <c r="G81">
-        <v>3.727</v>
+        <v>3.722</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -2594,13 +2594,13 @@
         <v>3.892</v>
       </c>
       <c r="E82">
-        <v>3.825</v>
+        <v>3.817</v>
       </c>
       <c r="F82">
         <v>3.508</v>
       </c>
       <c r="G82">
-        <v>3.721</v>
+        <v>3.716</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -2617,13 +2617,13 @@
         <v>3.785</v>
       </c>
       <c r="E83">
-        <v>3.744</v>
+        <v>3.733</v>
       </c>
       <c r="F83">
         <v>3.619</v>
       </c>
       <c r="G83">
-        <v>3.711</v>
+        <v>3.706</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -2640,13 +2640,13 @@
         <v>4</v>
       </c>
       <c r="E84">
-        <v>3.766</v>
+        <v>3.756</v>
       </c>
       <c r="F84">
         <v>3.469</v>
       </c>
       <c r="G84">
-        <v>3.708</v>
+        <v>3.703</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -2663,13 +2663,13 @@
         <v>3.785</v>
       </c>
       <c r="E85">
-        <v>3.622</v>
+        <v>3.596</v>
       </c>
       <c r="F85">
         <v>3.757</v>
       </c>
       <c r="G85">
-        <v>3.704</v>
+        <v>3.693</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -2686,13 +2686,13 @@
         <v>3.85</v>
       </c>
       <c r="E86">
-        <v>3.7</v>
+        <v>3.686</v>
       </c>
       <c r="F86">
         <v>3.599</v>
       </c>
       <c r="G86">
-        <v>3.696</v>
+        <v>3.691</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -2709,13 +2709,13 @@
         <v>4</v>
       </c>
       <c r="E87">
-        <v>3.837</v>
+        <v>3.83</v>
       </c>
       <c r="F87">
         <v>3.339</v>
       </c>
       <c r="G87">
-        <v>3.686</v>
+        <v>3.681</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -2732,13 +2732,13 @@
         <v>4</v>
       </c>
       <c r="E88">
-        <v>3.758</v>
+        <v>3.747</v>
       </c>
       <c r="F88">
         <v>3.424</v>
       </c>
       <c r="G88">
-        <v>3.683</v>
+        <v>3.678</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -2755,13 +2755,13 @@
         <v>3.85</v>
       </c>
       <c r="E89">
-        <v>3.633</v>
+        <v>3.617</v>
       </c>
       <c r="F89">
         <v>3.638</v>
       </c>
       <c r="G89">
-        <v>3.682</v>
+        <v>3.677</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -2778,13 +2778,13 @@
         <v>3.85</v>
       </c>
       <c r="E90">
-        <v>3.837</v>
+        <v>3.83</v>
       </c>
       <c r="F90">
         <v>3.417</v>
       </c>
       <c r="G90">
-        <v>3.681</v>
+        <v>3.676</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -2801,13 +2801,13 @@
         <v>3.957</v>
       </c>
       <c r="E91">
-        <v>3.725</v>
+        <v>3.713</v>
       </c>
       <c r="F91">
         <v>3.465</v>
       </c>
       <c r="G91">
-        <v>3.68</v>
+        <v>3.675</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -2824,13 +2824,13 @@
         <v>3.935</v>
       </c>
       <c r="E92">
-        <v>3.795</v>
+        <v>3.786</v>
       </c>
       <c r="F92">
         <v>3.399</v>
       </c>
       <c r="G92">
-        <v>3.678</v>
+        <v>3.673</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -2847,13 +2847,13 @@
         <v>3.935</v>
       </c>
       <c r="E93">
-        <v>3.65</v>
+        <v>3.634</v>
       </c>
       <c r="F93">
         <v>3.543</v>
       </c>
       <c r="G93">
-        <v>3.675</v>
+        <v>3.67</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -2870,13 +2870,13 @@
         <v>3.892</v>
       </c>
       <c r="E94">
-        <v>3.837</v>
+        <v>3.83</v>
       </c>
       <c r="F94">
         <v>3.347</v>
       </c>
       <c r="G94">
-        <v>3.665</v>
+        <v>3.659</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -2893,13 +2893,13 @@
         <v>3.85</v>
       </c>
       <c r="E95">
-        <v>3.775</v>
+        <v>3.765</v>
       </c>
       <c r="F95">
         <v>3.4</v>
       </c>
       <c r="G95">
-        <v>3.659</v>
+        <v>3.653</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -2916,13 +2916,13 @@
         <v>4</v>
       </c>
       <c r="E96">
-        <v>3.72</v>
+        <v>3.708</v>
       </c>
       <c r="F96">
         <v>3.373</v>
       </c>
       <c r="G96">
-        <v>3.654</v>
+        <v>3.648</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -2939,13 +2939,13 @@
         <v>4</v>
       </c>
       <c r="E97">
-        <v>3.633</v>
+        <v>3.617</v>
       </c>
       <c r="F97">
         <v>3.46</v>
       </c>
       <c r="G97">
-        <v>3.652</v>
+        <v>3.646</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -2985,13 +2985,13 @@
         <v>3.892</v>
       </c>
       <c r="E99">
-        <v>3.737</v>
+        <v>3.726</v>
       </c>
       <c r="F99">
         <v>3.304</v>
       </c>
       <c r="G99">
-        <v>3.609</v>
+        <v>3.603</v>
       </c>
     </row>
     <row r="100" spans="1:7">
@@ -3008,13 +3008,13 @@
         <v>3.85</v>
       </c>
       <c r="E100">
-        <v>3.912</v>
+        <v>3.908</v>
       </c>
       <c r="F100">
         <v>3.13</v>
       </c>
       <c r="G100">
-        <v>3.603</v>
+        <v>3.596</v>
       </c>
     </row>
     <row r="101" spans="1:7">
@@ -3022,7 +3022,7 @@
         <v>100</v>
       </c>
       <c r="B101">
-        <v>230395</v>
+        <v>230259</v>
       </c>
       <c r="C101" t="s">
         <v>106</v>
@@ -3031,13 +3031,13 @@
         <v>3.85</v>
       </c>
       <c r="E101">
-        <v>3.67</v>
+        <v>3.551</v>
       </c>
       <c r="F101">
-        <v>3.334</v>
+        <v>3.447</v>
       </c>
       <c r="G101">
-        <v>3.585</v>
+        <v>3.583</v>
       </c>
     </row>
     <row r="102" spans="1:7">
@@ -3045,7 +3045,7 @@
         <v>101</v>
       </c>
       <c r="B102">
-        <v>230259</v>
+        <v>230395</v>
       </c>
       <c r="C102" t="s">
         <v>107</v>
@@ -3054,13 +3054,13 @@
         <v>3.85</v>
       </c>
       <c r="E102">
-        <v>3.551</v>
+        <v>3.656</v>
       </c>
       <c r="F102">
-        <v>3.447</v>
+        <v>3.334</v>
       </c>
       <c r="G102">
-        <v>3.583</v>
+        <v>3.578</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -3077,13 +3077,13 @@
         <v>4</v>
       </c>
       <c r="E103">
-        <v>3.862</v>
+        <v>3.856</v>
       </c>
       <c r="F103">
         <v>3.004</v>
       </c>
       <c r="G103">
-        <v>3.57</v>
+        <v>3.563</v>
       </c>
     </row>
     <row r="104" spans="1:7">
@@ -3100,13 +3100,13 @@
         <v>3.85</v>
       </c>
       <c r="E104">
-        <v>3.62</v>
+        <v>3.604</v>
       </c>
       <c r="F104">
         <v>3.347</v>
       </c>
       <c r="G104">
-        <v>3.57</v>
+        <v>3.563</v>
       </c>
     </row>
     <row r="105" spans="1:7">
@@ -3123,13 +3123,13 @@
         <v>3.892</v>
       </c>
       <c r="E105">
-        <v>3.595</v>
+        <v>3.578</v>
       </c>
       <c r="F105">
         <v>3.278</v>
       </c>
       <c r="G105">
-        <v>3.544</v>
+        <v>3.536</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -3146,13 +3146,13 @@
         <v>3.85</v>
       </c>
       <c r="E106">
-        <v>3.737</v>
+        <v>3.726</v>
       </c>
       <c r="F106">
         <v>3.039</v>
       </c>
       <c r="G106">
-        <v>3.5</v>
+        <v>3.491</v>
       </c>
     </row>
     <row r="107" spans="1:7">
@@ -3169,13 +3169,13 @@
         <v>3.85</v>
       </c>
       <c r="E107">
-        <v>3.508</v>
+        <v>3.486</v>
       </c>
       <c r="F107">
         <v>3.221</v>
       </c>
       <c r="G107">
-        <v>3.478</v>
+        <v>3.47</v>
       </c>
     </row>
     <row r="108" spans="1:7">
@@ -3183,22 +3183,22 @@
         <v>107</v>
       </c>
       <c r="B108">
-        <v>230268</v>
+        <v>230581</v>
       </c>
       <c r="C108" t="s">
         <v>113</v>
       </c>
       <c r="D108">
-        <v>3.85</v>
+        <v>3.792</v>
       </c>
       <c r="E108">
-        <v>3.604</v>
+        <v>3.629</v>
       </c>
       <c r="F108">
-        <v>3.095</v>
+        <v>3.014</v>
       </c>
       <c r="G108">
-        <v>3.468</v>
+        <v>3.465</v>
       </c>
     </row>
     <row r="109" spans="1:7">
@@ -3206,22 +3206,22 @@
         <v>108</v>
       </c>
       <c r="B109">
-        <v>230581</v>
+        <v>230268</v>
       </c>
       <c r="C109" t="s">
         <v>114</v>
       </c>
       <c r="D109">
-        <v>3.792</v>
+        <v>3.85</v>
       </c>
       <c r="E109">
-        <v>3.629</v>
+        <v>3.586</v>
       </c>
       <c r="F109">
-        <v>3.014</v>
+        <v>3.095</v>
       </c>
       <c r="G109">
-        <v>3.465</v>
+        <v>3.46</v>
       </c>
     </row>
     <row r="110" spans="1:7">
@@ -3238,13 +3238,13 @@
         <v>3.871</v>
       </c>
       <c r="E110">
-        <v>3.445</v>
+        <v>3.421</v>
       </c>
       <c r="F110">
         <v>3.221</v>
       </c>
       <c r="G110">
-        <v>3.459</v>
+        <v>3.45</v>
       </c>
     </row>
     <row r="111" spans="1:7">
@@ -3284,13 +3284,13 @@
         <v>3.935</v>
       </c>
       <c r="E112">
-        <v>3.095</v>
+        <v>3.069</v>
       </c>
       <c r="F112">
         <v>3.334</v>
       </c>
       <c r="G112">
-        <v>3.378</v>
+        <v>3.373</v>
       </c>
     </row>
     <row r="113" spans="1:7">
@@ -3307,13 +3307,13 @@
         <v>3.85</v>
       </c>
       <c r="E113">
-        <v>3.479</v>
+        <v>3.456</v>
       </c>
       <c r="F113">
         <v>2.785</v>
       </c>
       <c r="G113">
-        <v>3.32</v>
+        <v>3.308</v>
       </c>
     </row>
     <row r="114" spans="1:7">
@@ -3330,13 +3330,13 @@
         <v>3.807</v>
       </c>
       <c r="E114">
-        <v>3.292</v>
+        <v>3.266</v>
       </c>
       <c r="F114">
         <v>2.835</v>
       </c>
       <c r="G114">
-        <v>3.26</v>
+        <v>3.249</v>
       </c>
     </row>
     <row r="115" spans="1:7">
@@ -3353,13 +3353,13 @@
         <v>4</v>
       </c>
       <c r="E115">
-        <v>3.641</v>
+        <v>3.626</v>
       </c>
       <c r="F115">
         <v>2.343</v>
       </c>
       <c r="G115">
-        <v>3.234</v>
+        <v>3.221</v>
       </c>
     </row>
     <row r="116" spans="1:7">
@@ -3376,13 +3376,13 @@
         <v>4</v>
       </c>
       <c r="E116">
-        <v>3.516</v>
+        <v>3.508</v>
       </c>
       <c r="F116">
         <v>2.404</v>
       </c>
       <c r="G116">
-        <v>3.208</v>
+        <v>3.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CALC + CDP re-correction commit1
</commit_message>
<xml_diff>
--- a/output/CGPA_Results.xlsx
+++ b/output/CGPA_Results.xlsx
@@ -157,6 +157,9 @@
     <t>WIJESEKARA W.A.G.S.</t>
   </si>
   <si>
+    <t>ANTHONY C.S.B.</t>
+  </si>
+  <si>
     <t>AMARATHUNGE A.M.N.L.</t>
   </si>
   <si>
@@ -190,9 +193,6 @@
     <t>GUNASEKARA K.S.</t>
   </si>
   <si>
-    <t>ANTHONY C.S.B.</t>
-  </si>
-  <si>
     <t>RATHEESHAN A.R.</t>
   </si>
   <si>
@@ -286,19 +286,19 @@
     <t>MEEDENIYA M.M.H.</t>
   </si>
   <si>
+    <t>PRABHARSHA H.W.D.</t>
+  </si>
+  <si>
     <t>NIRMANI W.T.</t>
   </si>
   <si>
+    <t>INDUWARA M.L.A.S.</t>
+  </si>
+  <si>
     <t>LENMINI B.L.W.</t>
   </si>
   <si>
-    <t>PRABHARSHA H.W.D.</t>
-  </si>
-  <si>
     <t>RANAWAKA R.A.G.K.</t>
-  </si>
-  <si>
-    <t>INDUWARA M.L.A.S.</t>
   </si>
   <si>
     <t>ABEYWARNA D.H.</t>
@@ -1665,7 +1665,7 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>230038</v>
+        <v>230045</v>
       </c>
       <c r="C42" t="s">
         <v>47</v>
@@ -1677,10 +1677,10 @@
         <v>4</v>
       </c>
       <c r="F42">
-        <v>3.691</v>
+        <v>3.704</v>
       </c>
       <c r="G42">
-        <v>3.881</v>
+        <v>3.886</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1688,7 +1688,7 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>230130</v>
+        <v>230038</v>
       </c>
       <c r="C43" t="s">
         <v>48</v>
@@ -1697,10 +1697,10 @@
         <v>4</v>
       </c>
       <c r="E43">
-        <v>3.96</v>
+        <v>4</v>
       </c>
       <c r="F43">
-        <v>3.714</v>
+        <v>3.691</v>
       </c>
       <c r="G43">
         <v>3.881</v>
@@ -1711,22 +1711,22 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>230212</v>
+        <v>230130</v>
       </c>
       <c r="C44" t="s">
         <v>49</v>
       </c>
       <c r="D44">
-        <v>3.957</v>
+        <v>4</v>
       </c>
       <c r="E44">
-        <v>3.882</v>
+        <v>3.96</v>
       </c>
       <c r="F44">
-        <v>3.821</v>
+        <v>3.714</v>
       </c>
       <c r="G44">
-        <v>3.876</v>
+        <v>3.881</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1734,19 +1734,19 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>230321</v>
+        <v>230212</v>
       </c>
       <c r="C45" t="s">
         <v>50</v>
       </c>
       <c r="D45">
-        <v>4</v>
+        <v>3.957</v>
       </c>
       <c r="E45">
-        <v>3.947</v>
+        <v>3.882</v>
       </c>
       <c r="F45">
-        <v>3.73</v>
+        <v>3.821</v>
       </c>
       <c r="G45">
         <v>3.876</v>
@@ -1757,22 +1757,22 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>230300</v>
+        <v>230321</v>
       </c>
       <c r="C46" t="s">
         <v>51</v>
       </c>
       <c r="D46">
-        <v>3.935</v>
+        <v>4</v>
       </c>
       <c r="E46">
-        <v>4</v>
+        <v>3.947</v>
       </c>
       <c r="F46">
-        <v>3.713</v>
+        <v>3.73</v>
       </c>
       <c r="G46">
-        <v>3.875</v>
+        <v>3.876</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -1780,7 +1780,7 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>230145</v>
+        <v>230300</v>
       </c>
       <c r="C47" t="s">
         <v>52</v>
@@ -1792,10 +1792,10 @@
         <v>4</v>
       </c>
       <c r="F47">
-        <v>3.704</v>
+        <v>3.713</v>
       </c>
       <c r="G47">
-        <v>3.871</v>
+        <v>3.875</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -1803,7 +1803,7 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>230477</v>
+        <v>230145</v>
       </c>
       <c r="C48" t="s">
         <v>53</v>
@@ -1812,13 +1812,13 @@
         <v>3.935</v>
       </c>
       <c r="E48">
-        <v>3.817</v>
+        <v>4</v>
       </c>
       <c r="F48">
-        <v>3.873</v>
+        <v>3.704</v>
       </c>
       <c r="G48">
-        <v>3.866</v>
+        <v>3.871</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -1826,22 +1826,22 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>230613</v>
+        <v>230477</v>
       </c>
       <c r="C49" t="s">
         <v>54</v>
       </c>
       <c r="D49">
-        <v>4</v>
+        <v>3.935</v>
       </c>
       <c r="E49">
-        <v>3.947</v>
+        <v>3.817</v>
       </c>
       <c r="F49">
-        <v>3.699</v>
+        <v>3.873</v>
       </c>
       <c r="G49">
-        <v>3.865</v>
+        <v>3.866</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -1849,7 +1849,7 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>230058</v>
+        <v>230613</v>
       </c>
       <c r="C50" t="s">
         <v>55</v>
@@ -1858,13 +1858,13 @@
         <v>4</v>
       </c>
       <c r="E50">
-        <v>3.908</v>
+        <v>3.947</v>
       </c>
       <c r="F50">
-        <v>3.713</v>
+        <v>3.699</v>
       </c>
       <c r="G50">
-        <v>3.855</v>
+        <v>3.865</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -1872,19 +1872,19 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>230697</v>
+        <v>230058</v>
       </c>
       <c r="C51" t="s">
         <v>56</v>
       </c>
       <c r="D51">
-        <v>3.957</v>
+        <v>4</v>
       </c>
       <c r="E51">
-        <v>3.96</v>
+        <v>3.908</v>
       </c>
       <c r="F51">
-        <v>3.671</v>
+        <v>3.713</v>
       </c>
       <c r="G51">
         <v>3.855</v>
@@ -1895,22 +1895,22 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>230211</v>
+        <v>230697</v>
       </c>
       <c r="C52" t="s">
         <v>57</v>
       </c>
       <c r="D52">
-        <v>4</v>
+        <v>3.957</v>
       </c>
       <c r="E52">
-        <v>3.895</v>
+        <v>3.96</v>
       </c>
       <c r="F52">
-        <v>3.721</v>
+        <v>3.671</v>
       </c>
       <c r="G52">
-        <v>3.853</v>
+        <v>3.855</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -1918,7 +1918,7 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>230045</v>
+        <v>230211</v>
       </c>
       <c r="C53" t="s">
         <v>58</v>
@@ -1927,13 +1927,13 @@
         <v>4</v>
       </c>
       <c r="E53">
-        <v>3.908</v>
+        <v>3.895</v>
       </c>
       <c r="F53">
-        <v>3.704</v>
+        <v>3.721</v>
       </c>
       <c r="G53">
-        <v>3.851</v>
+        <v>3.853</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -2654,22 +2654,22 @@
         <v>84</v>
       </c>
       <c r="B85">
-        <v>230444</v>
+        <v>230495</v>
       </c>
       <c r="C85" t="s">
         <v>90</v>
       </c>
       <c r="D85">
-        <v>3.785</v>
+        <v>3.85</v>
       </c>
       <c r="E85">
-        <v>3.596</v>
+        <v>3.869</v>
       </c>
       <c r="F85">
-        <v>3.757</v>
+        <v>3.443</v>
       </c>
       <c r="G85">
-        <v>3.693</v>
+        <v>3.701</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -2677,22 +2677,22 @@
         <v>85</v>
       </c>
       <c r="B86">
-        <v>230375</v>
+        <v>230444</v>
       </c>
       <c r="C86" t="s">
         <v>91</v>
       </c>
       <c r="D86">
-        <v>3.85</v>
+        <v>3.785</v>
       </c>
       <c r="E86">
-        <v>3.686</v>
+        <v>3.596</v>
       </c>
       <c r="F86">
-        <v>3.599</v>
+        <v>3.757</v>
       </c>
       <c r="G86">
-        <v>3.691</v>
+        <v>3.693</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -2700,19 +2700,19 @@
         <v>86</v>
       </c>
       <c r="B87">
-        <v>230495</v>
+        <v>230261</v>
       </c>
       <c r="C87" t="s">
         <v>92</v>
       </c>
       <c r="D87">
-        <v>3.85</v>
+        <v>4</v>
       </c>
       <c r="E87">
-        <v>3.869</v>
+        <v>3.747</v>
       </c>
       <c r="F87">
-        <v>3.417</v>
+        <v>3.458</v>
       </c>
       <c r="G87">
         <v>3.691</v>
@@ -2723,22 +2723,22 @@
         <v>87</v>
       </c>
       <c r="B88">
-        <v>230527</v>
+        <v>230375</v>
       </c>
       <c r="C88" t="s">
         <v>93</v>
       </c>
       <c r="D88">
-        <v>4</v>
+        <v>3.85</v>
       </c>
       <c r="E88">
-        <v>3.83</v>
+        <v>3.686</v>
       </c>
       <c r="F88">
-        <v>3.339</v>
+        <v>3.599</v>
       </c>
       <c r="G88">
-        <v>3.681</v>
+        <v>3.691</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -2746,7 +2746,7 @@
         <v>88</v>
       </c>
       <c r="B89">
-        <v>230261</v>
+        <v>230527</v>
       </c>
       <c r="C89" t="s">
         <v>94</v>
@@ -2755,13 +2755,13 @@
         <v>4</v>
       </c>
       <c r="E89">
-        <v>3.747</v>
+        <v>3.83</v>
       </c>
       <c r="F89">
-        <v>3.424</v>
+        <v>3.339</v>
       </c>
       <c r="G89">
-        <v>3.678</v>
+        <v>3.681</v>
       </c>
     </row>
     <row r="90" spans="1:7">

</xml_diff>

<commit_message>
corrections.json error and indexcheck test commit
</commit_message>
<xml_diff>
--- a/output/CGPA_Results.xlsx
+++ b/output/CGPA_Results.xlsx
@@ -169,6 +169,9 @@
     <t>DESHAN W.U.</t>
   </si>
   <si>
+    <t>GUNASEKARA K.S.</t>
+  </si>
+  <si>
     <t>GUNASEKARA L.U.A.</t>
   </si>
   <si>
@@ -193,12 +196,12 @@
     <t>WEERASINGHE J.A.H.R.</t>
   </si>
   <si>
-    <t>GUNASEKARA K.S.</t>
-  </si>
-  <si>
     <t>RATHEESHAN A.R.</t>
   </si>
   <si>
+    <t>TENNAKOON U.G.R.B.</t>
+  </si>
+  <si>
     <t>GUNATHUNGA U.A.</t>
   </si>
   <si>
@@ -212,9 +215,6 @@
   </si>
   <si>
     <t>FERNANDO H.M.D.</t>
-  </si>
-  <si>
-    <t>TENNAKOON U.G.R.B.</t>
   </si>
   <si>
     <t>PRIYADARSHANA S.A.D.</t>
@@ -1757,19 +1757,19 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>230212</v>
+        <v>230211</v>
       </c>
       <c r="C46" t="s">
         <v>51</v>
       </c>
       <c r="D46">
-        <v>3.957</v>
+        <v>4</v>
       </c>
       <c r="E46">
-        <v>3.882</v>
+        <v>3.895</v>
       </c>
       <c r="F46">
-        <v>3.821</v>
+        <v>3.782</v>
       </c>
       <c r="G46">
         <v>3.876</v>
@@ -1780,19 +1780,19 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>230321</v>
+        <v>230212</v>
       </c>
       <c r="C47" t="s">
         <v>52</v>
       </c>
       <c r="D47">
-        <v>4</v>
+        <v>3.957</v>
       </c>
       <c r="E47">
-        <v>3.947</v>
+        <v>3.882</v>
       </c>
       <c r="F47">
-        <v>3.73</v>
+        <v>3.821</v>
       </c>
       <c r="G47">
         <v>3.876</v>
@@ -1803,22 +1803,22 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>230300</v>
+        <v>230321</v>
       </c>
       <c r="C48" t="s">
         <v>53</v>
       </c>
       <c r="D48">
-        <v>3.935</v>
+        <v>4</v>
       </c>
       <c r="E48">
-        <v>4</v>
+        <v>3.947</v>
       </c>
       <c r="F48">
-        <v>3.713</v>
+        <v>3.73</v>
       </c>
       <c r="G48">
-        <v>3.875</v>
+        <v>3.876</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -1826,7 +1826,7 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>230145</v>
+        <v>230300</v>
       </c>
       <c r="C49" t="s">
         <v>54</v>
@@ -1838,10 +1838,10 @@
         <v>4</v>
       </c>
       <c r="F49">
-        <v>3.704</v>
+        <v>3.713</v>
       </c>
       <c r="G49">
-        <v>3.871</v>
+        <v>3.875</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -1849,7 +1849,7 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>230477</v>
+        <v>230145</v>
       </c>
       <c r="C50" t="s">
         <v>55</v>
@@ -1858,13 +1858,13 @@
         <v>3.935</v>
       </c>
       <c r="E50">
-        <v>3.817</v>
+        <v>4</v>
       </c>
       <c r="F50">
-        <v>3.873</v>
+        <v>3.704</v>
       </c>
       <c r="G50">
-        <v>3.866</v>
+        <v>3.871</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -1872,22 +1872,22 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>230613</v>
+        <v>230477</v>
       </c>
       <c r="C51" t="s">
         <v>56</v>
       </c>
       <c r="D51">
-        <v>4</v>
+        <v>3.935</v>
       </c>
       <c r="E51">
-        <v>3.947</v>
+        <v>3.817</v>
       </c>
       <c r="F51">
-        <v>3.699</v>
+        <v>3.873</v>
       </c>
       <c r="G51">
-        <v>3.865</v>
+        <v>3.866</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -1895,7 +1895,7 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>230058</v>
+        <v>230613</v>
       </c>
       <c r="C52" t="s">
         <v>57</v>
@@ -1904,13 +1904,13 @@
         <v>4</v>
       </c>
       <c r="E52">
-        <v>3.908</v>
+        <v>3.947</v>
       </c>
       <c r="F52">
-        <v>3.713</v>
+        <v>3.699</v>
       </c>
       <c r="G52">
-        <v>3.855</v>
+        <v>3.865</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -1918,19 +1918,19 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>230697</v>
+        <v>230058</v>
       </c>
       <c r="C53" t="s">
         <v>58</v>
       </c>
       <c r="D53">
-        <v>3.957</v>
+        <v>4</v>
       </c>
       <c r="E53">
-        <v>3.96</v>
+        <v>3.908</v>
       </c>
       <c r="F53">
-        <v>3.671</v>
+        <v>3.713</v>
       </c>
       <c r="G53">
         <v>3.855</v>
@@ -1941,22 +1941,22 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>230211</v>
+        <v>230697</v>
       </c>
       <c r="C54" t="s">
         <v>59</v>
       </c>
       <c r="D54">
-        <v>4</v>
+        <v>3.957</v>
       </c>
       <c r="E54">
-        <v>3.895</v>
+        <v>3.96</v>
       </c>
       <c r="F54">
-        <v>3.721</v>
+        <v>3.671</v>
       </c>
       <c r="G54">
-        <v>3.853</v>
+        <v>3.855</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -1987,22 +1987,22 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>230218</v>
+        <v>230629</v>
       </c>
       <c r="C56" t="s">
         <v>61</v>
       </c>
       <c r="D56">
-        <v>3.935</v>
+        <v>3.957</v>
       </c>
       <c r="E56">
-        <v>3.811</v>
+        <v>3.908</v>
       </c>
       <c r="F56">
-        <v>3.825</v>
+        <v>3.726</v>
       </c>
       <c r="G56">
-        <v>3.844</v>
+        <v>3.85</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -2010,22 +2010,22 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>230659</v>
+        <v>230218</v>
       </c>
       <c r="C57" t="s">
         <v>62</v>
       </c>
       <c r="D57">
-        <v>3.857</v>
+        <v>3.935</v>
       </c>
       <c r="E57">
-        <v>3.869</v>
+        <v>3.811</v>
       </c>
       <c r="F57">
-        <v>3.804</v>
+        <v>3.825</v>
       </c>
       <c r="G57">
-        <v>3.841</v>
+        <v>3.844</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -2033,22 +2033,22 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>230492</v>
+        <v>230659</v>
       </c>
       <c r="C58" t="s">
         <v>63</v>
       </c>
       <c r="D58">
-        <v>3.935</v>
+        <v>3.857</v>
       </c>
       <c r="E58">
-        <v>3.908</v>
+        <v>3.869</v>
       </c>
       <c r="F58">
-        <v>3.69</v>
+        <v>3.804</v>
       </c>
       <c r="G58">
-        <v>3.836</v>
+        <v>3.841</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -2056,22 +2056,22 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>230500</v>
+        <v>230492</v>
       </c>
       <c r="C59" t="s">
         <v>64</v>
       </c>
       <c r="D59">
-        <v>3.957</v>
+        <v>3.935</v>
       </c>
       <c r="E59">
         <v>3.908</v>
       </c>
       <c r="F59">
-        <v>3.678</v>
+        <v>3.69</v>
       </c>
       <c r="G59">
-        <v>3.831</v>
+        <v>3.836</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -2079,22 +2079,22 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>230180</v>
+        <v>230500</v>
       </c>
       <c r="C60" t="s">
         <v>65</v>
       </c>
       <c r="D60">
-        <v>3.935</v>
+        <v>3.957</v>
       </c>
       <c r="E60">
-        <v>3.817</v>
+        <v>3.908</v>
       </c>
       <c r="F60">
-        <v>3.778</v>
+        <v>3.678</v>
       </c>
       <c r="G60">
-        <v>3.83</v>
+        <v>3.831</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -2102,19 +2102,19 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>230629</v>
+        <v>230180</v>
       </c>
       <c r="C61" t="s">
         <v>66</v>
       </c>
       <c r="D61">
-        <v>3.957</v>
+        <v>3.935</v>
       </c>
       <c r="E61">
-        <v>3.908</v>
+        <v>3.817</v>
       </c>
       <c r="F61">
-        <v>3.673</v>
+        <v>3.778</v>
       </c>
       <c r="G61">
         <v>3.83</v>

</xml_diff>